<commit_message>
adding empty physical copy
</commit_message>
<xml_diff>
--- a/04_output_data/folder.xlsx
+++ b/04_output_data/folder.xlsx
@@ -3883,1930 +3883,1930 @@
     <t>DH.TMIK.M 274/14</t>
   </si>
   <si>
-    <t>pou_2492e70846089b93</t>
-  </si>
-  <si>
-    <t>pou_1522c52673c8032e</t>
-  </si>
-  <si>
-    <t>pou_aff4d580e7ba866e;pou_2c0b60d30985cfa2</t>
-  </si>
-  <si>
-    <t>pou_81f6080407436d2a</t>
-  </si>
-  <si>
-    <t>pou_9258575443480e2b</t>
-  </si>
-  <si>
-    <t>pou_45c26ac31682324c</t>
-  </si>
-  <si>
-    <t>pou_30f077d65ec50d94</t>
-  </si>
-  <si>
-    <t>pou_939a88bd3d3930a8</t>
-  </si>
-  <si>
-    <t>pou_f1d15a3dbed721b1</t>
-  </si>
-  <si>
-    <t>pou_af2bf45b49b78ce8</t>
-  </si>
-  <si>
-    <t>pou_9b40fdc3faa00b1c</t>
-  </si>
-  <si>
-    <t>pou_27bcf8341b50fe91</t>
-  </si>
-  <si>
-    <t>pou_a577744e5ef5f12d</t>
-  </si>
-  <si>
-    <t>pou_007dffee45355dee</t>
-  </si>
-  <si>
-    <t>pou_b777a0f6988bf38f;pou_c63e1e9716b6caa1</t>
-  </si>
-  <si>
-    <t>pou_f9dd7bb686a550de</t>
-  </si>
-  <si>
-    <t>pou_1939d6faf2f1957f</t>
-  </si>
-  <si>
-    <t>pou_40515860fc0522d0;pou_5025df5a08503534</t>
-  </si>
-  <si>
-    <t>pou_fc29cd179079e864</t>
-  </si>
-  <si>
-    <t>pou_096db3ff7e3207f7</t>
-  </si>
-  <si>
-    <t>pou_b4ab0729f6291121</t>
-  </si>
-  <si>
-    <t>pou_c232a5371ff74030</t>
-  </si>
-  <si>
-    <t>pou_ebf93123a5e7c3ac;pou_a7590d86fe174da0</t>
-  </si>
-  <si>
-    <t>pou_4618bfc04443dec8;pou_04982e9f8743c62d</t>
-  </si>
-  <si>
-    <t>pou_32a328901a30d2dc</t>
-  </si>
-  <si>
-    <t>pou_60358b01a5d6b457</t>
-  </si>
-  <si>
-    <t>pou_290362065f7b17d4</t>
-  </si>
-  <si>
-    <t>pou_b45237217830da48;pou_93c7d4f546891942;pou_9e01b1c737881f5f;pou_eea1ef70c226b4a6;pou_df601c32794c8edb;pou_090241c958f46e6b;pou_11d9df817c638837;pou_b5aa2b4b00dc034b;pou_47ae95a3de153efd</t>
-  </si>
-  <si>
-    <t>pou_680faf8c0efaf114</t>
-  </si>
-  <si>
-    <t>pou_821fe50976a60be9</t>
-  </si>
-  <si>
-    <t>pou_6422153083736dbb</t>
-  </si>
-  <si>
-    <t>pou_4f10ebb7cc2da608</t>
-  </si>
-  <si>
-    <t>pou_197cf0ed7666af2e</t>
-  </si>
-  <si>
-    <t>pou_604df49bfb9b5db6</t>
-  </si>
-  <si>
-    <t>pou_3ca4e110ebee7cd3;pou_69e3d51ac8d77429</t>
-  </si>
-  <si>
-    <t>pou_9d945027ca8b74f0</t>
-  </si>
-  <si>
-    <t>pou_f41a117c79793481</t>
-  </si>
-  <si>
-    <t>pou_d56c52dade9514e7</t>
-  </si>
-  <si>
-    <t>pou_054a3c7286893809;pou_683a06dbfe17d318</t>
-  </si>
-  <si>
-    <t>pou_0f7af17b206a9097</t>
-  </si>
-  <si>
-    <t>pou_b478e8a86cf599c3</t>
-  </si>
-  <si>
-    <t>pou_107686ff10c7a399</t>
-  </si>
-  <si>
-    <t>pou_2ec7a31ee10b42c7</t>
-  </si>
-  <si>
-    <t>pou_72c5017fc4ae4ef5</t>
-  </si>
-  <si>
-    <t>pou_80d089690b149583</t>
-  </si>
-  <si>
-    <t>pou_60ef8ee14efbd790;pou_bec800f7862b8c48</t>
-  </si>
-  <si>
-    <t>pou_39ced034cc9b7c21</t>
-  </si>
-  <si>
-    <t>pou_6cfd143f0f2c99eb</t>
-  </si>
-  <si>
-    <t>pou_9f5e8eead572fbd4</t>
-  </si>
-  <si>
-    <t>pou_210f43fba32fd270</t>
-  </si>
-  <si>
-    <t>pou_8c6c1d47a68c3467</t>
-  </si>
-  <si>
-    <t>pou_668a117f2c52d459</t>
-  </si>
-  <si>
-    <t>pou_fa68813d1c1225ca</t>
-  </si>
-  <si>
-    <t>pou_fb01b700745ad120</t>
-  </si>
-  <si>
-    <t>pou_566773c20fa9aa76</t>
-  </si>
-  <si>
-    <t>pou_d9bd678fdd3c0cbf</t>
-  </si>
-  <si>
-    <t>pou_044a917428e841ce</t>
-  </si>
-  <si>
-    <t>pou_769bc25991362bc7</t>
-  </si>
-  <si>
-    <t>pou_63331d118eeeee1a</t>
-  </si>
-  <si>
-    <t>pou_a1cfaec58c5873d1</t>
-  </si>
-  <si>
-    <t>pou_61f137eea909af05</t>
-  </si>
-  <si>
-    <t>pou_78c8c93ae2c1e710</t>
-  </si>
-  <si>
-    <t>pou_aa51e6c49c40c24f</t>
-  </si>
-  <si>
-    <t>pou_0a0df5d3b393713a</t>
-  </si>
-  <si>
-    <t>pou_9ec5cae6a9847884</t>
-  </si>
-  <si>
-    <t>pou_6b36096934fc10d2</t>
-  </si>
-  <si>
-    <t>pou_2b86aacf59a938f8</t>
-  </si>
-  <si>
-    <t>pou_65570c36cb4ba01c</t>
-  </si>
-  <si>
-    <t>pou_1125e461cec5d4a0</t>
-  </si>
-  <si>
-    <t>pou_a39656910f4891d2</t>
-  </si>
-  <si>
-    <t>pou_9b91dd5d3fae5e19</t>
-  </si>
-  <si>
-    <t>pou_87df9338bd9a2432</t>
-  </si>
-  <si>
-    <t>pou_3fc5ea7f07370307</t>
-  </si>
-  <si>
-    <t>pou_248fc0357d62b173</t>
-  </si>
-  <si>
-    <t>pou_05c926697eeb335c</t>
-  </si>
-  <si>
-    <t>pou_2681dbb7464429f1</t>
-  </si>
-  <si>
-    <t>pou_224bb50b8a4fd72c</t>
-  </si>
-  <si>
-    <t>pou_7e6e35cf5f39f3d4</t>
-  </si>
-  <si>
-    <t>pou_28f7ec0e9f5ad60f</t>
-  </si>
-  <si>
-    <t>pou_65cc3fbe965b9353</t>
-  </si>
-  <si>
-    <t>pou_d59eb828dbf614cd</t>
-  </si>
-  <si>
-    <t>pou_fac125cac1e329f1</t>
-  </si>
-  <si>
-    <t>pou_f9493db8772183e9</t>
-  </si>
-  <si>
-    <t>pou_257fc545ee7b43ce</t>
-  </si>
-  <si>
-    <t>pou_c9add1f3b69d1d02</t>
-  </si>
-  <si>
-    <t>pou_334cf7cea84ec41a</t>
-  </si>
-  <si>
-    <t>pou_47fd6fce7197f90f</t>
-  </si>
-  <si>
-    <t>pou_c0c2795b77c2238f</t>
-  </si>
-  <si>
-    <t>pou_7f1026ffdcd3b879</t>
-  </si>
-  <si>
-    <t>pou_ba24d86818a18fb8</t>
-  </si>
-  <si>
-    <t>pou_827539a35122bb34</t>
-  </si>
-  <si>
-    <t>pou_c0279aeaac03cfbf</t>
-  </si>
-  <si>
-    <t>pou_1439d3dcf45e9619</t>
-  </si>
-  <si>
-    <t>pou_80b21577bcfce40f</t>
-  </si>
-  <si>
-    <t>pou_f25016fd9678748c</t>
-  </si>
-  <si>
-    <t>pou_12d2c9d57b8f1457</t>
-  </si>
-  <si>
-    <t>pou_4f8d6838b8585dc6</t>
-  </si>
-  <si>
-    <t>pou_b9bd796abf674971</t>
-  </si>
-  <si>
-    <t>pou_ea12e37f4353f2f2</t>
-  </si>
-  <si>
-    <t>pou_347a162e4b11d3ae</t>
-  </si>
-  <si>
-    <t>pou_86fa90046d2c67d5</t>
-  </si>
-  <si>
-    <t>pou_8841ef2287aac6af</t>
-  </si>
-  <si>
-    <t>pou_6e27522132f04b9e</t>
-  </si>
-  <si>
-    <t>pou_297205349a80256d</t>
-  </si>
-  <si>
-    <t>pou_2f1b1de26c97aff3</t>
-  </si>
-  <si>
-    <t>pou_50816ef3a38773b6</t>
-  </si>
-  <si>
-    <t>pou_14baf721d4c59758</t>
-  </si>
-  <si>
-    <t>pou_63adb1aaed5a116c</t>
-  </si>
-  <si>
-    <t>pou_a21ed67cddfb16fe</t>
-  </si>
-  <si>
-    <t>pou_4b85c7dcd039fb1d</t>
-  </si>
-  <si>
-    <t>pou_8d646cf75ba691d0</t>
-  </si>
-  <si>
-    <t>pou_d2edf8c3bba0386d</t>
-  </si>
-  <si>
-    <t>pou_c799f4b69bca6e4d</t>
-  </si>
-  <si>
-    <t>pou_6a84636ecbd62184</t>
-  </si>
-  <si>
-    <t>pou_e075ad33d275b9ac</t>
-  </si>
-  <si>
-    <t>pou_18296971838d990d</t>
-  </si>
-  <si>
-    <t>pou_e810bc47ec56a76d</t>
-  </si>
-  <si>
-    <t>pou_7bc42a988a5ba466</t>
-  </si>
-  <si>
-    <t>pou_d41a1fb76d56af65</t>
-  </si>
-  <si>
-    <t>pou_7c80808b33bfe35d</t>
-  </si>
-  <si>
-    <t>pou_e7f374484e934156</t>
-  </si>
-  <si>
-    <t>pou_9fb8ae0832130af7</t>
-  </si>
-  <si>
-    <t>pou_f57ae29422b4abbc</t>
-  </si>
-  <si>
-    <t>pou_4e907f84fb19f260</t>
-  </si>
-  <si>
-    <t>pou_74c833093fa5226b</t>
-  </si>
-  <si>
-    <t>pou_5fa5c77c3d4f2972;pou_e486b92d6ecc8297;pou_c1c096c658d70a6a</t>
-  </si>
-  <si>
-    <t>pou_2aedcbe7dfff283d</t>
-  </si>
-  <si>
-    <t>pou_b433216ce24f51fa</t>
-  </si>
-  <si>
-    <t>pou_6e948ce7b9a141fc</t>
-  </si>
-  <si>
-    <t>pou_7d73f261ca8dc4d4;pou_d483ada348cd5ed2</t>
-  </si>
-  <si>
-    <t>pou_3040e11d00c6f197</t>
-  </si>
-  <si>
-    <t>pou_0b1e4a3d8363056c</t>
-  </si>
-  <si>
-    <t>pou_60c37e69e3f3d28f</t>
-  </si>
-  <si>
-    <t>pou_37587cf37cfaa525</t>
-  </si>
-  <si>
-    <t>pou_8af819e1fa6812a3</t>
-  </si>
-  <si>
-    <t>pou_9ee974b5b0d997af</t>
-  </si>
-  <si>
-    <t>pou_f87a2167e4db5959</t>
-  </si>
-  <si>
-    <t>pou_fdf919bb355c720d</t>
-  </si>
-  <si>
-    <t>pou_521a480b111e5775</t>
-  </si>
-  <si>
-    <t>pou_87e23bf618b97e70</t>
-  </si>
-  <si>
-    <t>pou_c74d40ae00929f26</t>
-  </si>
-  <si>
-    <t>pou_56221c19160fa327</t>
-  </si>
-  <si>
-    <t>pou_b51894219143a2cd</t>
-  </si>
-  <si>
-    <t>pou_7dec514804fd3372</t>
-  </si>
-  <si>
-    <t>pou_9150661d905e4f7a</t>
-  </si>
-  <si>
-    <t>pou_0ace40e3ef7e7b11</t>
-  </si>
-  <si>
-    <t>pou_d280878cdf30e963</t>
-  </si>
-  <si>
-    <t>pou_e3332145eaf9d1eb</t>
-  </si>
-  <si>
-    <t>pou_14a01d295cb1dbc5</t>
-  </si>
-  <si>
-    <t>pou_8483733a4518b021</t>
-  </si>
-  <si>
-    <t>pou_3838d803c6da3d67;pou_046bd58eb4219c16;pou_3e6d827824a0eea5;pou_f5eec2eaffdb1c17;pou_82cf2ec8af9e14b5;pou_f68dd78906e8e0b6;pou_dfe4d59f482140f8;pou_e9d1a7cf3724adbd;pou_971e03e4bacfad9f;pou_db9832d8a1841517;pou_d64540262cf9b133</t>
-  </si>
-  <si>
-    <t>pou_295c1cbd1ad3d716</t>
-  </si>
-  <si>
-    <t>pou_8f884639ff2b4ed5</t>
-  </si>
-  <si>
-    <t>pou_c4b5b84bbdc1f2d2;pou_1a97eff6856f7932</t>
-  </si>
-  <si>
-    <t>pou_f2d0bca1b6e04a6a</t>
-  </si>
-  <si>
-    <t>pou_8c1ca98a4e3adde1</t>
-  </si>
-  <si>
-    <t>pou_58ff0ba15dd7ffeb</t>
-  </si>
-  <si>
-    <t>pou_4c151faed65f88a8</t>
-  </si>
-  <si>
-    <t>pou_9f01d0c4dbc15fdb</t>
-  </si>
-  <si>
-    <t>pou_0a619390cb3f6a1e</t>
-  </si>
-  <si>
-    <t>pou_c69a116da5aaf41b</t>
-  </si>
-  <si>
-    <t>pou_d20d711465a61332</t>
-  </si>
-  <si>
-    <t>pou_7049e990b07db0ac</t>
-  </si>
-  <si>
-    <t>pou_ca99137f6eb65947</t>
-  </si>
-  <si>
-    <t>pou_15531096b5b164cf</t>
-  </si>
-  <si>
-    <t>pou_4ca92e2b2c3b23dc</t>
-  </si>
-  <si>
-    <t>pou_48cf02cc012ab636</t>
-  </si>
-  <si>
-    <t>pou_cf2f98c834e5cdc5</t>
-  </si>
-  <si>
-    <t>pou_812a62e7cea4c89c</t>
-  </si>
-  <si>
-    <t>pou_bdc80723b9e4f950</t>
-  </si>
-  <si>
-    <t>pou_550d649dd4f3d006</t>
-  </si>
-  <si>
-    <t>pou_faf8cea2e13d8101</t>
-  </si>
-  <si>
-    <t>pou_a012b9d0b8c166e0</t>
-  </si>
-  <si>
-    <t>pou_48fe5b33f0d751cb</t>
-  </si>
-  <si>
-    <t>pou_12e886d1e695724e</t>
-  </si>
-  <si>
-    <t>pou_c2776d4db039b16b</t>
-  </si>
-  <si>
-    <t>pou_cddaab98dcbedba1</t>
-  </si>
-  <si>
-    <t>pou_bd7e362410e2cf07</t>
-  </si>
-  <si>
-    <t>pou_a0fe82ff06eb1e56</t>
-  </si>
-  <si>
-    <t>pou_ead0ca7a3a6b0133</t>
-  </si>
-  <si>
-    <t>pou_c0fe33b9d404624e</t>
-  </si>
-  <si>
-    <t>pou_bcaf31c8ac3ba188</t>
-  </si>
-  <si>
-    <t>pou_e1f3d5f1f91fcba5</t>
-  </si>
-  <si>
-    <t>pou_96c9573e13c3fd8a</t>
-  </si>
-  <si>
-    <t>pou_bb65f20f9666a13c</t>
-  </si>
-  <si>
-    <t>pou_90ed06c96ddeda9b</t>
-  </si>
-  <si>
-    <t>pou_1e90edb659fd8b51</t>
-  </si>
-  <si>
-    <t>pou_6e63cac2c5290513</t>
-  </si>
-  <si>
-    <t>pou_7494b081d504de79</t>
-  </si>
-  <si>
-    <t>pou_b3a53627928b22f5</t>
-  </si>
-  <si>
-    <t>pou_d25ff97caa270829</t>
-  </si>
-  <si>
-    <t>pou_2805215c8a1407a4</t>
-  </si>
-  <si>
-    <t>pou_587f380bbefbc8b5</t>
-  </si>
-  <si>
-    <t>pou_f9928b5325e63cf2</t>
-  </si>
-  <si>
-    <t>pou_8d4cb49efb02445b</t>
-  </si>
-  <si>
-    <t>pou_9917526d95b8b2ee</t>
-  </si>
-  <si>
-    <t>pou_72f7228c0eb63a82</t>
-  </si>
-  <si>
-    <t>pou_7e5b20cf766162f7</t>
-  </si>
-  <si>
-    <t>pou_4936f8c08dfd0d0f</t>
-  </si>
-  <si>
-    <t>pou_b52e7a7eb8c9f4b7</t>
-  </si>
-  <si>
-    <t>pou_c195f47fe8336b19</t>
-  </si>
-  <si>
-    <t>pou_8c4043a024dbe119</t>
-  </si>
-  <si>
-    <t>pou_14ac534e8515cf53</t>
-  </si>
-  <si>
-    <t>pou_7b6d0191c465d8ee</t>
-  </si>
-  <si>
-    <t>pou_b2c4cf2726015747</t>
-  </si>
-  <si>
-    <t>pou_561cdb7eadc832ee</t>
-  </si>
-  <si>
-    <t>pou_4fb4b9a0078d3be7</t>
-  </si>
-  <si>
-    <t>pou_493395157bee3208</t>
-  </si>
-  <si>
-    <t>pou_ae718d78ab91cd92</t>
-  </si>
-  <si>
-    <t>pou_ec2543a13da4f271</t>
-  </si>
-  <si>
-    <t>pou_0b8676d49de69c6d</t>
-  </si>
-  <si>
-    <t>pou_78c1ce1cb1acbeeb</t>
-  </si>
-  <si>
-    <t>pou_54290a11cd3ac0c6</t>
-  </si>
-  <si>
-    <t>pou_be9c5042ea80cdf8</t>
-  </si>
-  <si>
-    <t>pou_708f59ee0afb9b66</t>
-  </si>
-  <si>
-    <t>pou_1db4190cbc10ba2d</t>
-  </si>
-  <si>
-    <t>pou_9e35ab5026c55f6d</t>
-  </si>
-  <si>
-    <t>pou_fe58c2de38ea577c</t>
-  </si>
-  <si>
-    <t>pou_2616b2b23525ffa7</t>
-  </si>
-  <si>
-    <t>pou_91aeb908a4b8fac6</t>
-  </si>
-  <si>
-    <t>pou_60a970c754e2253d</t>
-  </si>
-  <si>
-    <t>pou_a47f5264398673df</t>
-  </si>
-  <si>
-    <t>pou_60f3fc300d069329</t>
-  </si>
-  <si>
-    <t>pou_b08f902164f94b6d</t>
-  </si>
-  <si>
-    <t>pou_b6666ed255c031c8</t>
-  </si>
-  <si>
-    <t>pou_a240c7b2a3bf3880</t>
-  </si>
-  <si>
-    <t>pou_e6569b087215ef30</t>
-  </si>
-  <si>
-    <t>pou_4475a0e17b1919d6</t>
-  </si>
-  <si>
-    <t>pou_f21b67ff5615e228</t>
-  </si>
-  <si>
-    <t>pou_a0e8536d644950c0</t>
-  </si>
-  <si>
-    <t>pou_4b3c90ab11da8eb3</t>
-  </si>
-  <si>
-    <t>pou_12f47f8d72b68308</t>
-  </si>
-  <si>
-    <t>pou_2fe11b37be876650</t>
-  </si>
-  <si>
-    <t>pou_dbc5b2357a51f98c</t>
-  </si>
-  <si>
-    <t>pou_f3ed0d547e847291</t>
-  </si>
-  <si>
-    <t>pou_6caf3584971a6588</t>
-  </si>
-  <si>
-    <t>pou_59ab8edbdd98b88b</t>
-  </si>
-  <si>
-    <t>pou_349d1466dada6b50</t>
-  </si>
-  <si>
-    <t>pou_712232736a0d9f1b</t>
-  </si>
-  <si>
-    <t>pou_27501605e3e51654</t>
-  </si>
-  <si>
-    <t>pou_a3d21635800dac28</t>
-  </si>
-  <si>
-    <t>pou_a3151da01d37757e</t>
-  </si>
-  <si>
-    <t>pou_ccb327f753fb6949</t>
-  </si>
-  <si>
-    <t>pou_6e4c49b8776fe712</t>
-  </si>
-  <si>
-    <t>pou_983f104ac6e61ff4</t>
-  </si>
-  <si>
-    <t>pou_df5a6d9d84ed831a</t>
-  </si>
-  <si>
-    <t>pou_fa39819eea53059f</t>
-  </si>
-  <si>
-    <t>pou_dd46192d74f363a3</t>
-  </si>
-  <si>
-    <t>pou_4f543f826f82c96f</t>
-  </si>
-  <si>
-    <t>pou_b1224f701f0ba2b7</t>
-  </si>
-  <si>
-    <t>pou_9eec722d2f80efb6</t>
-  </si>
-  <si>
-    <t>pou_b87e76e9ed8e84ea</t>
-  </si>
-  <si>
-    <t>pou_9172cecb539a388f</t>
-  </si>
-  <si>
-    <t>pou_4eb7506de3ece741</t>
-  </si>
-  <si>
-    <t>pou_53a08b6979ed9bf8</t>
-  </si>
-  <si>
-    <t>pou_79d962d0424e6198</t>
-  </si>
-  <si>
-    <t>pou_9502e46cd0ede0c0</t>
-  </si>
-  <si>
-    <t>pou_a8597538dc3aae6e</t>
-  </si>
-  <si>
-    <t>pou_a3d2cef91a4f5349</t>
-  </si>
-  <si>
-    <t>pou_1efb68aa9768e37c</t>
-  </si>
-  <si>
-    <t>pou_bfbd112882ae2e9d</t>
-  </si>
-  <si>
-    <t>pou_066d98ea119a4be5</t>
-  </si>
-  <si>
-    <t>pou_3f0bccb14ef4b8c3;pou_3e843913ad47a1e4</t>
-  </si>
-  <si>
-    <t>pou_4c7ab4f44556a8bd</t>
-  </si>
-  <si>
-    <t>pou_885a43a31d8cfdd8;pou_fbf867faf63b4db5;pou_1c2833904b60ff83;pou_534b7641851ee019;pou_d65e3f317845c3a5;pou_524c07d35afe0068;pou_7b529d8958032ab5;pou_d950af62be3cb9fe;pou_f5688383cece2f25;pou_ec25e336bbfdb6fd;pou_3546228b71082aa9;pou_6855e5bbace3e94c</t>
-  </si>
-  <si>
-    <t>pou_ea8d732f90011612</t>
-  </si>
-  <si>
-    <t>pou_d391c9af7e358a17</t>
-  </si>
-  <si>
-    <t>pou_7f055dbe0630beb7</t>
-  </si>
-  <si>
-    <t>pou_34541c502e86727c</t>
-  </si>
-  <si>
-    <t>pou_27975fc39399a7b1</t>
-  </si>
-  <si>
-    <t>pou_fd416c8e282e0a20</t>
-  </si>
-  <si>
-    <t>pou_7ee964f11934656e</t>
-  </si>
-  <si>
-    <t>pou_1c2a1d7b7824d885</t>
-  </si>
-  <si>
-    <t>pou_a7f5f32008710ef1</t>
-  </si>
-  <si>
-    <t>pou_8e06203a6a936959</t>
-  </si>
-  <si>
-    <t>pou_1e5022259348db37;pou_9b10170a3df69f24</t>
-  </si>
-  <si>
-    <t>pou_1f035727f1616384</t>
-  </si>
-  <si>
-    <t>pou_d737d20c37e2bf74</t>
-  </si>
-  <si>
-    <t>pou_c7be9e0f823e43c8</t>
-  </si>
-  <si>
-    <t>pou_4c85c7f6a84642be</t>
-  </si>
-  <si>
-    <t>pou_ffec994370696494</t>
-  </si>
-  <si>
-    <t>pou_aa2c8e02413df498</t>
-  </si>
-  <si>
-    <t>pou_c87b96da149f1855</t>
-  </si>
-  <si>
-    <t>pou_28d32ce019604257</t>
-  </si>
-  <si>
-    <t>pou_123dcfef558f8646</t>
-  </si>
-  <si>
-    <t>pou_06cc40d2dbd20ba9;pou_d5818eee33293a33;pou_8e9ef864b98518e1;pou_f866900dbb3cd573;pou_b33babfbac5f4824;pou_a7a51f510ade153d;pou_b7bf1afb3a6e5ec3</t>
-  </si>
-  <si>
-    <t>pou_608f18027cb30c91;pou_b97d38ac0c2eaf01</t>
-  </si>
-  <si>
-    <t>pou_ce6d66858d33ed47</t>
-  </si>
-  <si>
-    <t>pou_68deed1baa6108c5</t>
-  </si>
-  <si>
-    <t>pou_7c9fab81ffdf9a7a</t>
-  </si>
-  <si>
-    <t>pou_966197b880f5fd7e</t>
-  </si>
-  <si>
-    <t>pou_8f886f348fbabd3a</t>
-  </si>
-  <si>
-    <t>pou_ac7a0a22e8374fc6</t>
-  </si>
-  <si>
-    <t>pou_084aceb497c033cb</t>
-  </si>
-  <si>
-    <t>pou_39e6924735f09f5a</t>
-  </si>
-  <si>
-    <t>pou_06ddf84879b08b81</t>
-  </si>
-  <si>
-    <t>pou_936ce568c7e708d5</t>
-  </si>
-  <si>
-    <t>pou_d5e1f94d93705228</t>
-  </si>
-  <si>
-    <t>pou_de1c892b295cc596;pou_27c3ea6c019eb763;pou_ab8f9a4ca9732ef8;pou_e61384c8b72f69a9;pou_11ea312bc825aaf9;pou_8b9a1c7875e18316;pou_0df9b802e4113703;pou_1eec545ddc7eeb56;pou_63ba011e61e1f584</t>
-  </si>
-  <si>
-    <t>pou_654ab3d22bf15a3c;pou_1fbff09d692070b6;pou_c878e673f3c5a689;pou_404e70992a571549;pou_1f2a3df6a3a6bc44;pou_b9c66d11504184bb;pou_0bda3a6c177ffae3</t>
-  </si>
-  <si>
-    <t>pou_07b59b82e2ae21bb</t>
-  </si>
-  <si>
-    <t>pou_3a52b8d9dbfa36d2;pou_9356f388639c1e7b;pou_cf513549f8c22d64;pou_41e33f2792aca08d</t>
-  </si>
-  <si>
-    <t>pou_4c074ea757e3667d;pou_d7f138e54eeaba06;pou_7d1b51b716d6af81;pou_18b10d8b068a958f;pou_f478c19a5952ade5;pou_e521b52074e7c446;pou_5ff062e6279d1daa;pou_baeee29f0ca0ce7f;pou_9f5bdec38257afda;pou_e277e00b8897ada6</t>
-  </si>
-  <si>
-    <t>pou_656affc5d719cce8</t>
-  </si>
-  <si>
-    <t>pou_15bb891e55364e31;pou_c5000ecbfe878779;pou_77a73b065933b1d6;pou_34959e9fc1a9e9a6;pou_73c0902f5d185c8e;pou_90188d971a087efb;pou_4bcc36c4a1b8855a;pou_b3cee747309113cd;pou_e9bc72453b36f2a5;pou_069fd6b61239fd2e;pou_70aae3d82b286219;pou_289ce28f456a2c6d;pou_7da2db5a3764acaa;pou_9f709ac31c0aae82;pou_2517809c121ca792;pou_8c1f56cec9bc6c95;pou_5145fd4146e28bf0;pou_5ba706879a7a75b7;pou_64a8c4dff3881278;pou_e70202adaf7eef84;pou_771e21d7c912d6d3;pou_19ea2796e35a83b8;pou_26f0bcb9c731dbd0;pou_0e994efbee2fa15d;pou_88227fdd4d294fed;pou_78072c7551cfaa90;pou_37c348fc0387eb2b;pou_00cb5a32d8f6ff03;pou_430e964638439ad2;pou_25f6ef4779069741;pou_372823064264ad8e;pou_303c3ed7f99676aa;pou_bb0b59df241cceaf;pou_0e4a94d0743f6a9d;pou_42c6e0181c208800;pou_bb82f36992192e21;pou_87b09d5e70d5694d;pou_e7940097f37605f0;pou_52e8008b5961fa30;pou_7a0436940375cff5;pou_83df9f849d0beecd;pou_63fc2bf03eef8210;pou_68b8c8a5095036db;pou_32e980a1fbbf1bc7;pou_7da499a4e7455a0f;pou_5af3518a325ca17b;pou_081f218b1cef60c1;pou_deeca22aa171db75;pou_1a2108bdb3c500d7;pou_1c2459415221356d;pou_84f8499f860bf69a;pou_65c4179335b2307d;pou_b2c6631be63d56f4;pou_51b5ecd34fce0945;pou_6ad2333642d25e4f;pou_93947007d1276575;pou_f238dbc9d477e3f4;pou_9e982ea20eb84505;pou_27f6abd1af308240;pou_258024d0b3d46a51;pou_08c2d73144a16f55;pou_13bc8adc1622033a;pou_bc9b2f44381d74f7;pou_a349311f92f8f3b3;pou_f894261e06ce801f;pou_961af4077788a23e;pou_3825c8e3b3680ddc;pou_e31cbf11d9237d69;pou_53f8ec42ba9d520c;pou_56f08384a46e34b8;pou_bce5bf6be4a0b696;pou_04fc3ab02a7bd45f;pou_b691160097cf7652;pou_84b54d19b735eb71;pou_8f58eb949c41bd5e;pou_8eeb94011bc58164;pou_1e719d019c23549c;pou_eecbb2f29a470819;pou_fb6eace1a844f502;pou_4c7f19240daf7c8f;pou_6ac4ccb73c211158;pou_5177e87a16a1638f;pou_a06d5b18f835f7cc;pou_16a8e0546481b31f;pou_51ebd29b3e53f640;pou_d162f97f2edbe6f4;pou_3345ca648023946f;pou_143647ad835608ae;pou_2e2e6248e9a633aa;pou_dda5ca0baa80d9a5;pou_815464f847e32f2b;pou_a74857d22d7e3b3c;pou_3fc23ef0fb34edb6;pou_5f00ea434cf54141;pou_dff1fbe2ed1725a0;pou_f1927f71f1d61177;pou_820145dd694c0364;pou_02fd99d00d8ecd4d;pou_f6d9fd67ed6c5394;pou_4320dfe4f004deae;pou_2c8628a8812ece6d;pou_853f8580ecd2eab8;pou_3c32ae40a1df04ca;pou_7d1652fa01ae689c;pou_cd7d5c45a9430eca;pou_fef79f6479570542;pou_625a9658b341af7b;pou_5d09be22ca425ea4;pou_96d62c5d8e1942f9;pou_ecd51e0a33b6b9e4;pou_0b6093f97efa8e92;pou_bb27abec800b69fd;pou_506f597d79d6d213;pou_f2b33464ef970287;pou_d7d334c39b069cd4;pou_9c2de85d5938aa95;pou_099717664515a71b;pou_d49fee111c06054b;pou_1aa2c44cd8b61cbe;pou_d4f8703549d5a915;pou_53b4fd1accb7857e;pou_65e3885b12512d1e;pou_5787530b90288bfb;pou_dbfb47c84f810dee;pou_03dabb3acf0b4827;pou_70eab3d6ca0b55eb;pou_7a11c40edfb48d9f;pou_12416e40cbe8bfb4;pou_8ada0784dc2a130e;pou_4ce91fced0cc7c79;pou_a3995d47aa127fdc;pou_aba72a52309ae4ac;pou_2bec2269a8808b23;pou_5baacac8be8425d7;pou_750cad0e9c1b09df;pou_a2f6b386f6e2b441;pou_b0a6bbe1351c4138;pou_37da1e9e447dc936;pou_885000ebc2e2595d;pou_8bafeed0376b4484;pou_c6e2e575ab18cf70;pou_749295acad89a288;pou_1afafe3f231f7008</t>
-  </si>
-  <si>
-    <t>pou_9b3221da52ccfb8e;pou_a468c3d4db33ca18;pou_a760b8850cd4a600</t>
-  </si>
-  <si>
-    <t>pou_c89dce4f615d5489</t>
-  </si>
-  <si>
-    <t>pou_dc2514c2cb91dd69</t>
-  </si>
-  <si>
-    <t>pou_9f067f1f93cfe6d7</t>
-  </si>
-  <si>
-    <t>pou_ed179b974b0bb46f</t>
-  </si>
-  <si>
-    <t>pou_92b65845c0f0cd92</t>
-  </si>
-  <si>
-    <t>pou_8f8a3da2d0e49147;pou_6315bf716f658d2d;pou_4b2d9f615e37c10d</t>
-  </si>
-  <si>
-    <t>pou_190abfb20bbfc203</t>
-  </si>
-  <si>
-    <t>pou_2dec46ecf378e129</t>
-  </si>
-  <si>
-    <t>pou_0cec2cdb41761829</t>
-  </si>
-  <si>
-    <t>pou_8162bc48afb2a5f3</t>
-  </si>
-  <si>
-    <t>pou_091938f27b63026d</t>
-  </si>
-  <si>
-    <t>pou_2661df583924211c;pou_65adbd987d1a5dd9;pou_bcf31024c41cf82f;pou_b20a9a1aa3f2ea36;pou_56a12b2e57f220ec;pou_e00b874dac06a434;pou_bc400401cb8a0dcc</t>
-  </si>
-  <si>
-    <t>pou_592ab3a685ba9705</t>
-  </si>
-  <si>
-    <t>pou_4feeb205dfe73491</t>
-  </si>
-  <si>
-    <t>pou_5ab353fe49dddbc3;pou_192d0c24357dc2ce</t>
-  </si>
-  <si>
-    <t>pou_d9df3cbcc85f2c48</t>
-  </si>
-  <si>
-    <t>pou_ee5a52e4e8ff2221</t>
-  </si>
-  <si>
-    <t>pou_3087089a8f124e1d</t>
-  </si>
-  <si>
-    <t>pou_60d8243117e0b0cf</t>
-  </si>
-  <si>
-    <t>pou_f2e921c46f2659ce</t>
-  </si>
-  <si>
-    <t>pou_3dea65fb00ea5fa8;pou_606a78c936f4b102</t>
-  </si>
-  <si>
-    <t>pou_e1e62a1e4acf704c;pou_3c401a9459419c7a</t>
-  </si>
-  <si>
-    <t>pou_4d9db521b9859266;pou_d72cb779e542c26a;pou_4b3c090c13a0ec25;pou_cd4be9860b0039c0;pou_c42179e9bd6e8b34;pou_421cce5e61e32a66;pou_67ed0d85eb737ee2;pou_1308b874b4316e7d;pou_63c8128fd7ef9265;pou_5696985e5ece9c5d;pou_18e78d8835b11b81;pou_93bf1f0e02ac8962;pou_396243d1ebe3dd3c;pou_94c83588a30ec7c9;pou_8a71ace04138603c;pou_3908699aa22aad5e;pou_926ad02906fda377;pou_7feb1963d29f1183;pou_b9d2ec7c33604d15;pou_c233088c4586c305;pou_e5062cd241d234fc;pou_0593a23a1423a731;pou_e0e7c51884687871;pou_73aa4b7d252d0742;pou_533dccac27564fc1;pou_c8cfa7ac386d5673;pou_4b5f698906b776d8</t>
-  </si>
-  <si>
-    <t>pou_1c6ca76050b2fb06</t>
-  </si>
-  <si>
-    <t>pou_8bfb6068928da2ec</t>
-  </si>
-  <si>
-    <t>pou_52cca8d7e6bccc98;pou_6552a2e869287664;pou_def3dd4022e00695;pou_68d18b780f075399;pou_2da057e5e532b59a</t>
-  </si>
-  <si>
-    <t>pou_c3090c3eb578de7b;pou_47c70b9002635f3b;pou_0216634f972922ac;pou_28211764ab558a32;pou_d26910199871bfa4;pou_c6abfa2ccc60218d;pou_4b45d8b49f742218;pou_3b7cdb27abd446fe;pou_a98cdd7549014535;pou_7977e56b8383c449;pou_4aa30244dc78c5f8;pou_df41bd860c618103;pou_07e60c8df29865cc;pou_12fd387f7627283d;pou_22d170dac3edf472;pou_99aa5de06cb11793;pou_bd3627c31546d287;pou_c021da55f3370b1d;pou_c9e9f07c8e6c16ad;pou_fb7f608f08813f51;pou_ffc3be589d7d1342;pou_b087b4898756e411;pou_36c951bbaff98c12;pou_70714d09b82b31cf;pou_8f445057e94fc9a8;pou_95f9f9307d5f86fa;pou_ccac55179e713868;pou_9469e560779b24e6;pou_f803c1d321960b59</t>
-  </si>
-  <si>
-    <t>pou_efc2b2b1b98139c7;pou_c41a547b040b684a;pou_7dc0ca2134a30d95;pou_2ace4d714ee61878;pou_daded07e19ee4f90;pou_7243febc6bb5a6d6;pou_6b436f56db1e809f;pou_e5a4329fa67d5db7</t>
-  </si>
-  <si>
-    <t>pou_9573e21bf02bc905;pou_58935557af12e5f4</t>
-  </si>
-  <si>
-    <t>pou_e1e5f297fa88df26</t>
-  </si>
-  <si>
-    <t>pou_771222cc4f3d7113</t>
-  </si>
-  <si>
-    <t>pou_ba2d63a6301a1409;pou_62a75a87da570beb;pou_7d4cd36b845ea0f5;pou_60f97021b3fe68d8;pou_1730eb4faae6992d;pou_21fb79e835d5ec7c;pou_c81bb0322dbbacec;pou_eaf9a58962500eb3;pou_3a451a4c867656e9;pou_f164eccd0ddd6246;pou_c6c6ea467ee7ffe0;pou_46a411dcd97e7e34;pou_ca58acd8020f3b52;pou_0824066b0f5c6370;pou_6c76fe7ee8c9d2fd</t>
-  </si>
-  <si>
-    <t>pou_97916a67f641ed2d;pou_db7504c359bcd729;pou_b7d8a073a0e3f96c;pou_1fae1d51d2f3a6c8;pou_62500f3d7ddd7223;pou_305c625e915e5bea;pou_0d29d9a65cd1be83</t>
-  </si>
-  <si>
-    <t>pou_8f79dfd27be7871e</t>
-  </si>
-  <si>
-    <t>pou_f05b468149695d3c</t>
-  </si>
-  <si>
-    <t>pou_2b998bc840ff7fee</t>
-  </si>
-  <si>
-    <t>pou_da1119345d77fbf2</t>
-  </si>
-  <si>
-    <t>pou_b1f04b40a0f39ad8</t>
-  </si>
-  <si>
-    <t>pou_d044f0fc4e62c653</t>
-  </si>
-  <si>
-    <t>pou_9201886f6c83b386</t>
-  </si>
-  <si>
-    <t>pou_64082b4916d8c843</t>
-  </si>
-  <si>
-    <t>pou_b179c4815cbdeaeb</t>
-  </si>
-  <si>
-    <t>pou_65386d959282c620;pou_899f56762e4647ed;pou_c70afdda7d20d362;pou_d05d7ab780060d43;pou_6bedac37171ae2d7;pou_5c4fb316e2c9a48b;pou_7e721fd157e68cb1;pou_2c8727fc8569503b;pou_9b0a3cb721f58386;pou_22d8492ef8a55698;pou_6e8e378bca79c8ce;pou_5f74b7c77cdef6c0</t>
-  </si>
-  <si>
-    <t>pou_adc67f129c95d046</t>
-  </si>
-  <si>
-    <t>pou_813253d4d4a535e5;pou_03d5584561c1231d</t>
-  </si>
-  <si>
-    <t>pou_731e156f4be8344c;pou_27f1eb62e988dbae;pou_fec8a47b2a526d9f;pou_3e176be12ead265d;pou_cfed9ccedd568a6a;pou_7ab948abe11819db</t>
-  </si>
-  <si>
-    <t>pou_cf0e1324eb21bc6d;pou_3d1ad753bdef14cf;pou_e7f4f7caf968b0ef;pou_67c5060b6442e630;pou_82380462ff121bbc;pou_dc82a81761a88171;pou_519b6530a97a6fba;pou_9d26b82fbebde1ed;pou_0af403faf603c7f8;pou_24c823ab052f9970;pou_06e166e7f07410cc;pou_2d7212135df6a69e;pou_f9800687cc71c9cb;pou_95924c1d370e7107</t>
-  </si>
-  <si>
-    <t>pou_401730971c707d52;pou_121e7270b2831647;pou_b2a06f3169968944;pou_2016607812e8acbd;pou_19c276048907edfc;pou_da4026ef14ec1e8d;pou_813b37386fa4f79a;pou_a7fb22a7406b86cf;pou_d9928dd538c94606;pou_8c145f0a5ee71be5;pou_cf630d1e5b89591c</t>
-  </si>
-  <si>
-    <t>pou_68ddd217ccb99029</t>
-  </si>
-  <si>
-    <t>pou_07ac850fed938a23</t>
-  </si>
-  <si>
-    <t>pou_18a0e11c1a28b653;pou_d793de3ac4c89587;pou_12bc63a657218408;pou_ef54a3b358fcc851;pou_fb102354c83d75a4;pou_f7efc33b824e6f06;pou_91bcd40e45229f02</t>
-  </si>
-  <si>
-    <t>pou_7247a90681d934c7;pou_88187deef9df59d4;pou_1ba441bf07896543;pou_c67440ed19ee0286;pou_f3e9136f39afe989;pou_e2d25bcdc74457c1;pou_d89972af93bc2c53;pou_e4f62f3da753ef77;pou_b120ebc384e37960;pou_ecf83b51acf7b513;pou_2fe40819c9d3b45a;pou_6b9696c5e3fe17d8;pou_60899bc3d86f4bbe;pou_42f94c10702946a3;pou_6a0e8bb48146552c;pou_fac0c65b04e48c90;pou_7ec1e015774f4213;pou_82dba87e73b2f3f8;pou_50bd4b129ab29c21</t>
-  </si>
-  <si>
-    <t>pou_41208c17ddd38bf7</t>
-  </si>
-  <si>
-    <t>pou_311e67755fb87b75;pou_923f6ff98c246314;pou_33440a19823940ac;pou_9fe950847eb56785;pou_f7ca333b977367c9;pou_5b779d687593d3f4</t>
-  </si>
-  <si>
-    <t>pou_bb5a692d8a6d4206</t>
-  </si>
-  <si>
-    <t>pou_567927fc1b32d8c1;pou_b0f5e1d360831b0a;pou_a2a350a7f56d061e</t>
-  </si>
-  <si>
-    <t>pou_e42d723e824db32b</t>
-  </si>
-  <si>
-    <t>pou_bc79eac4f3a79582;pou_fe34cf4da34bb0d8;pou_3bebda11e2116898;pou_bd116d88017007bd;pou_78072e2abcdff325;pou_1dbf26dee95c41f9</t>
-  </si>
-  <si>
-    <t>pou_11af3bf77a5fbe7c</t>
-  </si>
-  <si>
-    <t>pou_be62fcf2c3664437</t>
-  </si>
-  <si>
-    <t>pou_5b99b139f087ae69</t>
-  </si>
-  <si>
-    <t>pou_7ef3c0c9246d51f4;pou_dbdc4390f8681f01;pou_82198f13bb63d154;pou_2c66f8ab8390e45e;pou_3f15ac83fc0b9da7;pou_45bcb69ccbcf3289;pou_927e85acdea06905;pou_b361b32d81f07e6d;pou_6c0fab98ed0adb99;pou_6f02cc8eb6ab5625;pou_f82cd0fbbe198349;pou_145ef5bf7365b9da;pou_44f72656b3128084;pou_dd7ad0fb22af17bc;pou_ff6ed412c13cfd69;pou_e96bf84e3fcee4bc;pou_0fe3822b6646469e;pou_c4843281e1fcfee1;pou_6a283a2d2f866b5f;pou_ee41fcb3c84f3192;pou_ad56091fabc8b4f8</t>
-  </si>
-  <si>
-    <t>pou_85c3266598bcf05d</t>
-  </si>
-  <si>
-    <t>pou_3c43010911cde750</t>
-  </si>
-  <si>
-    <t>pou_0bbd0495ed6f4062</t>
-  </si>
-  <si>
-    <t>pou_3b426e83c0622c81;pou_4210590c76570f46;pou_a4ff93771ed1a06b;pou_289a3fa0855f4959;pou_744984cbfbe4212d;pou_1691044141e1f147;pou_edefd131f80d03bd;pou_7e015e55e4b693bb;pou_3815a6e9e1b4dd90;pou_715b2871a8307aa0;pou_555180e0eb291189;pou_9b7eba4aa20a498a;pou_c3c7a39f94b072b6;pou_174db32ee46c7b08;pou_a15ca6399f651238</t>
-  </si>
-  <si>
-    <t>pou_fe5809363f39cac1</t>
-  </si>
-  <si>
-    <t>pou_96752041b349beb7</t>
-  </si>
-  <si>
-    <t>pou_990ddbb1c6749e9f</t>
-  </si>
-  <si>
-    <t>pou_b069af2bc1ddecf6</t>
-  </si>
-  <si>
-    <t>pou_4067e373c62cb72d</t>
-  </si>
-  <si>
-    <t>pou_6ad56aa3ca46e87a</t>
-  </si>
-  <si>
-    <t>pou_a6dd504ced9b8bd9</t>
-  </si>
-  <si>
-    <t>pou_148cc1370819c52e</t>
-  </si>
-  <si>
-    <t>pou_d428cdd926dcd9c2</t>
-  </si>
-  <si>
-    <t>pou_cc925cf8358bd258</t>
-  </si>
-  <si>
-    <t>pou_c4a7d875979a5939</t>
-  </si>
-  <si>
-    <t>pou_b4d68fbbeee1e735;pou_f7e83ccfb3317228</t>
-  </si>
-  <si>
-    <t>pou_118acaa5dfd3b1e0</t>
-  </si>
-  <si>
-    <t>pou_4c3f495f22ef31fd</t>
-  </si>
-  <si>
-    <t>pou_a9cad8d97bc93d55</t>
-  </si>
-  <si>
-    <t>pou_c7a6e83751530449</t>
-  </si>
-  <si>
-    <t>pou_56b04fc7bb83dadd</t>
-  </si>
-  <si>
-    <t>pou_a9e68d61f08929c5</t>
-  </si>
-  <si>
-    <t>pou_72897dbfe026ea2c</t>
-  </si>
-  <si>
-    <t>pou_97e0ebb6d8918b3c</t>
-  </si>
-  <si>
-    <t>pou_dc270875b1f06bc5</t>
-  </si>
-  <si>
-    <t>pou_f4dd0558c016a41f</t>
-  </si>
-  <si>
-    <t>pou_774bde7ae5bcf981</t>
-  </si>
-  <si>
-    <t>pou_4c3336446f716ed2</t>
-  </si>
-  <si>
-    <t>pou_185a3e2bd1ea0e50</t>
-  </si>
-  <si>
-    <t>pou_2c71e104b9119339</t>
-  </si>
-  <si>
-    <t>pou_e7dea7c7afb39b95</t>
-  </si>
-  <si>
-    <t>pou_a23242c6b639140a</t>
-  </si>
-  <si>
-    <t>pou_b91004bcc7b68e8e</t>
-  </si>
-  <si>
-    <t>pou_4b96a4622c282726</t>
-  </si>
-  <si>
-    <t>pou_e24304761120fb85</t>
-  </si>
-  <si>
-    <t>pou_8dbad8ff0a72b585</t>
-  </si>
-  <si>
-    <t>pou_eb44ce777c2b9667</t>
-  </si>
-  <si>
-    <t>pou_dcf7aa9e06fc581d</t>
-  </si>
-  <si>
-    <t>pou_9ff168e89d4dea35</t>
-  </si>
-  <si>
-    <t>pou_fabaa062700af1cc</t>
-  </si>
-  <si>
-    <t>pou_8274b7b1d85b39ae</t>
-  </si>
-  <si>
-    <t>pou_08dfa3f7cd22b8f9</t>
-  </si>
-  <si>
-    <t>pou_fbccc9b50bb67e40</t>
-  </si>
-  <si>
-    <t>pou_f29fa270bd7e75d1</t>
-  </si>
-  <si>
-    <t>pou_fcef373c80615ef1</t>
-  </si>
-  <si>
-    <t>pou_20a030899e747e2a</t>
-  </si>
-  <si>
-    <t>pou_1618f04bedb721a1</t>
-  </si>
-  <si>
-    <t>pou_3a6d2cbd2a70761e</t>
-  </si>
-  <si>
-    <t>pou_861abc2a7c0f1359</t>
-  </si>
-  <si>
-    <t>pou_c404a704f1b7ea66</t>
-  </si>
-  <si>
-    <t>pou_fa57db1aaa1d2334</t>
-  </si>
-  <si>
-    <t>pou_819c8906d4467d0f</t>
-  </si>
-  <si>
-    <t>pou_e06bc01c06abd110</t>
-  </si>
-  <si>
-    <t>pou_2839e4f84b50de0b</t>
-  </si>
-  <si>
-    <t>pou_8aef084414292602</t>
-  </si>
-  <si>
-    <t>pou_e765715df00dc706</t>
-  </si>
-  <si>
-    <t>pou_a5e41fad447f2a96</t>
-  </si>
-  <si>
-    <t>pou_bce9efb16b8cf947</t>
-  </si>
-  <si>
-    <t>pou_fb7318cf05fc9bd9</t>
-  </si>
-  <si>
-    <t>pou_7b0fc639e88e77d6</t>
-  </si>
-  <si>
-    <t>pou_66c7066284571bc5</t>
-  </si>
-  <si>
-    <t>pou_4d053c88ddf7e140</t>
-  </si>
-  <si>
-    <t>pou_02e4b7d556c387ce</t>
-  </si>
-  <si>
-    <t>pou_19998d9674c927a4</t>
-  </si>
-  <si>
-    <t>pou_40313cd39fc0a96b</t>
-  </si>
-  <si>
-    <t>pou_b9233f252d3fd7c4</t>
-  </si>
-  <si>
-    <t>pou_ea4dfded4a02d3ca</t>
-  </si>
-  <si>
-    <t>pou_52e900a3373b00f9</t>
-  </si>
-  <si>
-    <t>pou_5f9665714379a9e8</t>
-  </si>
-  <si>
-    <t>pou_dbfd16b7fafeb252</t>
-  </si>
-  <si>
-    <t>pou_d6ef4d95554497d9</t>
-  </si>
-  <si>
-    <t>pou_7ae6459265289747</t>
-  </si>
-  <si>
-    <t>pou_305980a0534c82ee</t>
-  </si>
-  <si>
-    <t>pou_d3b0264b4bbf6a0e</t>
-  </si>
-  <si>
-    <t>pou_3a671cbc116972da</t>
-  </si>
-  <si>
-    <t>pou_4b7cd07e40cd4354</t>
-  </si>
-  <si>
-    <t>pou_964c211d1f28fb3d</t>
-  </si>
-  <si>
-    <t>pou_20b566e73bd0f166</t>
-  </si>
-  <si>
-    <t>pou_f4056a0a7000f75a</t>
-  </si>
-  <si>
-    <t>pou_af443053fdd5cd02</t>
-  </si>
-  <si>
-    <t>pou_bd23540ed10f5087</t>
-  </si>
-  <si>
-    <t>pou_f89dc5a5d41f9e35</t>
-  </si>
-  <si>
-    <t>pou_8f98c14e13f0e972</t>
-  </si>
-  <si>
-    <t>pou_6ab3bd499601b5b1</t>
-  </si>
-  <si>
-    <t>pou_1a48a760393eadd6</t>
-  </si>
-  <si>
-    <t>pou_74446005743af677</t>
-  </si>
-  <si>
-    <t>pou_57411b89938457a4</t>
-  </si>
-  <si>
-    <t>pou_8a5850d4f02df3f0</t>
-  </si>
-  <si>
-    <t>pou_49797fac36d7a913</t>
-  </si>
-  <si>
-    <t>pou_e739928ccfeb5735</t>
-  </si>
-  <si>
-    <t>pou_74489ea5378387e1</t>
-  </si>
-  <si>
-    <t>pou_21de50b1941f869a</t>
-  </si>
-  <si>
-    <t>pou_3bb14aab1d791236</t>
-  </si>
-  <si>
-    <t>pou_b5e6366f4d220a79</t>
-  </si>
-  <si>
-    <t>pou_0ae48920663c0517</t>
-  </si>
-  <si>
-    <t>pou_b04d8f5d4d7db9eb</t>
-  </si>
-  <si>
-    <t>pou_d457a36f93b95b1a</t>
-  </si>
-  <si>
-    <t>pou_c63d5707c765a8c9</t>
-  </si>
-  <si>
-    <t>pou_7f12706626f5bcc2</t>
-  </si>
-  <si>
-    <t>pou_be436e743f35dd60</t>
-  </si>
-  <si>
-    <t>pou_c092c71bc8e0ef62</t>
-  </si>
-  <si>
-    <t>pou_a1e96534416754ca</t>
-  </si>
-  <si>
-    <t>pou_b7d247cda103152e</t>
-  </si>
-  <si>
-    <t>pou_162fd2b329c3074c</t>
-  </si>
-  <si>
-    <t>pou_6f6ce2d0b3ec43a9</t>
-  </si>
-  <si>
-    <t>pou_0f556c06997d5880</t>
-  </si>
-  <si>
-    <t>pou_cf3c68185355cb09</t>
-  </si>
-  <si>
-    <t>pou_3ba2c498bbfdd664</t>
-  </si>
-  <si>
-    <t>pou_8528ed74869c8d08</t>
-  </si>
-  <si>
-    <t>pou_814a95a6f45cc528</t>
-  </si>
-  <si>
-    <t>pou_2a94c5688de0f038</t>
-  </si>
-  <si>
-    <t>pou_e8e6c60f9b90f23b</t>
-  </si>
-  <si>
-    <t>pou_4ffe1f879eabf2f1</t>
-  </si>
-  <si>
-    <t>pou_babba591d57dd7ce</t>
-  </si>
-  <si>
-    <t>pou_b08ae516c9e8766b</t>
-  </si>
-  <si>
-    <t>pou_b6a1fbe4b94d4e1a</t>
-  </si>
-  <si>
-    <t>pou_98edae9204bf28e3</t>
-  </si>
-  <si>
-    <t>pou_240a7ed1c08a454b</t>
-  </si>
-  <si>
-    <t>pou_36fc3a5ca5c0b1e2</t>
-  </si>
-  <si>
-    <t>pou_0724a1e8a779cb35</t>
-  </si>
-  <si>
-    <t>pou_c1b9690bbeb0e55b</t>
-  </si>
-  <si>
-    <t>pou_55ac78f53f71fe3c</t>
-  </si>
-  <si>
-    <t>pou_ac3f2e3cb754864e</t>
-  </si>
-  <si>
-    <t>pou_013e90fbf211c4e2</t>
-  </si>
-  <si>
-    <t>pou_c5b9bb7aef0ad559</t>
-  </si>
-  <si>
-    <t>pou_a8794beac5fcab80</t>
-  </si>
-  <si>
-    <t>pou_b90e79ae2f6ede19</t>
-  </si>
-  <si>
-    <t>pou_e3c6d561ce39d976</t>
-  </si>
-  <si>
-    <t>pou_42e4ac3f533afcc8</t>
-  </si>
-  <si>
-    <t>pou_39d12d99672115f5</t>
-  </si>
-  <si>
-    <t>pou_c988eef4cc624034</t>
-  </si>
-  <si>
-    <t>pou_38c32603fb6ee7bd</t>
-  </si>
-  <si>
-    <t>pou_af2f049dc88e032b</t>
-  </si>
-  <si>
-    <t>pou_b749dc6fb4573724</t>
-  </si>
-  <si>
-    <t>pou_3f11b08b7c77314e</t>
-  </si>
-  <si>
-    <t>pou_88d37f4cc428c7d8</t>
-  </si>
-  <si>
-    <t>pou_6335b563a77c5e21</t>
-  </si>
-  <si>
-    <t>pou_e1b37ca0b8a21499</t>
-  </si>
-  <si>
-    <t>pou_686b2ec92e01d01e</t>
-  </si>
-  <si>
-    <t>pou_c06867e80b1f6e8e</t>
-  </si>
-  <si>
-    <t>pou_22991e901b76378e</t>
-  </si>
-  <si>
-    <t>pou_a8c422cad3f1c77e</t>
-  </si>
-  <si>
-    <t>pou_eb4f1b96c04b3934</t>
-  </si>
-  <si>
-    <t>pou_3d4085eec9ec33f0</t>
-  </si>
-  <si>
-    <t>pou_1893c13ad1813c7b</t>
-  </si>
-  <si>
-    <t>pou_bd67a26f6aef75d7</t>
-  </si>
-  <si>
-    <t>pou_3e038a056948477b</t>
-  </si>
-  <si>
-    <t>pou_e7ce853e853eb57b</t>
-  </si>
-  <si>
-    <t>pou_092bb4d58303ec88</t>
-  </si>
-  <si>
-    <t>pou_da59f18c1a112e69</t>
-  </si>
-  <si>
-    <t>pou_9741f48ddf6a6788</t>
-  </si>
-  <si>
-    <t>pou_afcf52218b394e79</t>
-  </si>
-  <si>
-    <t>pou_cd81a4cadd1b349a</t>
-  </si>
-  <si>
-    <t>pou_3843e7674647aa3d</t>
-  </si>
-  <si>
-    <t>pou_530f5c44ccd7a815</t>
-  </si>
-  <si>
-    <t>pou_c226cea6ec537cbe</t>
-  </si>
-  <si>
-    <t>pou_fc474b64ef48fdb4</t>
-  </si>
-  <si>
-    <t>pou_6d66e643e60374e4</t>
-  </si>
-  <si>
-    <t>pou_f374af9bc5313d59</t>
-  </si>
-  <si>
-    <t>pou_dbcb97ff768f6bbd</t>
-  </si>
-  <si>
-    <t>pou_908bf30ec4f82045</t>
-  </si>
-  <si>
-    <t>pou_642fc5c9a2c56505</t>
-  </si>
-  <si>
-    <t>pou_51d508cf272de860</t>
-  </si>
-  <si>
-    <t>pou_f0eb3045a44be6d4</t>
-  </si>
-  <si>
-    <t>pou_8cc953e9d333c81b</t>
-  </si>
-  <si>
-    <t>pou_72a23486ada4a542</t>
-  </si>
-  <si>
-    <t>pou_fdb6852a24dc4296</t>
-  </si>
-  <si>
-    <t>pou_042119649162cac4</t>
-  </si>
-  <si>
-    <t>pou_8dc9f0e5c8a1774b</t>
-  </si>
-  <si>
-    <t>pou_92ea0e72a7429776</t>
-  </si>
-  <si>
-    <t>pou_38850ba3f9b802e9</t>
-  </si>
-  <si>
-    <t>pou_b33d50d4d5e1fcff</t>
-  </si>
-  <si>
-    <t>pou_44e422a2b8780fbc</t>
-  </si>
-  <si>
-    <t>pou_98a9ec06b2e4fdc5</t>
-  </si>
-  <si>
-    <t>pou_4e2120bf75859c0f</t>
-  </si>
-  <si>
-    <t>pou_2c8fbcf8195e9a30</t>
-  </si>
-  <si>
-    <t>pou_a1e3398711ce2b98</t>
-  </si>
-  <si>
-    <t>pou_183837758b29cb3a</t>
-  </si>
-  <si>
-    <t>pou_0f65df658cd6c3ee</t>
-  </si>
-  <si>
-    <t>pou_7d205f9afc97d6e3</t>
-  </si>
-  <si>
-    <t>pou_6d8103708a7a5634</t>
-  </si>
-  <si>
-    <t>pou_0ae515ff90900335</t>
-  </si>
-  <si>
-    <t>pou_64c53cf5c5c5b203</t>
-  </si>
-  <si>
-    <t>pou_056d39321e07f677</t>
-  </si>
-  <si>
-    <t>pou_339dfccd139adc8e</t>
-  </si>
-  <si>
-    <t>pou_4366ecf7e0873163</t>
-  </si>
-  <si>
-    <t>pou_f6f23fae65b8a9a9</t>
-  </si>
-  <si>
-    <t>pou_0caa558f1a0707ff</t>
-  </si>
-  <si>
-    <t>pou_c19de7b9c39358dc</t>
-  </si>
-  <si>
-    <t>pou_bb89cd7c59fde42c</t>
-  </si>
-  <si>
-    <t>pou_36c4f0c3397ba9c2</t>
-  </si>
-  <si>
-    <t>pou_e1ea9707a9a53500</t>
-  </si>
-  <si>
-    <t>pou_13de8620cc7a87d6</t>
-  </si>
-  <si>
-    <t>pou_46e51723a5289039</t>
-  </si>
-  <si>
-    <t>pou_6d0f190451f1e196</t>
-  </si>
-  <si>
-    <t>pou_638ff01257a7b8f0</t>
-  </si>
-  <si>
-    <t>pou_deca3c1e59df9051</t>
-  </si>
-  <si>
-    <t>pou_396047c957baf369</t>
-  </si>
-  <si>
-    <t>pou_5b77794ae5cbb108</t>
-  </si>
-  <si>
-    <t>pou_ca7476b998f1e729</t>
-  </si>
-  <si>
-    <t>pou_991f3847c201b237</t>
-  </si>
-  <si>
-    <t>pou_2dcec0a4a609cb2a</t>
-  </si>
-  <si>
-    <t>pou_045e82438099fb3f</t>
-  </si>
-  <si>
-    <t>pou_f7a78331cfd03ea1</t>
-  </si>
-  <si>
-    <t>pou_fc2f5780564ae865</t>
-  </si>
-  <si>
-    <t>pou_a3c2551b7beb203b</t>
-  </si>
-  <si>
-    <t>pou_1ac06452a5a40122</t>
-  </si>
-  <si>
-    <t>pou_cb355a5486735deb</t>
-  </si>
-  <si>
-    <t>pou_15206ca7d90a67c2</t>
-  </si>
-  <si>
-    <t>pou_532be86b79063684</t>
-  </si>
-  <si>
-    <t>pou_ea6d326c2df7aeea</t>
-  </si>
-  <si>
-    <t>pou_fe31613ce005259a</t>
-  </si>
-  <si>
-    <t>pou_1348c492587cc41d</t>
-  </si>
-  <si>
-    <t>pou_6b32ac6f2657fd82</t>
-  </si>
-  <si>
-    <t>pou_d7ccf6cc26e6b8af</t>
-  </si>
-  <si>
-    <t>pou_cdcb59747d14ce07</t>
-  </si>
-  <si>
-    <t>pou_c99957b2ed9481cc</t>
-  </si>
-  <si>
-    <t>pou_cb22d61d05d77450</t>
-  </si>
-  <si>
-    <t>pou_1b7e4e3b51b9a6d6</t>
-  </si>
-  <si>
-    <t>pou_fe994cb6717c85e4</t>
-  </si>
-  <si>
-    <t>pou_9b77666da2d65a1e</t>
-  </si>
-  <si>
-    <t>pou_4c0a7f6e567c8936</t>
-  </si>
-  <si>
-    <t>pou_fbdaffc85b7df326</t>
-  </si>
-  <si>
-    <t>pou_eedd4241e265dcdf</t>
-  </si>
-  <si>
-    <t>pou_04d91997e8c47afd</t>
-  </si>
-  <si>
-    <t>pou_942aaf4075fd8a12</t>
-  </si>
-  <si>
-    <t>pou_3966def0cf63d6d1</t>
-  </si>
-  <si>
-    <t>pou_6c9e5b81f09cfece</t>
-  </si>
-  <si>
-    <t>pou_129678e5ca5fbd11</t>
-  </si>
-  <si>
-    <t>pou_a9ffa7c88d585379</t>
-  </si>
-  <si>
-    <t>pou_ac5709f53378e053;pou_dd27f13d26b66be7</t>
-  </si>
-  <si>
-    <t>pou_ba5c4cf88014b2d2;pou_180fd95713a4da99;pou_76967c830e9c4e5a;pou_691e833e6ed30623;pou_4aa8fc7616f16b16;pou_83d52843923e3b65;pou_2135cbb85a3b70ba;pou_18fac03a81adfee9;pou_97fd97de3e8ec5cd;pou_260a3184140fb858;pou_1d450d9cc46cbc0a;pou_81293de79af9660b</t>
-  </si>
-  <si>
-    <t>pou_33924a0991211a7c</t>
-  </si>
-  <si>
-    <t>pou_c7e66a60786debfe</t>
-  </si>
-  <si>
-    <t>pou_f38d24bfdb9e97af</t>
-  </si>
-  <si>
-    <t>pou_0693f31a3c8ad5fd</t>
-  </si>
-  <si>
-    <t>pou_a96fd0749197f776</t>
-  </si>
-  <si>
-    <t>pou_128841edb0b75b27</t>
-  </si>
-  <si>
-    <t>pou_dfa2ab5c76dc4ff0</t>
-  </si>
-  <si>
-    <t>pou_b4d9d21843a42dca</t>
-  </si>
-  <si>
-    <t>pou_6b3173257ce2eacf</t>
-  </si>
-  <si>
-    <t>pou_41f3689baa472644</t>
-  </si>
-  <si>
-    <t>pou_8b7bca48e0f17a48</t>
-  </si>
-  <si>
-    <t>pou_ba3eeab3625699a7</t>
-  </si>
-  <si>
-    <t>pou_2c10102d75c03624</t>
-  </si>
-  <si>
-    <t>pou_f8512bf6de1b5350</t>
-  </si>
-  <si>
-    <t>pou_2e4ab4b44d21cf3b</t>
-  </si>
-  <si>
-    <t>pou_75ff3436c436cdf7</t>
-  </si>
-  <si>
-    <t>pou_e47d60d5603ed1af</t>
-  </si>
-  <si>
-    <t>pou_b9e2fff68dfb462f</t>
-  </si>
-  <si>
-    <t>pou_9636eb316a42a9b6</t>
-  </si>
-  <si>
-    <t>pou_be03e3df7dae4eb1</t>
-  </si>
-  <si>
-    <t>pou_26810cb5b1809e64</t>
-  </si>
-  <si>
-    <t>pou_0d902cf6a4b97024</t>
-  </si>
-  <si>
-    <t>pou_13e3b34b9c28890f</t>
-  </si>
-  <si>
-    <t>pou_2e9a12943710923d</t>
-  </si>
-  <si>
-    <t>pou_59962f3a866f101d</t>
-  </si>
-  <si>
-    <t>pou_3ad164bf4be26ae8</t>
-  </si>
-  <si>
-    <t>pou_185363c8f98228f9</t>
-  </si>
-  <si>
-    <t>pou_b32bde18329d4d47</t>
-  </si>
-  <si>
-    <t>pou_9418b72bb07aa6f7</t>
-  </si>
-  <si>
-    <t>pou_0f43f1153fb24b61</t>
-  </si>
-  <si>
-    <t>pou_aa0a5e2317ce4e99</t>
-  </si>
-  <si>
-    <t>pou_e793c87bf60333a0</t>
-  </si>
-  <si>
-    <t>pou_276954732356fe86</t>
-  </si>
-  <si>
-    <t>pou_9a834caa0e006c0e</t>
-  </si>
-  <si>
-    <t>pou_6d28fd01bb1900c3</t>
-  </si>
-  <si>
-    <t>pou_b33949295bd68ab9</t>
-  </si>
-  <si>
-    <t>pou_e0acdf2531084b02</t>
-  </si>
-  <si>
-    <t>pou_b43007d81ec0eae4</t>
-  </si>
-  <si>
-    <t>pou_6be0ad34dfb79c9e</t>
-  </si>
-  <si>
-    <t>pou_2370b02b14356608</t>
-  </si>
-  <si>
-    <t>pou_3f21190aadd182e4</t>
-  </si>
-  <si>
-    <t>pou_09d2519148f07f49</t>
+    <t>pou_f24eb51424f88b62</t>
+  </si>
+  <si>
+    <t>pou_8e8bb4f612ecc869</t>
+  </si>
+  <si>
+    <t>pou_b1d943c79554edf6;pou_486d66f2173713b4</t>
+  </si>
+  <si>
+    <t>pou_c6642a78d328cbe0</t>
+  </si>
+  <si>
+    <t>pou_a4a6cd7562bb2fc6</t>
+  </si>
+  <si>
+    <t>pou_59bb6edfaea4263a</t>
+  </si>
+  <si>
+    <t>pou_1981c4a315e125ed</t>
+  </si>
+  <si>
+    <t>pou_bb62bca15eb4505b</t>
+  </si>
+  <si>
+    <t>pou_db157609a270d7f9</t>
+  </si>
+  <si>
+    <t>pou_5a78427920139029</t>
+  </si>
+  <si>
+    <t>pou_286c200d76e7ce9c</t>
+  </si>
+  <si>
+    <t>pou_df1fd9a659470efa</t>
+  </si>
+  <si>
+    <t>pou_9650bc8bce81360d</t>
+  </si>
+  <si>
+    <t>pou_b4e81e09d77ad309</t>
+  </si>
+  <si>
+    <t>pou_77fac64d12c1229f;pou_89c6c0985e443d25</t>
+  </si>
+  <si>
+    <t>pou_7061fa9e02c1924c</t>
+  </si>
+  <si>
+    <t>pou_aaa3b2674d7d556a</t>
+  </si>
+  <si>
+    <t>pou_02b9679ebd296058;pou_fd957fabaf2d2aab</t>
+  </si>
+  <si>
+    <t>pou_30b799c19368fccf</t>
+  </si>
+  <si>
+    <t>pou_b83e84efa9743225</t>
+  </si>
+  <si>
+    <t>pou_79231d74d43af48c</t>
+  </si>
+  <si>
+    <t>pou_ebc3240b92702b84</t>
+  </si>
+  <si>
+    <t>pou_51c3a42dbbbffd86;pou_a5923be7f721ec92</t>
+  </si>
+  <si>
+    <t>pou_0c99d9786694e2bb;pou_611a955bbbbb2e82</t>
+  </si>
+  <si>
+    <t>pou_89acef9bb493c97b</t>
+  </si>
+  <si>
+    <t>pou_a4094a46c7c140b4</t>
+  </si>
+  <si>
+    <t>pou_4dd70e322f5db8a5</t>
+  </si>
+  <si>
+    <t>pou_7f5872ba831bf695;pou_24b27df60d490ca1;pou_3af405f4aab1aed5;pou_afcb4331b950945a;pou_d409d279486cf2e2;pou_b5c6aea3a2d3a57a;pou_6bf1e29b6ed0ea9f;pou_2bdd7c48a9a92294;pou_928ac59bb40da6c7</t>
+  </si>
+  <si>
+    <t>pou_fc77126f8cf93a0e</t>
+  </si>
+  <si>
+    <t>pou_babbe07e56bb0c2f</t>
+  </si>
+  <si>
+    <t>pou_a9c3ad22153ee02e</t>
+  </si>
+  <si>
+    <t>pou_87a82b9d1f6ee985</t>
+  </si>
+  <si>
+    <t>pou_32c0dc04be0632c6</t>
+  </si>
+  <si>
+    <t>pou_c68e882711c34a15</t>
+  </si>
+  <si>
+    <t>pou_7e938680764829af;pou_2347435230a42925</t>
+  </si>
+  <si>
+    <t>pou_fbaf2d40e2d610b8</t>
+  </si>
+  <si>
+    <t>pou_f873df811f328259</t>
+  </si>
+  <si>
+    <t>pou_9457db1c2e23381a</t>
+  </si>
+  <si>
+    <t>pou_995bf5d2dfa33466;pou_7365cfb69c58c776</t>
+  </si>
+  <si>
+    <t>pou_19158f196e08eb47</t>
+  </si>
+  <si>
+    <t>pou_0dac7ac9b01ce924</t>
+  </si>
+  <si>
+    <t>pou_8abea929cd45afb4</t>
+  </si>
+  <si>
+    <t>pou_64a8dba1b1115de5</t>
+  </si>
+  <si>
+    <t>pou_3dfbc4ecab31628b</t>
+  </si>
+  <si>
+    <t>pou_83262a50454e0c0a</t>
+  </si>
+  <si>
+    <t>pou_f25247cda5ad1baa;pou_d6c87dc3d2b05622</t>
+  </si>
+  <si>
+    <t>pou_29966e965f83299f</t>
+  </si>
+  <si>
+    <t>pou_3c83f846a9ea07e3</t>
+  </si>
+  <si>
+    <t>pou_fce128c04535f8c5</t>
+  </si>
+  <si>
+    <t>pou_27be48cf736aa4d4</t>
+  </si>
+  <si>
+    <t>pou_568a6bff6add8060</t>
+  </si>
+  <si>
+    <t>pou_d9b6ce98ab980513</t>
+  </si>
+  <si>
+    <t>pou_9c3c1cda64f03d3d</t>
+  </si>
+  <si>
+    <t>pou_b8a5f9f2414a2798</t>
+  </si>
+  <si>
+    <t>pou_58f41fe8d1916979</t>
+  </si>
+  <si>
+    <t>pou_285388dca6ead21f</t>
+  </si>
+  <si>
+    <t>pou_fbb8bb50f1630d3a</t>
+  </si>
+  <si>
+    <t>pou_6f6e6f30231492bd</t>
+  </si>
+  <si>
+    <t>pou_b33ed17441159453</t>
+  </si>
+  <si>
+    <t>pou_2e86cebf6b699d8f</t>
+  </si>
+  <si>
+    <t>pou_aa5c878f81779b49</t>
+  </si>
+  <si>
+    <t>pou_b2665cd7ff39c525</t>
+  </si>
+  <si>
+    <t>pou_0a09bbf309583d2d</t>
+  </si>
+  <si>
+    <t>pou_9f53453f55371553</t>
+  </si>
+  <si>
+    <t>pou_8367f4c49c9e467c</t>
+  </si>
+  <si>
+    <t>pou_c67919d584d4d8ab</t>
+  </si>
+  <si>
+    <t>pou_183a245a35b84538</t>
+  </si>
+  <si>
+    <t>pou_4edf14590c520ae7</t>
+  </si>
+  <si>
+    <t>pou_9b394d2b4f361adb</t>
+  </si>
+  <si>
+    <t>pou_5d8ff769178fd365</t>
+  </si>
+  <si>
+    <t>pou_7e68e83ed227446d</t>
+  </si>
+  <si>
+    <t>pou_dc1b08cca08f2fa9</t>
+  </si>
+  <si>
+    <t>pou_1f913b063f542940</t>
+  </si>
+  <si>
+    <t>pou_b027954f6840ea5f</t>
+  </si>
+  <si>
+    <t>pou_141d1cd49a2ec1f1</t>
+  </si>
+  <si>
+    <t>pou_759dbb8e73e12720</t>
+  </si>
+  <si>
+    <t>pou_6eb923c652a44eea</t>
+  </si>
+  <si>
+    <t>pou_a8b7ce58e486a4e5</t>
+  </si>
+  <si>
+    <t>pou_6ff3d19ce04f0829</t>
+  </si>
+  <si>
+    <t>pou_55e4a6f6ca6ea318</t>
+  </si>
+  <si>
+    <t>pou_8510d89e19d6d061</t>
+  </si>
+  <si>
+    <t>pou_3482b580e0bda838</t>
+  </si>
+  <si>
+    <t>pou_2c9d2ce6c10cc7fb</t>
+  </si>
+  <si>
+    <t>pou_f5ea63c907fe3a61</t>
+  </si>
+  <si>
+    <t>pou_77e23e9b47dd2f68</t>
+  </si>
+  <si>
+    <t>pou_61525256e318c9d0</t>
+  </si>
+  <si>
+    <t>pou_d6ce6e898bc19a33</t>
+  </si>
+  <si>
+    <t>pou_3c71e524fcfccdca</t>
+  </si>
+  <si>
+    <t>pou_7600cd2ba52a5906</t>
+  </si>
+  <si>
+    <t>pou_2fcf77af8b48b637</t>
+  </si>
+  <si>
+    <t>pou_52247fbe0929b272</t>
+  </si>
+  <si>
+    <t>pou_94362bd70407b6ae</t>
+  </si>
+  <si>
+    <t>pou_880a84ed791a95ba</t>
+  </si>
+  <si>
+    <t>pou_8971cb7a64afe3de</t>
+  </si>
+  <si>
+    <t>pou_c91d80326b62e763</t>
+  </si>
+  <si>
+    <t>pou_0f15dccc3a612472</t>
+  </si>
+  <si>
+    <t>pou_2ef6503ba163131a</t>
+  </si>
+  <si>
+    <t>pou_d7ebc9e68ad1952a</t>
+  </si>
+  <si>
+    <t>pou_d489b3c93e096b8b</t>
+  </si>
+  <si>
+    <t>pou_f4bbca71a13b0c1f</t>
+  </si>
+  <si>
+    <t>pou_96ad43ac23203cdd</t>
+  </si>
+  <si>
+    <t>pou_62d30ac686347fcd</t>
+  </si>
+  <si>
+    <t>pou_c58451c304f7d05f</t>
+  </si>
+  <si>
+    <t>pou_f22f43b0c35a45ef</t>
+  </si>
+  <si>
+    <t>pou_46cb86db61671924</t>
+  </si>
+  <si>
+    <t>pou_24fd4f048834dfd2</t>
+  </si>
+  <si>
+    <t>pou_fa83419f8adc54f9</t>
+  </si>
+  <si>
+    <t>pou_5a1453fc24257774</t>
+  </si>
+  <si>
+    <t>pou_0a4e20638d4d38eb</t>
+  </si>
+  <si>
+    <t>pou_1d3af3f0dd483e89</t>
+  </si>
+  <si>
+    <t>pou_537190b55122d1e3</t>
+  </si>
+  <si>
+    <t>pou_4ed02675765f129f</t>
+  </si>
+  <si>
+    <t>pou_ec1f6b395b55078f</t>
+  </si>
+  <si>
+    <t>pou_079504445a342e00</t>
+  </si>
+  <si>
+    <t>pou_d04451950e92ce49</t>
+  </si>
+  <si>
+    <t>pou_069558d32ece92e5</t>
+  </si>
+  <si>
+    <t>pou_54ae6652bb3c0fd1</t>
+  </si>
+  <si>
+    <t>pou_6d2c833effc8855a</t>
+  </si>
+  <si>
+    <t>pou_f9334b4b41079c6a</t>
+  </si>
+  <si>
+    <t>pou_1149d85f7814d0ed</t>
+  </si>
+  <si>
+    <t>pou_0088e3a0c1516446</t>
+  </si>
+  <si>
+    <t>pou_2eeff31d669d7593</t>
+  </si>
+  <si>
+    <t>pou_68f302b12e870f0d</t>
+  </si>
+  <si>
+    <t>pou_019e50ac8cea68d9</t>
+  </si>
+  <si>
+    <t>pou_f0c458ede05d27fb</t>
+  </si>
+  <si>
+    <t>pou_f6215282a60207e5;pou_19b5528128e9a2ac;pou_256378a2cf697a7b</t>
+  </si>
+  <si>
+    <t>pou_827c99daea52280c</t>
+  </si>
+  <si>
+    <t>pou_74fb25421f13ccbc</t>
+  </si>
+  <si>
+    <t>pou_cd2a1742b5ea8c69</t>
+  </si>
+  <si>
+    <t>pou_ec426bdaa289e6c5;pou_c0ffdfa6fbb77624</t>
+  </si>
+  <si>
+    <t>pou_08bb7772cd802cd8</t>
+  </si>
+  <si>
+    <t>pou_692bb74ce7fbc9fe</t>
+  </si>
+  <si>
+    <t>pou_4c3fb15904dbfee0</t>
+  </si>
+  <si>
+    <t>pou_ebad4bc7db4f3754</t>
+  </si>
+  <si>
+    <t>pou_a45d5bdcc09c0695</t>
+  </si>
+  <si>
+    <t>pou_a38778119c40583f</t>
+  </si>
+  <si>
+    <t>pou_de35ebf6eaa69c26</t>
+  </si>
+  <si>
+    <t>pou_c2cbe8a31239dfea</t>
+  </si>
+  <si>
+    <t>pou_5aa5cbec6cc044fb</t>
+  </si>
+  <si>
+    <t>pou_ed7b5c3c97cae9f9</t>
+  </si>
+  <si>
+    <t>pou_5ee69d3f03322af2</t>
+  </si>
+  <si>
+    <t>pou_e09f4b31064eb50c</t>
+  </si>
+  <si>
+    <t>pou_ff06472f1660edc1</t>
+  </si>
+  <si>
+    <t>pou_824f1da18b954c80</t>
+  </si>
+  <si>
+    <t>pou_72f739c8a9807532</t>
+  </si>
+  <si>
+    <t>pou_1238e70fda77f65f</t>
+  </si>
+  <si>
+    <t>pou_1badf265b331623a</t>
+  </si>
+  <si>
+    <t>pou_b5878514379ccf5e</t>
+  </si>
+  <si>
+    <t>pou_57cf3567f664cda8</t>
+  </si>
+  <si>
+    <t>pou_6cfb16946c09eee8</t>
+  </si>
+  <si>
+    <t>pou_863401674c6691db;pou_607b148e3ce80b05;pou_ef5144b151552532;pou_c09c4c137c180595;pou_b83c8dd6ef36c30f;pou_ba23a9763bf65408;pou_1d4fdee4a3173279;pou_ecf2153a4bf06b28;pou_642b404c52b03daa;pou_f33f590b0de3807a;pou_1588bfffb9844bdf</t>
+  </si>
+  <si>
+    <t>pou_23c037a8b7751ef5</t>
+  </si>
+  <si>
+    <t>pou_75b2e8647dfa7563</t>
+  </si>
+  <si>
+    <t>pou_c920ffc01fe9a1cc;pou_40721df5fce15266</t>
+  </si>
+  <si>
+    <t>pou_7487f71ed27e45a7</t>
+  </si>
+  <si>
+    <t>pou_d245ef20be960f91</t>
+  </si>
+  <si>
+    <t>pou_687dfc827e71095a</t>
+  </si>
+  <si>
+    <t>pou_b7a0a08ec96c5178</t>
+  </si>
+  <si>
+    <t>pou_9aa056bdaf8778f0</t>
+  </si>
+  <si>
+    <t>pou_edcb4729f8fc33a4</t>
+  </si>
+  <si>
+    <t>pou_77d41bdfedca48a8</t>
+  </si>
+  <si>
+    <t>pou_72386367493bafab</t>
+  </si>
+  <si>
+    <t>pou_45a844a65ed14a0f</t>
+  </si>
+  <si>
+    <t>pou_fcdc20aafa2e69c9</t>
+  </si>
+  <si>
+    <t>pou_8c4caee9481c3a12</t>
+  </si>
+  <si>
+    <t>pou_015e3b815ed105f4</t>
+  </si>
+  <si>
+    <t>pou_c514263a6ea15295</t>
+  </si>
+  <si>
+    <t>pou_a190126d8aaae6fa</t>
+  </si>
+  <si>
+    <t>pou_400bae93cca0200d</t>
+  </si>
+  <si>
+    <t>pou_3f139672cba0843f</t>
+  </si>
+  <si>
+    <t>pou_042aea9a09cfd90c</t>
+  </si>
+  <si>
+    <t>pou_1d617e1258d4e6d6</t>
+  </si>
+  <si>
+    <t>pou_12a1767b81102de0</t>
+  </si>
+  <si>
+    <t>pou_ff5914ae4434fc34</t>
+  </si>
+  <si>
+    <t>pou_7eece01521ab3514</t>
+  </si>
+  <si>
+    <t>pou_30bb6220f78b5576</t>
+  </si>
+  <si>
+    <t>pou_7279d55ec53de8b8</t>
+  </si>
+  <si>
+    <t>pou_04642ac899ca99ad</t>
+  </si>
+  <si>
+    <t>pou_e8b47d9148299c11</t>
+  </si>
+  <si>
+    <t>pou_27b1a1c4fdcc429d</t>
+  </si>
+  <si>
+    <t>pou_390091b27eef0c19</t>
+  </si>
+  <si>
+    <t>pou_b8de6ca1013fd490</t>
+  </si>
+  <si>
+    <t>pou_947353069ea67cc2</t>
+  </si>
+  <si>
+    <t>pou_cfc2e98f0450aa73</t>
+  </si>
+  <si>
+    <t>pou_e43b006a07d3698a</t>
+  </si>
+  <si>
+    <t>pou_9991a953faf330ee</t>
+  </si>
+  <si>
+    <t>pou_ae57e4c61eba4234</t>
+  </si>
+  <si>
+    <t>pou_b6c3740d7f729904</t>
+  </si>
+  <si>
+    <t>pou_b069654d75122199</t>
+  </si>
+  <si>
+    <t>pou_0224370c05a75058</t>
+  </si>
+  <si>
+    <t>pou_aacdfd170573b14d</t>
+  </si>
+  <si>
+    <t>pou_b39bb9bdd8c86112</t>
+  </si>
+  <si>
+    <t>pou_187eab67e0be9d00</t>
+  </si>
+  <si>
+    <t>pou_560741f87ae0b24e</t>
+  </si>
+  <si>
+    <t>pou_57e83e9f2ef0b27b</t>
+  </si>
+  <si>
+    <t>pou_cf741a101e7e3424</t>
+  </si>
+  <si>
+    <t>pou_1903be7f76f1746c</t>
+  </si>
+  <si>
+    <t>pou_be6e76442aa48411</t>
+  </si>
+  <si>
+    <t>pou_664e00507959fc1d</t>
+  </si>
+  <si>
+    <t>pou_e23fc661ffd78541</t>
+  </si>
+  <si>
+    <t>pou_e1db92a6176bdd59</t>
+  </si>
+  <si>
+    <t>pou_4742ed7bb6f1cae3</t>
+  </si>
+  <si>
+    <t>pou_0461939b4ea8d293</t>
+  </si>
+  <si>
+    <t>pou_6d5e08ecce2cb9ad</t>
+  </si>
+  <si>
+    <t>pou_f1fed661c263835d</t>
+  </si>
+  <si>
+    <t>pou_13d52b3a93c0b904</t>
+  </si>
+  <si>
+    <t>pou_54a00b817c4efd94</t>
+  </si>
+  <si>
+    <t>pou_e958138325df6a66</t>
+  </si>
+  <si>
+    <t>pou_b276e6becd0bb7d8</t>
+  </si>
+  <si>
+    <t>pou_78fb1a153221126a</t>
+  </si>
+  <si>
+    <t>pou_a5fd4243411c1ac8</t>
+  </si>
+  <si>
+    <t>pou_b909f498a88410b5</t>
+  </si>
+  <si>
+    <t>pou_9d6a5695a0a4df76</t>
+  </si>
+  <si>
+    <t>pou_b432e5606bbb511d</t>
+  </si>
+  <si>
+    <t>pou_acb26e9372bcfe37</t>
+  </si>
+  <si>
+    <t>pou_aec1e726b21a7dc5</t>
+  </si>
+  <si>
+    <t>pou_be08c5d2d5bd026c</t>
+  </si>
+  <si>
+    <t>pou_2e4714fefafe476b</t>
+  </si>
+  <si>
+    <t>pou_1518635532f12ef6</t>
+  </si>
+  <si>
+    <t>pou_fb9cde85b0de078d</t>
+  </si>
+  <si>
+    <t>pou_450562be7feb05d3</t>
+  </si>
+  <si>
+    <t>pou_48da2808f868c7c8</t>
+  </si>
+  <si>
+    <t>pou_68fb39eb6565bf68</t>
+  </si>
+  <si>
+    <t>pou_9993ad866cdcc128</t>
+  </si>
+  <si>
+    <t>pou_766f9f42bb672814</t>
+  </si>
+  <si>
+    <t>pou_be3a87515a8fc092</t>
+  </si>
+  <si>
+    <t>pou_383d98ea40689895</t>
+  </si>
+  <si>
+    <t>pou_1f094d1d1c64d9e1</t>
+  </si>
+  <si>
+    <t>pou_1bd4c41381966ea5</t>
+  </si>
+  <si>
+    <t>pou_3967b993ad6ebdec</t>
+  </si>
+  <si>
+    <t>pou_19acc221f9ec6f4e</t>
+  </si>
+  <si>
+    <t>pou_7768d965823bec80</t>
+  </si>
+  <si>
+    <t>pou_c72fca366dd18adb</t>
+  </si>
+  <si>
+    <t>pou_4290bece90c803b0</t>
+  </si>
+  <si>
+    <t>pou_c8cde19bb1d57c0c</t>
+  </si>
+  <si>
+    <t>pou_a69f07c6dce7c7e3</t>
+  </si>
+  <si>
+    <t>pou_f5e3e9b6966ddbf8</t>
+  </si>
+  <si>
+    <t>pou_2a8d0829bac47bb9</t>
+  </si>
+  <si>
+    <t>pou_e84e5dc821c13a96</t>
+  </si>
+  <si>
+    <t>pou_432c225ea01960d8</t>
+  </si>
+  <si>
+    <t>pou_ffebf213174f9bbf</t>
+  </si>
+  <si>
+    <t>pou_ca844d28e060a26b</t>
+  </si>
+  <si>
+    <t>pou_71b7d43ef0d89859</t>
+  </si>
+  <si>
+    <t>pou_0669133a2e2ad894</t>
+  </si>
+  <si>
+    <t>pou_cb1c070c3a9f402e</t>
+  </si>
+  <si>
+    <t>pou_8a3aa425e51e23b3</t>
+  </si>
+  <si>
+    <t>pou_8cffe8bc929684b2</t>
+  </si>
+  <si>
+    <t>pou_c125ade96694952c</t>
+  </si>
+  <si>
+    <t>pou_fa52eb8d2aa954ab</t>
+  </si>
+  <si>
+    <t>pou_8b9a184a1e4fc5a0</t>
+  </si>
+  <si>
+    <t>pou_ad95335fcf3b539e</t>
+  </si>
+  <si>
+    <t>pou_18b05b8e44144b42</t>
+  </si>
+  <si>
+    <t>pou_95844d2266068a7a</t>
+  </si>
+  <si>
+    <t>pou_072e6d4ffe785c51</t>
+  </si>
+  <si>
+    <t>pou_ecfc609e5df07fce</t>
+  </si>
+  <si>
+    <t>pou_c2a8cd3007a941bd</t>
+  </si>
+  <si>
+    <t>pou_8135ec10d685c82d</t>
+  </si>
+  <si>
+    <t>pou_55c2b395ff5ea88d</t>
+  </si>
+  <si>
+    <t>pou_2df6c7a4e5a9b062</t>
+  </si>
+  <si>
+    <t>pou_5ac8537bc396b583</t>
+  </si>
+  <si>
+    <t>pou_57a826cd39b20290</t>
+  </si>
+  <si>
+    <t>pou_6edc783fd5c2c96d</t>
+  </si>
+  <si>
+    <t>pou_9b7b0efa5b625531;pou_e8636cd57dacb069</t>
+  </si>
+  <si>
+    <t>pou_37bf951d4622786f</t>
+  </si>
+  <si>
+    <t>pou_e47e30d2a1e6d70d;pou_dc8d92db78892700;pou_8bde76e8769ea5bd;pou_43568fc168fa68d6;pou_3daab271de65b6ca;pou_e632fc77fd577a50;pou_9f9285e5387f6e0d;pou_dcacbf59c0e1d855;pou_e5e36f5efc7843de;pou_758255af3e974872;pou_5ff4a1b14fd91c3c;pou_d8ba029fc76f41f7</t>
+  </si>
+  <si>
+    <t>pou_ba6014de1beee8ec</t>
+  </si>
+  <si>
+    <t>pou_773b7e5622ff67d3</t>
+  </si>
+  <si>
+    <t>pou_4e26c56ae8632e1b</t>
+  </si>
+  <si>
+    <t>pou_cb3f9b73ac3f534d</t>
+  </si>
+  <si>
+    <t>pou_1fdbdf696ec4b9c8</t>
+  </si>
+  <si>
+    <t>pou_8e07b153f67a8b75</t>
+  </si>
+  <si>
+    <t>pou_aa54ee22018db3b0</t>
+  </si>
+  <si>
+    <t>pou_9a6dc2c24deab0b0</t>
+  </si>
+  <si>
+    <t>pou_51ac0fe4f635da09</t>
+  </si>
+  <si>
+    <t>pou_c4bb494eea755d33</t>
+  </si>
+  <si>
+    <t>pou_f80471d57e68eafa;pou_2f28d756c9bca18e</t>
+  </si>
+  <si>
+    <t>pou_f8175ad8f1a81717</t>
+  </si>
+  <si>
+    <t>pou_ddc9eac2b51c09a0</t>
+  </si>
+  <si>
+    <t>pou_f50b529a417b42ae</t>
+  </si>
+  <si>
+    <t>pou_e4f3e3121b9f76d2</t>
+  </si>
+  <si>
+    <t>pou_d6b254ecf49efd88</t>
+  </si>
+  <si>
+    <t>pou_a23cfc68cfd3f02f</t>
+  </si>
+  <si>
+    <t>pou_892fa63bec787f0d</t>
+  </si>
+  <si>
+    <t>pou_6fdb24c47de640e0</t>
+  </si>
+  <si>
+    <t>pou_7c1bfa242408c4e0</t>
+  </si>
+  <si>
+    <t>pou_8ca467cf4aca7a51;pou_0276c68c66dbd1a1;pou_20dfc3e67829dec6;pou_082a78d17a69d16b;pou_da7ed0bfafd10fab;pou_e6aaa2b7e1216d6b;pou_25ea6be11ed725dd</t>
+  </si>
+  <si>
+    <t>pou_6e0349a27d56b428;pou_04d795120b6519ee</t>
+  </si>
+  <si>
+    <t>pou_ae468a6b8f1feeae</t>
+  </si>
+  <si>
+    <t>pou_49a75e7a763f1f8b</t>
+  </si>
+  <si>
+    <t>pou_a53c69a9a618a931</t>
+  </si>
+  <si>
+    <t>pou_94c9a99338172d9b</t>
+  </si>
+  <si>
+    <t>pou_9b450bee72a12860</t>
+  </si>
+  <si>
+    <t>pou_7356f5f570b75cfc</t>
+  </si>
+  <si>
+    <t>pou_967f4df71797c169</t>
+  </si>
+  <si>
+    <t>pou_c166434da8dc7b7e</t>
+  </si>
+  <si>
+    <t>pou_3b5a01bd242a3958</t>
+  </si>
+  <si>
+    <t>pou_394b08252401db6a</t>
+  </si>
+  <si>
+    <t>pou_552789acb5603dd4</t>
+  </si>
+  <si>
+    <t>pou_db4ea0c027ce2a6a;pou_751f841f76d9dadf;pou_5eba88244e55e0a6;pou_2dee6b5b46fe2fd6;pou_5d909629ba60a572;pou_26d153c122e92984;pou_793e2bc4926c4467;pou_030732e41b972f30;pou_dcd2de03d2e2afc4</t>
+  </si>
+  <si>
+    <t>pou_53f613b0acbfdc8d;pou_5f2d7d2d98df3980;pou_83ce51684c01b4ce;pou_33381662d14f2c26;pou_96d5768246d41ab7;pou_8c9e0c5ada27deb4;pou_9812433104aa39cf</t>
+  </si>
+  <si>
+    <t>pou_637a2bf9feda826c</t>
+  </si>
+  <si>
+    <t>pou_3b85f5dfef5eb60f;pou_452b4caf250a7ec3;pou_7a85807bb6286232;pou_671bd99ac93ea3b6</t>
+  </si>
+  <si>
+    <t>pou_0741b9bde4a30b51;pou_430b7fad20b5ca4b;pou_6dfa54192bc4cea4;pou_fc0f58be13f2287e;pou_89e145059bba35b7;pou_e718348b4a7f6744;pou_69424ddbf56f628b;pou_c11703a112df6432;pou_9d08c35507522e4d;pou_ab0f0032ef44d752</t>
+  </si>
+  <si>
+    <t>pou_176a137ec6404b2c</t>
+  </si>
+  <si>
+    <t>pou_e941c16499604bac;pou_24f05bd75fe85239;pou_c8739c5009172b51;pou_8208d599c9490193;pou_27156cb4558c4107;pou_fa8c72a8d726a85f;pou_13faf8e5ee7e1d8e;pou_c30ff0a0ecb1f1a3;pou_b74c09d7f1de9527;pou_45f4891d3ca2c92f;pou_82de3c6815c670fe;pou_e95928e49c5b9200;pou_ba414aff1c9937e4;pou_75e3a2045ed6ffc0;pou_53d2a587d7d2a18d;pou_214e6c1395d425ba;pou_684246c3a6e9c630;pou_3232e90a8dae0f9d;pou_59f3981f7595f1a7;pou_caa4c9c02a89d441;pou_a2ad5c0401fe9475;pou_fa9b8665e59839cd;pou_937e799a8d2bd71c;pou_9689e605c471b8c7;pou_8abad0777b064e34;pou_6e8321ee5faef8e2;pou_4274a19e33c569d1;pou_ac04fb9c058440ee;pou_6fb3386f405116b1;pou_59ff5f919fe20ddd;pou_7adfa2019ec69b5e;pou_775d098d9f415e20;pou_6866b92ce985bbc0;pou_5716c8a34e971e49;pou_ab48f16f536a332d;pou_d0bdd85cdf6835b0;pou_d6926dba99e1bd87;pou_10ddf40c498fd303;pou_ff0e70f11d031114;pou_70c5f2b8e3032fbe;pou_3e250290c63ee1ec;pou_3ef137b36e088ab0;pou_5ef0c84b7af7e11f;pou_3086efcb31a2d80c;pou_4506462d91a0e418;pou_98363a63f66a6fca;pou_82b05548394529f0;pou_04a84a27af94b361;pou_66d74cc26725a803;pou_9bd7ea26f9c834cc;pou_8f66d8544bc2d6e3;pou_66f053fd9382ec07;pou_0bef509dead88e54;pou_8f2975c32662a397;pou_5d3d72d547eb9f96;pou_eac9d0e8cc8f4370;pou_086d2458b6c9f9f8;pou_76d7be32fbf5b3b9;pou_9a06bdf1987d2da9;pou_e0750cc3762cb9f2;pou_e9958b77e20fa7f8;pou_9b3c216d203c1812;pou_ce36be22b25c381c;pou_5bd08b056cab3d91;pou_2dcee2e533a63b08;pou_a0a1ddae6a764e63;pou_376ee3258c8cad39;pou_e34ac8fc133c316e;pou_9151d109ccb4ff98;pou_932bdef46211ef6d;pou_6e10537c16642cd0;pou_05ef687e955b8b56;pou_085fcdfd8dec750f;pou_76776827e8735d97;pou_cc464eb82c013056;pou_b2d10122401d8de0;pou_e3f7be62e87b1658;pou_6a9cd481df8bb21c;pou_2816e4e9244fdaa1;pou_abf55a18f125bf9e;pou_cbde53bb72fade3e;pou_65973781a33a3a83;pou_f1ec847043160c87;pou_0081cdb3feed0a33;pou_fb3165e2dc6014f1;pou_b952df53485ee3a4;pou_17e063bc0ac3ae54;pou_4e7db1d155d8503f;pou_917933d14148169b;pou_c6542544ae306ebe;pou_34d72ddae51019b4;pou_ba8c18be3e1df863;pou_48783d199032343c;pou_bd68f22ee255d156;pou_269cee3cb99840e5;pou_847c37712ba69a9b;pou_1f92764d90024bfa;pou_b1827f6ed5262551;pou_4927080ae25a5caf;pou_133db9f225aad7ab;pou_f0370c28a35d3fb8;pou_54b78d64d580a9d6;pou_0f3001dcef1a681b;pou_c3b335d7eaf927cc;pou_9d0887f1fd219bb5;pou_33dc0ccbce4bdd78;pou_e274d003a78ceee0;pou_700deef2bb56c038;pou_124fcc59baa1c355;pou_64927a39d55d0cab;pou_ee87b418e0b14b1d;pou_629b6f80b5e55b9b;pou_8cdda553360bc79a;pou_adafcc70ee756fa7;pou_a9031cd93c54a1e8;pou_c7aeaaca08910eff;pou_1ad1931caeef0273;pou_d8cdd2c614f3873f;pou_1d3369da329bed75;pou_2359171013cc2be5;pou_f6999724e697ba50;pou_0fa1792375efd399;pou_ae71577b4c3fabbf;pou_015a8063c3f91f66;pou_aa84162c45d44957;pou_fb04a2ca39e3d631;pou_ad9092b2bc14863a;pou_cadeced1727c1bfb;pou_5d192ea837617554;pou_f769e68e71940d4c;pou_224aaa114fd2a044;pou_dd66429d6e302331;pou_6154777478020369;pou_7d979d7cbe5fd6a1;pou_e881ccdaf9d217f9;pou_81bffea8f56e7a36;pou_142de7af5c096709;pou_ce65c06a662c9d56;pou_351b9866bd8eb5d3;pou_073e0fcb685b4dbe;pou_e313ad598b47b325;pou_078fe4daf80a13e4;pou_b2d49fd883206aac</t>
+  </si>
+  <si>
+    <t>pou_775d302a749061c9;pou_b004321e64f52e3e;pou_aaee35b0e5788279</t>
+  </si>
+  <si>
+    <t>pou_22fb71db75aebeb7</t>
+  </si>
+  <si>
+    <t>pou_ae6b30222ce85167</t>
+  </si>
+  <si>
+    <t>pou_96d4d7571910e159</t>
+  </si>
+  <si>
+    <t>pou_504757ce58822e0d</t>
+  </si>
+  <si>
+    <t>pou_557d39aaa00577fc</t>
+  </si>
+  <si>
+    <t>pou_3f85292b584b4a58;pou_dc89309f1255d10a;pou_e8207eaaf7632e9a</t>
+  </si>
+  <si>
+    <t>pou_8b3b6cf43724bdd7</t>
+  </si>
+  <si>
+    <t>pou_1dbf02b688e5fd19</t>
+  </si>
+  <si>
+    <t>pou_0d5d71f2f7cb3c37</t>
+  </si>
+  <si>
+    <t>pou_ccf22daec0707423</t>
+  </si>
+  <si>
+    <t>pou_a93556316a9a06a4</t>
+  </si>
+  <si>
+    <t>pou_4f1494d0d62e90fc;pou_c5b8d1559c1fb84a;pou_5e8e293d29d2df0b;pou_91c3c4914fafbef8;pou_cb83e98466c5c116;pou_7e3b2a3edf84fa11;pou_39031f0026b5d700</t>
+  </si>
+  <si>
+    <t>pou_98ff4061c2088942</t>
+  </si>
+  <si>
+    <t>pou_5b4f3d5d90d21837</t>
+  </si>
+  <si>
+    <t>pou_50f5bc16488dfd72;pou_96ac8f2d71d3118b</t>
+  </si>
+  <si>
+    <t>pou_eb58ce4c94eaab9b</t>
+  </si>
+  <si>
+    <t>pou_a8dc86d57183e942</t>
+  </si>
+  <si>
+    <t>pou_41834508f6ffa919</t>
+  </si>
+  <si>
+    <t>pou_cbe8821a0e51610c</t>
+  </si>
+  <si>
+    <t>pou_63f923a4f9ca84b9</t>
+  </si>
+  <si>
+    <t>pou_a7a19a853f68f025;pou_50a8ea040dba70c8</t>
+  </si>
+  <si>
+    <t>pou_dcf34af8a861c605;pou_ea44126c8eb3a980</t>
+  </si>
+  <si>
+    <t>pou_53cd332e6d7ac65e;pou_a22089a434c9d1ea;pou_9cdab0867d457d56;pou_8af992378d8b4c5e;pou_b357bd1aa20e24ff;pou_8716d0c7d2736251;pou_25c041ec654089d6;pou_1950a23ed50d3561;pou_cc6b8ce559e50415;pou_550fccb2f0dd12b1;pou_ac9542c8d0b21c8f;pou_7b4a8f287a679ea3;pou_0974637ad3ec02f1;pou_dc39b687f03a29ff;pou_bc67e408fc8c5f94;pou_679c1f58fa697e47;pou_f540d45f5ff5363b;pou_1ee7a2ff8b576fda;pou_93180113906161ba;pou_3731239e087bb7c4;pou_d92e027f82e4eb29;pou_2006dab5327c5d34;pou_d05508349e42952d;pou_30684b7bbe9295c5;pou_908d9653f60ff439;pou_353de51b4ff42a5d;pou_d5915c3bf898835a</t>
+  </si>
+  <si>
+    <t>pou_36a366d6115b36d7</t>
+  </si>
+  <si>
+    <t>pou_554250e809082e9d</t>
+  </si>
+  <si>
+    <t>pou_e09ca7b4cce1b86f;pou_c3c0a1a09dfdc0bd;pou_b9cbf89bbf92ec2f;pou_097cf815d61a64bc;pou_d21a96733b68d272</t>
+  </si>
+  <si>
+    <t>pou_4acb0a3263cc206b;pou_f48f7677147074ab;pou_da78d3cec705c5b9;pou_68afb6577ed46421;pou_c542bead931c24fd;pou_02d11cd533264d78;pou_b71de6d4913afe12;pou_aee42eb4bc0bbf9a;pou_bd155a32f3efce50;pou_e719f03b51b58e0a;pou_a12a8fa87bb3ee43;pou_04a7f10038c59dbb;pou_ccd54dbeb2c43965;pou_e5beab0c8d7ef7d0;pou_689548ca9f6bbfa8;pou_1f5f4ec5e7c78c20;pou_02b1e1f786ccf75f;pou_8c4aae42dd9787cf;pou_01a54f848b463105;pou_a1275989e3c54beb;pou_64e6a0c778e945b7;pou_41cd4bae5d19d4ab;pou_a23d97652592b24c;pou_4b402ecfd93d9d79;pou_ca23f543917170dd;pou_1a676731550005f9;pou_7fb062115613c954;pou_ef2c9de60aa1c1ac;pou_19e26910caba211c</t>
+  </si>
+  <si>
+    <t>pou_38e139ba32bf774e;pou_a4faab7b60f51bd2;pou_14a3dbc31f25f7cc;pou_aec7ab23b9873bd2;pou_cfce5a748ae86052;pou_e0c965b5ab0df6c2;pou_3c787366b82c048d;pou_bf73f35c12b5b215</t>
+  </si>
+  <si>
+    <t>pou_73c49084f2aeffd5;pou_51bb84b45381fe7d</t>
+  </si>
+  <si>
+    <t>pou_114d8a1c111310c6</t>
+  </si>
+  <si>
+    <t>pou_086b9996d0e916da</t>
+  </si>
+  <si>
+    <t>pou_b691828f3d9f7522;pou_edbe463f63f4c204;pou_75e895d18f5a973c;pou_40c2a8f25a74370f;pou_5ed1570ba23e9186;pou_f41ea50936a7ed3b;pou_1168968bacbbfc1f;pou_e6b6faf85788a075;pou_f1de09459cadb5ab;pou_a937c91138d15a24;pou_60f362a05f58e883;pou_5222d99f4d7cff7c;pou_714e8c2f2fcd9efc;pou_ebe2de625c188253;pou_0ba37cb1fe555c36</t>
+  </si>
+  <si>
+    <t>pou_8acea383b73ef488;pou_ffa6703830d148d1;pou_89b83435c5026576;pou_142842db4b14af68;pou_69afb278c321b7bf;pou_5db03f7eaddbd1b7;pou_fe1b9f3b5faec0e0</t>
+  </si>
+  <si>
+    <t>pou_2bb1a044ef6b8eb0</t>
+  </si>
+  <si>
+    <t>pou_e41b7de27d853dad</t>
+  </si>
+  <si>
+    <t>pou_5d3e5183cec66d53</t>
+  </si>
+  <si>
+    <t>pou_b33fd99e04c3b5a4</t>
+  </si>
+  <si>
+    <t>pou_1dc236bdbe88e3d1</t>
+  </si>
+  <si>
+    <t>pou_aa6b6ef6918cee94</t>
+  </si>
+  <si>
+    <t>pou_95656709770b0cba</t>
+  </si>
+  <si>
+    <t>pou_a1ba7751491cfcd1</t>
+  </si>
+  <si>
+    <t>pou_c29a8d90f1561020</t>
+  </si>
+  <si>
+    <t>pou_f9f6c9c08ebec294;pou_c3f3391b22ff19ff;pou_dbfa69d48468d412;pou_33de5bf7cc35fafb;pou_9e728e42f56e9d04;pou_b67ca80eb9a6b3a7;pou_843bf7fb780c3425;pou_d0a4465cadefbc17;pou_f3281e0a82fd71b4;pou_076e605182730f1e;pou_79ac4d3062ef3cc1;pou_8cfd22ffc8a52097</t>
+  </si>
+  <si>
+    <t>pou_8936489dbf72de9e</t>
+  </si>
+  <si>
+    <t>pou_1d8245ab080550c9;pou_53fb635e1a7e84a1</t>
+  </si>
+  <si>
+    <t>pou_1130ad79268021dd;pou_a703873417c18f6b;pou_35bf2b23535c038c;pou_a375b9a312bd3231;pou_d568c3cca5f723a6;pou_40060c55b89940e6</t>
+  </si>
+  <si>
+    <t>pou_11319b2271525430;pou_b05b4efa19caa3c2;pou_546b9dd60442fbcd;pou_0c3a65326a066d93;pou_87cc80991cc1d03c;pou_576d2133f8b29b00;pou_cc5ff7efebddd878;pou_1c53ee015753df2e;pou_e81ddd8ff44eefce;pou_e2395db5c721df2f;pou_0e80123692b9f612;pou_103f5aad02a335d6;pou_6891b4a516be8c78;pou_f4fff114408512ad</t>
+  </si>
+  <si>
+    <t>pou_ca82bb3c0a54c5dd;pou_8cdf88c416c54088;pou_c61e055e163d124d;pou_a94f2e91098d0e46;pou_5647d4962e802111;pou_1a8e5b3c1a8c8e58;pou_d464e0f25c765300;pou_aab7a7808377165f;pou_8448ab96a34c8768;pou_5e36dad12a7754e3;pou_cc6c5e1dded310f0</t>
+  </si>
+  <si>
+    <t>pou_f1f5aefbbed8b58c</t>
+  </si>
+  <si>
+    <t>pou_9c0d3dcd19d13c9a</t>
+  </si>
+  <si>
+    <t>pou_92146925dd3e79e1;pou_98085e4dba2e9a29;pou_dfa709bae3f40742;pou_309dfa49e7bd5930;pou_3377cd408b09f8c0;pou_fbf6bb59b4709967;pou_4a675444d6bbc82e</t>
+  </si>
+  <si>
+    <t>pou_22e0f3f44424b77e;pou_4bc6feb56ef2cff2;pou_c4e3531933fe487e;pou_0346cafd0b74f94f;pou_7c0419c4b9189e14;pou_f6605298baa549fe;pou_83b7bfa650158f2c;pou_7f14d805ea58cf23;pou_e5918faeb1eb9ba0;pou_6d5ebb116b4673fe;pou_9921f74bc64b9b51;pou_8eb770832938a071;pou_9306022faa2e1508;pou_ee8b3ca6613451e1;pou_df47c0f7a7b7417b;pou_74d8bb4473275549;pou_01b44447c7642a00;pou_50794e17aba7a84c;pou_728218ba75382c6b</t>
+  </si>
+  <si>
+    <t>pou_5601274853e63968</t>
+  </si>
+  <si>
+    <t>pou_766b274cc7297cb7;pou_e411253b684bc1d1;pou_0b1deb49fbe59cf0;pou_2c89cbf53f01daaa;pou_7aba2b70204b24ae;pou_bcc0f6a7754f4ab8</t>
+  </si>
+  <si>
+    <t>pou_16f7a1af5780b112</t>
+  </si>
+  <si>
+    <t>pou_163257fcd58abf67;pou_e6def53b38143fdd;pou_daf1997e64a8e63a</t>
+  </si>
+  <si>
+    <t>pou_a57a325247ebb690</t>
+  </si>
+  <si>
+    <t>pou_7b3e9a6a5613d2cb;pou_a0841689b8c17b72;pou_0348874e3357ab45;pou_3c66f9252d2492e8;pou_d2621e0fd4b82fd4;pou_7b77e6df0859456b</t>
+  </si>
+  <si>
+    <t>pou_332a245dfe5c20b7</t>
+  </si>
+  <si>
+    <t>pou_fccb42642123396f</t>
+  </si>
+  <si>
+    <t>pou_38f13b5eb025bdb6</t>
+  </si>
+  <si>
+    <t>pou_8545ee5e56203622;pou_3f9dae485672cb6a;pou_c5dba4e37a0bce9b;pou_d54962533391bee6;pou_5a83aa1059b429e4;pou_25e06ee5ee5ce062;pou_7bfcfa2ebd1f8a0c;pou_8fc5b267e08278d5;pou_f09b7227b4a56c87;pou_e2d796590ea9e821;pou_3b044dd3c7147c7e;pou_d0223f8a9074c67a;pou_a72731299cdbe88c;pou_6df580646972d65b;pou_1cf6db51726da6a6;pou_24478a7d3ecd1936;pou_2f3a789e5145d1e6;pou_048caccaddeb8768;pou_d8b0c905246fe8bd;pou_9c1abe108126436b;pou_a1f484f205a1b9f4</t>
+  </si>
+  <si>
+    <t>pou_6cf3ee6420d55a3f</t>
+  </si>
+  <si>
+    <t>pou_e894fde37f0fb6ff</t>
+  </si>
+  <si>
+    <t>pou_0fdd29ccf16b5872</t>
+  </si>
+  <si>
+    <t>pou_59764f5c99b6a1ad;pou_5a59aa811d1c0247;pou_dcc61de9d26d9421;pou_8283c4327a286a21;pou_c9a5b0fef2a09f62;pou_5f4e0cd45b336808;pou_4979f0cfb9d3780a;pou_0ee95d2b3a08e8b5;pou_e27fc26380ae6af4;pou_26380acf8c318832;pou_e0e48bcbbf16ee50;pou_5725d40ea8759d90;pou_efe407f4faf88c5d;pou_ee92964d2bad7b30;pou_69839da6a1de25e5</t>
+  </si>
+  <si>
+    <t>pou_0667ef1133350437</t>
+  </si>
+  <si>
+    <t>pou_d4e0a252a29cb7f5</t>
+  </si>
+  <si>
+    <t>pou_58ff37926bade032</t>
+  </si>
+  <si>
+    <t>pou_4334161bc80c6c7b</t>
+  </si>
+  <si>
+    <t>pou_2e6788498a1368b1</t>
+  </si>
+  <si>
+    <t>pou_5bb12222baf6a6d5</t>
+  </si>
+  <si>
+    <t>pou_b87795e1fca98048</t>
+  </si>
+  <si>
+    <t>pou_ceced6d4cca2166e</t>
+  </si>
+  <si>
+    <t>pou_1832ebeff3b6ba82</t>
+  </si>
+  <si>
+    <t>pou_14912e3f255bcd9c</t>
+  </si>
+  <si>
+    <t>pou_e5b0eac12d80fc36</t>
+  </si>
+  <si>
+    <t>pou_722c14d37c4e0ba7;pou_2cc4e73db9a948c3</t>
+  </si>
+  <si>
+    <t>pou_015f3c4cc6b7017d</t>
+  </si>
+  <si>
+    <t>pou_49f227073ccb0a65</t>
+  </si>
+  <si>
+    <t>pou_f03455693ae71ef2</t>
+  </si>
+  <si>
+    <t>pou_96fa62e61d848be8</t>
+  </si>
+  <si>
+    <t>pou_2e38d64c0e33cd74</t>
+  </si>
+  <si>
+    <t>pou_ddac54d31860b7b2</t>
+  </si>
+  <si>
+    <t>pou_522ec409ee37bc27</t>
+  </si>
+  <si>
+    <t>pou_feb0fb8ed225c742</t>
+  </si>
+  <si>
+    <t>pou_6febdc6be7c957bc</t>
+  </si>
+  <si>
+    <t>pou_e9d2500baffe12fc</t>
+  </si>
+  <si>
+    <t>pou_3e39e890dc6b2de4</t>
+  </si>
+  <si>
+    <t>pou_61203250446a1fe0</t>
+  </si>
+  <si>
+    <t>pou_e2aa9ba03a5c8cf1</t>
+  </si>
+  <si>
+    <t>pou_0dfaeeb5d8fa5aa7</t>
+  </si>
+  <si>
+    <t>pou_e0079c9479983b03</t>
+  </si>
+  <si>
+    <t>pou_3a1a83e49d9c7beb</t>
+  </si>
+  <si>
+    <t>pou_4c40f928b75608f6</t>
+  </si>
+  <si>
+    <t>pou_d7768e04c4bc8dc8</t>
+  </si>
+  <si>
+    <t>pou_3d7bc0ff32ee1bb0</t>
+  </si>
+  <si>
+    <t>pou_850e423d82deefe6</t>
+  </si>
+  <si>
+    <t>pou_9d5be082acf7bb0d</t>
+  </si>
+  <si>
+    <t>pou_279dd8bd2b0b0b9c</t>
+  </si>
+  <si>
+    <t>pou_ffcbfd160e51e98e</t>
+  </si>
+  <si>
+    <t>pou_cf18352b6d0797a2</t>
+  </si>
+  <si>
+    <t>pou_8f6cb0c83c56929f</t>
+  </si>
+  <si>
+    <t>pou_48b07b8b1b91d479</t>
+  </si>
+  <si>
+    <t>pou_e30ba1d4414e5412</t>
+  </si>
+  <si>
+    <t>pou_46e511448892ae47</t>
+  </si>
+  <si>
+    <t>pou_192186da159d1cbe</t>
+  </si>
+  <si>
+    <t>pou_1b8c5266d8f60e79</t>
+  </si>
+  <si>
+    <t>pou_648a39c26f22df59</t>
+  </si>
+  <si>
+    <t>pou_2ba0d7dbc18ba9d8</t>
+  </si>
+  <si>
+    <t>pou_f03ff23929bf56d9</t>
+  </si>
+  <si>
+    <t>pou_93d195a7d9ce0dbb</t>
+  </si>
+  <si>
+    <t>pou_1e663637e481f47f</t>
+  </si>
+  <si>
+    <t>pou_e6827f414eb31acb</t>
+  </si>
+  <si>
+    <t>pou_4fca5bdb4b0d7cfe</t>
+  </si>
+  <si>
+    <t>pou_ec06f8594261c69c</t>
+  </si>
+  <si>
+    <t>pou_5d4111a5d5563c89</t>
+  </si>
+  <si>
+    <t>pou_1ee09d4ec2a021dd</t>
+  </si>
+  <si>
+    <t>pou_cfc7857880618340</t>
+  </si>
+  <si>
+    <t>pou_20f8527eb8ae0773</t>
+  </si>
+  <si>
+    <t>pou_ee4df8e92b1c20b1</t>
+  </si>
+  <si>
+    <t>pou_96cbdef874333b5d</t>
+  </si>
+  <si>
+    <t>pou_542f8efed28e2a70</t>
+  </si>
+  <si>
+    <t>pou_3de15a5ececdf2fb</t>
+  </si>
+  <si>
+    <t>pou_8ce5c6cf60d64b76</t>
+  </si>
+  <si>
+    <t>pou_0e219cd9faef548e</t>
+  </si>
+  <si>
+    <t>pou_c1256a1c0b131495</t>
+  </si>
+  <si>
+    <t>pou_3d8898b1f18619f5</t>
+  </si>
+  <si>
+    <t>pou_6745befdd3b5b7bd</t>
+  </si>
+  <si>
+    <t>pou_8d6ae61fab28cb44</t>
+  </si>
+  <si>
+    <t>pou_693c57e900e1c564</t>
+  </si>
+  <si>
+    <t>pou_8cf0c77f62dc2619</t>
+  </si>
+  <si>
+    <t>pou_c574b094df4490f0</t>
+  </si>
+  <si>
+    <t>pou_4912dfc55974f036</t>
+  </si>
+  <si>
+    <t>pou_090d9976a2debff0</t>
+  </si>
+  <si>
+    <t>pou_ba3527798e450fa7</t>
+  </si>
+  <si>
+    <t>pou_8186d04aeaba8902</t>
+  </si>
+  <si>
+    <t>pou_bdbbbd56b0cc4778</t>
+  </si>
+  <si>
+    <t>pou_2d1baf1e81b81bae</t>
+  </si>
+  <si>
+    <t>pou_c68ba5fab7a61cfe</t>
+  </si>
+  <si>
+    <t>pou_ec2d89053a657eb3</t>
+  </si>
+  <si>
+    <t>pou_1f2d126eb1561aec</t>
+  </si>
+  <si>
+    <t>pou_a12ee4853073d17e</t>
+  </si>
+  <si>
+    <t>pou_e8c45f61b6614154</t>
+  </si>
+  <si>
+    <t>pou_20610802d63f173f</t>
+  </si>
+  <si>
+    <t>pou_0a98b730dee381a8</t>
+  </si>
+  <si>
+    <t>pou_a7405cea92f4721e</t>
+  </si>
+  <si>
+    <t>pou_adc6c9948c91b120</t>
+  </si>
+  <si>
+    <t>pou_bc1594a95a97c863</t>
+  </si>
+  <si>
+    <t>pou_1d220a67bc78dfc1</t>
+  </si>
+  <si>
+    <t>pou_355931b3d968e8e9</t>
+  </si>
+  <si>
+    <t>pou_374206575dcdfc30</t>
+  </si>
+  <si>
+    <t>pou_69068ce4bb842e8d</t>
+  </si>
+  <si>
+    <t>pou_a48007d55e896f7e</t>
+  </si>
+  <si>
+    <t>pou_b7c283ad83bb81d6</t>
+  </si>
+  <si>
+    <t>pou_1c23bba13ddf3061</t>
+  </si>
+  <si>
+    <t>pou_3ead452b5f8dde61</t>
+  </si>
+  <si>
+    <t>pou_b6add156266b67f6</t>
+  </si>
+  <si>
+    <t>pou_ee7d875cb9101deb</t>
+  </si>
+  <si>
+    <t>pou_d90d611b5542c253</t>
+  </si>
+  <si>
+    <t>pou_6b5d63b88ed62fe1</t>
+  </si>
+  <si>
+    <t>pou_f31fa8287dd7c929</t>
+  </si>
+  <si>
+    <t>pou_3ad89659213bd8cc</t>
+  </si>
+  <si>
+    <t>pou_e8eb54b802d85183</t>
+  </si>
+  <si>
+    <t>pou_146785c62b791d46</t>
+  </si>
+  <si>
+    <t>pou_48cc759545274597</t>
+  </si>
+  <si>
+    <t>pou_f6dc040ed432ac1e</t>
+  </si>
+  <si>
+    <t>pou_585cad8bfe7041a5</t>
+  </si>
+  <si>
+    <t>pou_6e43d1456fbe8986</t>
+  </si>
+  <si>
+    <t>pou_a0c7e77bfbbd6bb5</t>
+  </si>
+  <si>
+    <t>pou_6c80fd2d87fff3fc</t>
+  </si>
+  <si>
+    <t>pou_2cac25633833e4e9</t>
+  </si>
+  <si>
+    <t>pou_4f022d08751f6f54</t>
+  </si>
+  <si>
+    <t>pou_f3e44d2faa22fe0d</t>
+  </si>
+  <si>
+    <t>pou_c8c8f3d63857abe2</t>
+  </si>
+  <si>
+    <t>pou_c1c6639de29d0016</t>
+  </si>
+  <si>
+    <t>pou_22cee5690047badf</t>
+  </si>
+  <si>
+    <t>pou_e105151c5119ca5a</t>
+  </si>
+  <si>
+    <t>pou_c00e9dd00bfcbdf4</t>
+  </si>
+  <si>
+    <t>pou_85037000e59be04b</t>
+  </si>
+  <si>
+    <t>pou_c616dd19d3b704d9</t>
+  </si>
+  <si>
+    <t>pou_a5a4df4af8e8267f</t>
+  </si>
+  <si>
+    <t>pou_f37b2c2fe0ef0c9d</t>
+  </si>
+  <si>
+    <t>pou_ffa4b6e53b51d7c4</t>
+  </si>
+  <si>
+    <t>pou_42ad7f09cd8b9082</t>
+  </si>
+  <si>
+    <t>pou_8efcdcf775e74b30</t>
+  </si>
+  <si>
+    <t>pou_b197aabc5f5416d2</t>
+  </si>
+  <si>
+    <t>pou_78419e16f4059cf4</t>
+  </si>
+  <si>
+    <t>pou_07e70944c88b5cf3</t>
+  </si>
+  <si>
+    <t>pou_10d252b7476cedc5</t>
+  </si>
+  <si>
+    <t>pou_cf8e6ba678b20c73</t>
+  </si>
+  <si>
+    <t>pou_60f5c37c17a18461</t>
+  </si>
+  <si>
+    <t>pou_0903d7534cb777d0</t>
+  </si>
+  <si>
+    <t>pou_0a7672937126ad1a</t>
+  </si>
+  <si>
+    <t>pou_805286dc10047ff4</t>
+  </si>
+  <si>
+    <t>pou_ee391c3b4edcdcf5</t>
+  </si>
+  <si>
+    <t>pou_5084330796afc3b3</t>
+  </si>
+  <si>
+    <t>pou_f037a9d7126e9169</t>
+  </si>
+  <si>
+    <t>pou_d89525723782fc8f</t>
+  </si>
+  <si>
+    <t>pou_c41955914d77db67</t>
+  </si>
+  <si>
+    <t>pou_f43448198ce22971</t>
+  </si>
+  <si>
+    <t>pou_e363069fbe3f19da</t>
+  </si>
+  <si>
+    <t>pou_db138486c082a84a</t>
+  </si>
+  <si>
+    <t>pou_cebd7c90924202af</t>
+  </si>
+  <si>
+    <t>pou_8e6bbc5ffa525013</t>
+  </si>
+  <si>
+    <t>pou_bed9f805edd7f5de</t>
+  </si>
+  <si>
+    <t>pou_3b9178af6b4c2c53</t>
+  </si>
+  <si>
+    <t>pou_694e4f4d08e1a079</t>
+  </si>
+  <si>
+    <t>pou_3b46699fdc076f78</t>
+  </si>
+  <si>
+    <t>pou_c199adefdb4d408e</t>
+  </si>
+  <si>
+    <t>pou_ff4fd192bca50865</t>
+  </si>
+  <si>
+    <t>pou_2c841b451d9035f5</t>
+  </si>
+  <si>
+    <t>pou_f2fcec99016a389b</t>
+  </si>
+  <si>
+    <t>pou_8576c0aaedb2673a</t>
+  </si>
+  <si>
+    <t>pou_c2ac38601d74220e</t>
+  </si>
+  <si>
+    <t>pou_88be1be590a4d7fc</t>
+  </si>
+  <si>
+    <t>pou_768545bdcbdfcbc9</t>
+  </si>
+  <si>
+    <t>pou_d491d834814db5f0</t>
+  </si>
+  <si>
+    <t>pou_0629c50259a32203</t>
+  </si>
+  <si>
+    <t>pou_78a954d2ac6deff7</t>
+  </si>
+  <si>
+    <t>pou_500f17753265b608</t>
+  </si>
+  <si>
+    <t>pou_264682cd468973de</t>
+  </si>
+  <si>
+    <t>pou_d4e17acdebb6135c</t>
+  </si>
+  <si>
+    <t>pou_1e1a0f4b5b026919</t>
+  </si>
+  <si>
+    <t>pou_15fad7326626ab59</t>
+  </si>
+  <si>
+    <t>pou_0acb543e296c07f5</t>
+  </si>
+  <si>
+    <t>pou_99bdb91d69b369a0</t>
+  </si>
+  <si>
+    <t>pou_d56dc4a8e936015d</t>
+  </si>
+  <si>
+    <t>pou_a2ee4f98d3dfb309</t>
+  </si>
+  <si>
+    <t>pou_1761a787c95e3a2b</t>
+  </si>
+  <si>
+    <t>pou_a82d50e9889d3de7</t>
+  </si>
+  <si>
+    <t>pou_74e045fe392b3405</t>
+  </si>
+  <si>
+    <t>pou_630702cd7b8f2473</t>
+  </si>
+  <si>
+    <t>pou_2ffff143772f7a3a</t>
+  </si>
+  <si>
+    <t>pou_aa889f560b665a54</t>
+  </si>
+  <si>
+    <t>pou_f217bebe4e9f3261</t>
+  </si>
+  <si>
+    <t>pou_cbd794b22ee77c98</t>
+  </si>
+  <si>
+    <t>pou_812b75ad6850c8c8</t>
+  </si>
+  <si>
+    <t>pou_6cb756844bd023c1</t>
+  </si>
+  <si>
+    <t>pou_88991fb43fd56a2b</t>
+  </si>
+  <si>
+    <t>pou_9b2d187a4b547c6c</t>
+  </si>
+  <si>
+    <t>pou_5562cb96928f02ee</t>
+  </si>
+  <si>
+    <t>pou_00c1465153e429d0</t>
+  </si>
+  <si>
+    <t>pou_273950215b4d5bf3</t>
+  </si>
+  <si>
+    <t>pou_208aa168e247e6b5</t>
+  </si>
+  <si>
+    <t>pou_77bc738300cfe217</t>
+  </si>
+  <si>
+    <t>pou_01b08962c7da4f8d</t>
+  </si>
+  <si>
+    <t>pou_0ae50b03b0bb004d</t>
+  </si>
+  <si>
+    <t>pou_9aa1b8590f5a5187</t>
+  </si>
+  <si>
+    <t>pou_d0d9e131ff49316d</t>
+  </si>
+  <si>
+    <t>pou_2c14f43081b5d92a</t>
+  </si>
+  <si>
+    <t>pou_859c267b10484906</t>
+  </si>
+  <si>
+    <t>pou_a345fef1b8740442</t>
+  </si>
+  <si>
+    <t>pou_ce2178729f1235f8</t>
+  </si>
+  <si>
+    <t>pou_929c9ddee5571dfc</t>
+  </si>
+  <si>
+    <t>pou_d703377aa08dc041</t>
+  </si>
+  <si>
+    <t>pou_f20c43a5ba2abb1e</t>
+  </si>
+  <si>
+    <t>pou_959834bff9edeb76</t>
+  </si>
+  <si>
+    <t>pou_acf1f96e56e5e977</t>
+  </si>
+  <si>
+    <t>pou_537620b345c0bc96</t>
+  </si>
+  <si>
+    <t>pou_cf37b8fea0eb75c3</t>
+  </si>
+  <si>
+    <t>pou_b3934f396ff9b001</t>
+  </si>
+  <si>
+    <t>pou_a8dfa0b08d397ed8</t>
+  </si>
+  <si>
+    <t>pou_128e70ab42da249f</t>
+  </si>
+  <si>
+    <t>pou_323297fa10830a4b</t>
+  </si>
+  <si>
+    <t>pou_8465081f22bfb730</t>
+  </si>
+  <si>
+    <t>pou_25402826df32225b</t>
+  </si>
+  <si>
+    <t>pou_81447ac55d128b34</t>
+  </si>
+  <si>
+    <t>pou_63bc9235b6d214b8</t>
+  </si>
+  <si>
+    <t>pou_78343638b2d58337</t>
+  </si>
+  <si>
+    <t>pou_d590203873f52732</t>
+  </si>
+  <si>
+    <t>pou_902c2cbff5717c3e</t>
+  </si>
+  <si>
+    <t>pou_98ade39bb8b6e01f</t>
+  </si>
+  <si>
+    <t>pou_cfe13ff843a20d89</t>
+  </si>
+  <si>
+    <t>pou_d9aa00b9a0f9eb1a</t>
+  </si>
+  <si>
+    <t>pou_09c778454e0a3fca</t>
+  </si>
+  <si>
+    <t>pou_68fa91bb7b662c0b</t>
+  </si>
+  <si>
+    <t>pou_d9fe06d7203bf6b4</t>
+  </si>
+  <si>
+    <t>pou_e796f3fdea7db1fd</t>
+  </si>
+  <si>
+    <t>pou_0612f8409a8ef503</t>
+  </si>
+  <si>
+    <t>pou_6af0bd95dad6d51c</t>
+  </si>
+  <si>
+    <t>pou_6b19b86b93cd4df1</t>
+  </si>
+  <si>
+    <t>pou_a14e93e9362f0b76</t>
+  </si>
+  <si>
+    <t>pou_6be92f0c150a6ff9</t>
+  </si>
+  <si>
+    <t>pou_1d0b1f0d2ca62d08</t>
+  </si>
+  <si>
+    <t>pou_1106c53f5ffc20b6</t>
+  </si>
+  <si>
+    <t>pou_728d84a4127d3713</t>
+  </si>
+  <si>
+    <t>pou_e1a94f2f58ddc4a7</t>
+  </si>
+  <si>
+    <t>pou_16f51133b255579a</t>
+  </si>
+  <si>
+    <t>pou_9d6499506db400e2</t>
+  </si>
+  <si>
+    <t>pou_38efe72718f21fc6</t>
+  </si>
+  <si>
+    <t>pou_6c9cd354bf0a7d31</t>
+  </si>
+  <si>
+    <t>pou_fb678783b63a652d;pou_fca71b7c3b6ff832</t>
+  </si>
+  <si>
+    <t>pou_e780fa1c5a7ec305;pou_a6877c0f29791234;pou_0fee52440d658b26;pou_2a392e1e292641ac;pou_bb67b0db7491b505;pou_bdda089242efc6e6;pou_a3e391fb6bbe6b7e;pou_c8e59dbf6a2a54f3;pou_ca06763aee27fba7;pou_85808623edb52699;pou_25adbf6f6ad757b7;pou_7f52839301369625</t>
+  </si>
+  <si>
+    <t>pou_f833f8ea00e41902</t>
+  </si>
+  <si>
+    <t>pou_aa2a99f6ace62d77</t>
+  </si>
+  <si>
+    <t>pou_dad28fd4cc11f155</t>
+  </si>
+  <si>
+    <t>pou_39711686e8d22939</t>
+  </si>
+  <si>
+    <t>pou_3544be4a13bc39e1</t>
+  </si>
+  <si>
+    <t>pou_9a6bf4cff77440d8</t>
+  </si>
+  <si>
+    <t>pou_02745f9b77f44679</t>
+  </si>
+  <si>
+    <t>pou_e87c108b0e82b264</t>
+  </si>
+  <si>
+    <t>pou_ff876fdcbcd6c706</t>
+  </si>
+  <si>
+    <t>pou_68c73413374c315e</t>
+  </si>
+  <si>
+    <t>pou_c2da4b2f65d29f18</t>
+  </si>
+  <si>
+    <t>pou_f1cbd627f0439840</t>
+  </si>
+  <si>
+    <t>pou_cf20a011f5031993</t>
+  </si>
+  <si>
+    <t>pou_afbb513a91725815</t>
+  </si>
+  <si>
+    <t>pou_be1620316618dcff</t>
+  </si>
+  <si>
+    <t>pou_9669b2e1ec0dc069</t>
+  </si>
+  <si>
+    <t>pou_bc47812cabb44769</t>
+  </si>
+  <si>
+    <t>pou_03d623a61ce92034</t>
+  </si>
+  <si>
+    <t>pou_017e36fc82571abb</t>
+  </si>
+  <si>
+    <t>pou_9bc4407abbbc02c0</t>
+  </si>
+  <si>
+    <t>pou_cfe1eeca1876f5df</t>
+  </si>
+  <si>
+    <t>pou_579d3ecd465ac451</t>
+  </si>
+  <si>
+    <t>pou_b26c72d7bd602573</t>
+  </si>
+  <si>
+    <t>pou_9e68a7ddc7b9890f</t>
+  </si>
+  <si>
+    <t>pou_b7107c1f15a619bc</t>
+  </si>
+  <si>
+    <t>pou_1a83df1e5117ba3b</t>
+  </si>
+  <si>
+    <t>pou_4d796c446b5d85eb</t>
+  </si>
+  <si>
+    <t>pou_d832efc195913057</t>
+  </si>
+  <si>
+    <t>pou_59f525e658ecc0fc</t>
+  </si>
+  <si>
+    <t>pou_30009d7235da1c7d</t>
+  </si>
+  <si>
+    <t>pou_22b3a1b3928f4804</t>
+  </si>
+  <si>
+    <t>pou_1e76ccf8fe0f12b3</t>
+  </si>
+  <si>
+    <t>pou_aaa2c86844246c31</t>
+  </si>
+  <si>
+    <t>pou_36d5acf96141464b</t>
+  </si>
+  <si>
+    <t>pou_61e898bb74410ba3</t>
+  </si>
+  <si>
+    <t>pou_26708e3087d65119</t>
+  </si>
+  <si>
+    <t>pou_fcd67948080425b3</t>
+  </si>
+  <si>
+    <t>pou_d2f4b31a4ecee196</t>
+  </si>
+  <si>
+    <t>pou_19e2e449f38b08f3</t>
+  </si>
+  <si>
+    <t>pou_37adc1184526171e</t>
+  </si>
+  <si>
+    <t>pou_53d24d9873ac27e5</t>
+  </si>
+  <si>
+    <t>pou_cde5ebbc60fb4fb5</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
adding person of second part, column correction
</commit_message>
<xml_diff>
--- a/04_output_data/folder.xlsx
+++ b/04_output_data/folder.xlsx
@@ -4237,1930 +4237,1930 @@
     <t>FTG 1060</t>
   </si>
   <si>
-    <t>pou_a0de395be55a19ea</t>
-  </si>
-  <si>
-    <t>pou_6c421a0ed69d1976</t>
-  </si>
-  <si>
-    <t>pou_f25fa8a988c46a29;pou_4723a3f30502a8df</t>
-  </si>
-  <si>
-    <t>pou_8cca590c6e0c99d9</t>
-  </si>
-  <si>
-    <t>pou_5fea98217ab8dce3</t>
-  </si>
-  <si>
-    <t>pou_bdc2fe8932890cdc</t>
-  </si>
-  <si>
-    <t>pou_f6cae3876ebd44a9</t>
-  </si>
-  <si>
-    <t>pou_af6cbef75cad0d63</t>
-  </si>
-  <si>
-    <t>pou_c871a40b8639c5fc</t>
-  </si>
-  <si>
-    <t>pou_5687a3b95d450ff2</t>
-  </si>
-  <si>
-    <t>pou_290435b0ed972857</t>
-  </si>
-  <si>
-    <t>pou_218dade6de0b2eaf</t>
-  </si>
-  <si>
-    <t>pou_39ff8419342911e5</t>
-  </si>
-  <si>
-    <t>pou_bdcf0157ce80e171</t>
-  </si>
-  <si>
-    <t>pou_43f563910550ff2b;pou_54b549647bb7a8fd</t>
-  </si>
-  <si>
-    <t>pou_90277f1cf3dda883</t>
-  </si>
-  <si>
-    <t>pou_4ae885809038c538</t>
-  </si>
-  <si>
-    <t>pou_8a83f000fbc6a64f;pou_0f8df06a833ad6de</t>
-  </si>
-  <si>
-    <t>pou_55a2dda64f33f058</t>
-  </si>
-  <si>
-    <t>pou_93dece6f5fd5633f</t>
-  </si>
-  <si>
-    <t>pou_74bda9eb44e8ee5c</t>
-  </si>
-  <si>
-    <t>pou_3398f485532a4e26</t>
-  </si>
-  <si>
-    <t>pou_dc67ece58771119f;pou_83e8e09b2dbfa71b</t>
-  </si>
-  <si>
-    <t>pou_feb62e15905e4a90;pou_18f1a47667f07673</t>
-  </si>
-  <si>
-    <t>pou_ec03c25d6f619ff8</t>
-  </si>
-  <si>
-    <t>pou_29b6de189c57b2e8</t>
-  </si>
-  <si>
-    <t>pou_8a60908356d6e15e</t>
-  </si>
-  <si>
-    <t>pou_f61c25a558fa62ac;pou_089bd11eabebf4ec;pou_74add39bf6526f24;pou_19dfe2950b3c6902;pou_e701a0bbc961474c;pou_f099f8b712fdade1;pou_695216f944ba8461;pou_487ca2d280e0bcb1;pou_6a86ccf3c5041d28</t>
-  </si>
-  <si>
-    <t>pou_fb8ffb19bb48ccfa</t>
-  </si>
-  <si>
-    <t>pou_8866b9c1ac9827fa</t>
-  </si>
-  <si>
-    <t>pou_888afe0da1424913</t>
-  </si>
-  <si>
-    <t>pou_c1db532ee6ee588e</t>
-  </si>
-  <si>
-    <t>pou_6d1998537307ff40</t>
-  </si>
-  <si>
-    <t>pou_8c18fd6303ea4a21</t>
-  </si>
-  <si>
-    <t>pou_064321eac799ead8;pou_0dd37db185081537</t>
-  </si>
-  <si>
-    <t>pou_f43398e9e4afd747</t>
-  </si>
-  <si>
-    <t>pou_67e061c53472e6d4</t>
-  </si>
-  <si>
-    <t>pou_f81a3edf3e7e536a</t>
-  </si>
-  <si>
-    <t>pou_759b13b0478a0085;pou_b7d65a417fec51b2</t>
-  </si>
-  <si>
-    <t>pou_03d6b425f15e4156</t>
-  </si>
-  <si>
-    <t>pou_3e6e8feca10bb36e</t>
-  </si>
-  <si>
-    <t>pou_8b7ec46ba9f3a94e</t>
-  </si>
-  <si>
-    <t>pou_9b36904edfd032ac</t>
-  </si>
-  <si>
-    <t>pou_3c66f7dc027d1e54</t>
-  </si>
-  <si>
-    <t>pou_6ed278260e0dfc8f</t>
-  </si>
-  <si>
-    <t>pou_feffb27f778f1a9e;pou_ae65638aedbae664</t>
-  </si>
-  <si>
-    <t>pou_4a85a42480157f89</t>
-  </si>
-  <si>
-    <t>pou_124b9c02065dc792</t>
-  </si>
-  <si>
-    <t>pou_dce820bcecf88c93</t>
-  </si>
-  <si>
-    <t>pou_72698531f6cf1a86</t>
-  </si>
-  <si>
-    <t>pou_c16c7155794f1364</t>
-  </si>
-  <si>
-    <t>pou_4bd996635e087e0a</t>
-  </si>
-  <si>
-    <t>pou_2d6fd9568a658810</t>
-  </si>
-  <si>
-    <t>pou_523611c3793b3ac7</t>
-  </si>
-  <si>
-    <t>pou_38e8b0f18ff1d38b</t>
-  </si>
-  <si>
-    <t>pou_98b9b8a934b45d86</t>
-  </si>
-  <si>
-    <t>pou_746144d4d231bf6b</t>
-  </si>
-  <si>
-    <t>pou_c7412eb27a0d94d0</t>
-  </si>
-  <si>
-    <t>pou_dad80555e7a6bb50</t>
-  </si>
-  <si>
-    <t>pou_ef45384a432d7756</t>
-  </si>
-  <si>
-    <t>pou_19a85d3742f6b5b5</t>
-  </si>
-  <si>
-    <t>pou_a181250ac974634d</t>
-  </si>
-  <si>
-    <t>pou_fe85fdf7225cadc1</t>
-  </si>
-  <si>
-    <t>pou_9066b6e1e159d070</t>
-  </si>
-  <si>
-    <t>pou_b14c4f1ea6390ffe</t>
-  </si>
-  <si>
-    <t>pou_815bc12240fe5177</t>
-  </si>
-  <si>
-    <t>pou_8e3587ac10ed2400</t>
-  </si>
-  <si>
-    <t>pou_749dfc782f76dc73</t>
-  </si>
-  <si>
-    <t>pou_79bdb2c280e14a3a</t>
-  </si>
-  <si>
-    <t>pou_5417b7e60298adde</t>
-  </si>
-  <si>
-    <t>pou_da964dd4c2b55f39</t>
-  </si>
-  <si>
-    <t>pou_295c079cae58d5e0</t>
-  </si>
-  <si>
-    <t>pou_4e9889d06fa5f7bc</t>
-  </si>
-  <si>
-    <t>pou_ec0b909f6fcc23a6</t>
-  </si>
-  <si>
-    <t>pou_f7e303e2db8b4f0a</t>
-  </si>
-  <si>
-    <t>pou_7a03aad568e1813c</t>
-  </si>
-  <si>
-    <t>pou_d4eb85b8a32f5c68</t>
-  </si>
-  <si>
-    <t>pou_57de753a716680e5</t>
-  </si>
-  <si>
-    <t>pou_707545913ad9865e</t>
-  </si>
-  <si>
-    <t>pou_df8509d1d8cb1de1</t>
-  </si>
-  <si>
-    <t>pou_8e0a286075e057c1</t>
-  </si>
-  <si>
-    <t>pou_ed3c8b45b69dd902</t>
-  </si>
-  <si>
-    <t>pou_c59eb8a6e1745b1a</t>
-  </si>
-  <si>
-    <t>pou_350f503cd2842517</t>
-  </si>
-  <si>
-    <t>pou_d63bb44de2fe9410</t>
-  </si>
-  <si>
-    <t>pou_cca727d4769aef75</t>
-  </si>
-  <si>
-    <t>pou_6d790657db42d09c</t>
-  </si>
-  <si>
-    <t>pou_d0271fc7e7c452cf</t>
-  </si>
-  <si>
-    <t>pou_d8790e5cf73ce68a</t>
-  </si>
-  <si>
-    <t>pou_96aac952e53087b5</t>
-  </si>
-  <si>
-    <t>pou_c5af69a3c24c95e7</t>
-  </si>
-  <si>
-    <t>pou_4fd3220c705a1cee</t>
-  </si>
-  <si>
-    <t>pou_35e8c065b784e8e4</t>
-  </si>
-  <si>
-    <t>pou_def44c98d91b06c5</t>
-  </si>
-  <si>
-    <t>pou_959a5a566f8c53af</t>
-  </si>
-  <si>
-    <t>pou_c8bff6e87f7f2da2</t>
-  </si>
-  <si>
-    <t>pou_25333733f1adf839</t>
-  </si>
-  <si>
-    <t>pou_ccf4466872289231</t>
-  </si>
-  <si>
-    <t>pou_8ba66a80076d05ee</t>
-  </si>
-  <si>
-    <t>pou_4d7297b0de905526</t>
-  </si>
-  <si>
-    <t>pou_5c69e6429ac4dbbd</t>
-  </si>
-  <si>
-    <t>pou_356abeb70605a1b3</t>
-  </si>
-  <si>
-    <t>pou_645ce65e625289d4</t>
-  </si>
-  <si>
-    <t>pou_370884f02694aef6</t>
-  </si>
-  <si>
-    <t>pou_0c0fde309dc5e659</t>
-  </si>
-  <si>
-    <t>pou_f5315a5f47842b34</t>
-  </si>
-  <si>
-    <t>pou_3ee6595358bb4cb7</t>
-  </si>
-  <si>
-    <t>pou_9909c1f3d422a6d9</t>
-  </si>
-  <si>
-    <t>pou_4c8ed47b07abb37f</t>
-  </si>
-  <si>
-    <t>pou_5b001b6b45d3aa04</t>
-  </si>
-  <si>
-    <t>pou_f993f2016e5fb4bf</t>
-  </si>
-  <si>
-    <t>pou_4496720de6c97c61</t>
-  </si>
-  <si>
-    <t>pou_d6fc600f6ac72fc6</t>
-  </si>
-  <si>
-    <t>pou_aaa7a2a708cda7f0</t>
-  </si>
-  <si>
-    <t>pou_af50c5dbcbf129b0</t>
-  </si>
-  <si>
-    <t>pou_e690d7eb88a841d6</t>
-  </si>
-  <si>
-    <t>pou_531e0b880f3cb8d6</t>
-  </si>
-  <si>
-    <t>pou_68a3817785dd8771</t>
-  </si>
-  <si>
-    <t>pou_287c8aae3099cc35</t>
-  </si>
-  <si>
-    <t>pou_68eab1416cad1624</t>
-  </si>
-  <si>
-    <t>pou_a521470df395b704</t>
-  </si>
-  <si>
-    <t>pou_bd60e13d696d2c5e</t>
-  </si>
-  <si>
-    <t>pou_331a643a63a984b9</t>
-  </si>
-  <si>
-    <t>pou_14bff995a44640ab</t>
-  </si>
-  <si>
-    <t>pou_d5b925c17bb41980</t>
-  </si>
-  <si>
-    <t>pou_6e9bce644e971c37;pou_a58155c77b57ba45;pou_44abd06e75d3edf3</t>
-  </si>
-  <si>
-    <t>pou_3747d38bcacf6667</t>
-  </si>
-  <si>
-    <t>pou_1ac5b5fb1bc678a8</t>
-  </si>
-  <si>
-    <t>pou_81238adbc564d089</t>
-  </si>
-  <si>
-    <t>pou_fabfb34b118ce7ad;pou_e30a87044aab141a</t>
-  </si>
-  <si>
-    <t>pou_27c1bb8d9c319a73</t>
-  </si>
-  <si>
-    <t>pou_b41ac27162359688</t>
-  </si>
-  <si>
-    <t>pou_3c58bb863337124c</t>
-  </si>
-  <si>
-    <t>pou_3ed09c6d02e6a223</t>
-  </si>
-  <si>
-    <t>pou_758ca3fb7dc0866d</t>
-  </si>
-  <si>
-    <t>pou_9a2db7263edf1349</t>
-  </si>
-  <si>
-    <t>pou_9aa010928305fd15</t>
-  </si>
-  <si>
-    <t>pou_a33c915279db248d</t>
-  </si>
-  <si>
-    <t>pou_388687d5cad19159</t>
-  </si>
-  <si>
-    <t>pou_b91dc47539fa9df6</t>
-  </si>
-  <si>
-    <t>pou_6f9577324baa23f6</t>
-  </si>
-  <si>
-    <t>pou_fd14c7970b34dbc6</t>
-  </si>
-  <si>
-    <t>pou_4323b50d11682802</t>
-  </si>
-  <si>
-    <t>pou_347cf64798c5fa7d</t>
-  </si>
-  <si>
-    <t>pou_4ef88fc92be6e140</t>
-  </si>
-  <si>
-    <t>pou_c56a879027d470e0</t>
-  </si>
-  <si>
-    <t>pou_91027451246a8f80</t>
-  </si>
-  <si>
-    <t>pou_bf18e50be43e7fab</t>
-  </si>
-  <si>
-    <t>pou_438a5924abfe35cc</t>
-  </si>
-  <si>
-    <t>pou_eb785a67d09eb484</t>
-  </si>
-  <si>
-    <t>pou_03fb35d7ea752b97;pou_70f9ecc3f33c3c5e;pou_21e7b8212daf194f;pou_8930aaef7b142da2;pou_0c81d7de805ed776;pou_c3c791c5458dc4dc;pou_3259126690b7e974;pou_a14e08c625f4683b;pou_e28b70ed2abe0858;pou_8fca379165049725;pou_1fbdf39e54bcf9bd</t>
-  </si>
-  <si>
-    <t>pou_3513355bdd6ba9ef</t>
-  </si>
-  <si>
-    <t>pou_37969918a8550f45</t>
-  </si>
-  <si>
-    <t>pou_9dd2452fcd42e61e;pou_304ed4415914424d</t>
-  </si>
-  <si>
-    <t>pou_37bce23fb43f070d</t>
-  </si>
-  <si>
-    <t>pou_7c8839ead8c1efb2</t>
-  </si>
-  <si>
-    <t>pou_8bc0f9c1ea2007e9</t>
-  </si>
-  <si>
-    <t>pou_7e0980465108a812</t>
-  </si>
-  <si>
-    <t>pou_93e9ab08f18dcd98</t>
-  </si>
-  <si>
-    <t>pou_c691b95b564a9867</t>
-  </si>
-  <si>
-    <t>pou_dd7007d63da0440d</t>
-  </si>
-  <si>
-    <t>pou_70eeffb3aac24eb4</t>
-  </si>
-  <si>
-    <t>pou_d05a3192c9582e56</t>
-  </si>
-  <si>
-    <t>pou_8fc22624c388edb2</t>
-  </si>
-  <si>
-    <t>pou_38b967ca53320c0b</t>
-  </si>
-  <si>
-    <t>pou_7103e376a73c662a</t>
-  </si>
-  <si>
-    <t>pou_db1727105fc317d8</t>
-  </si>
-  <si>
-    <t>pou_366ac68c838f3e8b</t>
-  </si>
-  <si>
-    <t>pou_0e43c27cffa60f49</t>
-  </si>
-  <si>
-    <t>pou_45a61da8bf9379d7</t>
-  </si>
-  <si>
-    <t>pou_51752c73e65f7411</t>
-  </si>
-  <si>
-    <t>pou_7a9122e1aad7e74f</t>
-  </si>
-  <si>
-    <t>pou_ec9a8caf0cb1d662</t>
-  </si>
-  <si>
-    <t>pou_d8d9e6387ab91812</t>
-  </si>
-  <si>
-    <t>pou_1aa237f8e9deba1b</t>
-  </si>
-  <si>
-    <t>pou_e110171c28767efb</t>
-  </si>
-  <si>
-    <t>pou_f4b5ee61bab25916</t>
-  </si>
-  <si>
-    <t>pou_3304af0417016eeb</t>
-  </si>
-  <si>
-    <t>pou_91c10347907cf931</t>
-  </si>
-  <si>
-    <t>pou_2ad042aabeca3bd9</t>
-  </si>
-  <si>
-    <t>pou_0cd0bac171b39fcb</t>
-  </si>
-  <si>
-    <t>pou_93fc0ae942a0cca3</t>
-  </si>
-  <si>
-    <t>pou_295cacc974468097</t>
-  </si>
-  <si>
-    <t>pou_d11ed94fbc6b2e2f</t>
-  </si>
-  <si>
-    <t>pou_1517db95456413c2</t>
-  </si>
-  <si>
-    <t>pou_56882950f6a4dca8</t>
-  </si>
-  <si>
-    <t>pou_f3bff2da7c613511</t>
-  </si>
-  <si>
-    <t>pou_e882803f5493152e</t>
-  </si>
-  <si>
-    <t>pou_cbf5e736e5bba44b</t>
-  </si>
-  <si>
-    <t>pou_7fa63ab82eed50be</t>
-  </si>
-  <si>
-    <t>pou_3cc49295caab08b0</t>
-  </si>
-  <si>
-    <t>pou_c37c3d69adffeded</t>
-  </si>
-  <si>
-    <t>pou_6c205381b100f014</t>
-  </si>
-  <si>
-    <t>pou_35486489b1f994cc</t>
-  </si>
-  <si>
-    <t>pou_5e0acbe288b074f2</t>
-  </si>
-  <si>
-    <t>pou_74b80dbdb49caba7</t>
-  </si>
-  <si>
-    <t>pou_76972d666c803ad4</t>
-  </si>
-  <si>
-    <t>pou_3ea252b1ca3c17c5</t>
-  </si>
-  <si>
-    <t>pou_0fb36f50d8f8034b</t>
-  </si>
-  <si>
-    <t>pou_eeefdba63dd04995</t>
-  </si>
-  <si>
-    <t>pou_cd0fbfc388b9b497</t>
-  </si>
-  <si>
-    <t>pou_7dd436f9cf446c2a</t>
-  </si>
-  <si>
-    <t>pou_f09c137741eaeb15</t>
-  </si>
-  <si>
-    <t>pou_401fd83f350dafde</t>
-  </si>
-  <si>
-    <t>pou_e42573caf600666b</t>
-  </si>
-  <si>
-    <t>pou_f591dcb20cfedbe6</t>
-  </si>
-  <si>
-    <t>pou_469dcc71b72e9e79</t>
-  </si>
-  <si>
-    <t>pou_e93f154c9bfcc828</t>
-  </si>
-  <si>
-    <t>pou_f9cde19a43fc88e7</t>
-  </si>
-  <si>
-    <t>pou_52383bafc33ffe35</t>
-  </si>
-  <si>
-    <t>pou_4ce700c4ddecacd8</t>
-  </si>
-  <si>
-    <t>pou_ce353695293640dc</t>
-  </si>
-  <si>
-    <t>pou_d45cad99ba26028a</t>
-  </si>
-  <si>
-    <t>pou_ed28ea2c15519295</t>
-  </si>
-  <si>
-    <t>pou_9b309f84000e2c05</t>
-  </si>
-  <si>
-    <t>pou_4a4f6cd260007787</t>
-  </si>
-  <si>
-    <t>pou_39d441d97f692b6b</t>
-  </si>
-  <si>
-    <t>pou_29fbb47f407eb2c8</t>
-  </si>
-  <si>
-    <t>pou_8a016e0fb5c8febc</t>
-  </si>
-  <si>
-    <t>pou_1b356aff30572fa2</t>
-  </si>
-  <si>
-    <t>pou_2bc5c51d3da6af99</t>
-  </si>
-  <si>
-    <t>pou_1bba67c69a685195</t>
-  </si>
-  <si>
-    <t>pou_7b9e873e4f653978</t>
-  </si>
-  <si>
-    <t>pou_70ee4c91d413d24f</t>
-  </si>
-  <si>
-    <t>pou_adca042d41f156e7</t>
-  </si>
-  <si>
-    <t>pou_073ef7f66839fbdc</t>
-  </si>
-  <si>
-    <t>pou_445f2598f24b80aa</t>
-  </si>
-  <si>
-    <t>pou_059934877d8b622f</t>
-  </si>
-  <si>
-    <t>pou_6d6704271a28c746</t>
-  </si>
-  <si>
-    <t>pou_ea914878582734c8</t>
-  </si>
-  <si>
-    <t>pou_df0fec4e66a76814</t>
-  </si>
-  <si>
-    <t>pou_5957d2748273c470</t>
-  </si>
-  <si>
-    <t>pou_8a61d57675863671</t>
-  </si>
-  <si>
-    <t>pou_0cb34f1936c91864</t>
-  </si>
-  <si>
-    <t>pou_2630f157308f6d4a</t>
-  </si>
-  <si>
-    <t>pou_6082a9b1edaafaf0</t>
-  </si>
-  <si>
-    <t>pou_43b9353aade40c06</t>
-  </si>
-  <si>
-    <t>pou_33b7397656aa5a13</t>
-  </si>
-  <si>
-    <t>pou_1137fc06d2e06071</t>
-  </si>
-  <si>
-    <t>pou_b0125276f89255e3</t>
-  </si>
-  <si>
-    <t>pou_fd5bc77d97dbf8c1</t>
-  </si>
-  <si>
-    <t>pou_ee9a2674d48f738f</t>
-  </si>
-  <si>
-    <t>pou_84976ad25539e45b</t>
-  </si>
-  <si>
-    <t>pou_a20ab1beac37814c</t>
-  </si>
-  <si>
-    <t>pou_040d7b647eb5ac73</t>
-  </si>
-  <si>
-    <t>pou_01bffe189d731ad3</t>
-  </si>
-  <si>
-    <t>pou_29feef0ab513c5eb</t>
-  </si>
-  <si>
-    <t>pou_4cdabeaa4a1ffb07</t>
-  </si>
-  <si>
-    <t>pou_d39dc2a7bbb0d9ed</t>
-  </si>
-  <si>
-    <t>pou_c749f847e3ca01c4</t>
-  </si>
-  <si>
-    <t>pou_afbd1ec012bb2b5a</t>
-  </si>
-  <si>
-    <t>pou_20e715ad9592f9fa</t>
-  </si>
-  <si>
-    <t>pou_4fdd487d7531c705</t>
-  </si>
-  <si>
-    <t>pou_17b7a77dd3169eee</t>
-  </si>
-  <si>
-    <t>pou_d692dabcd2096ca9</t>
-  </si>
-  <si>
-    <t>pou_62bd6e6f4c0f6fa2</t>
-  </si>
-  <si>
-    <t>pou_84a25cf1276ec4f9</t>
-  </si>
-  <si>
-    <t>pou_09b21b6976dd3e60</t>
-  </si>
-  <si>
-    <t>pou_567c3ad611b81b2a</t>
-  </si>
-  <si>
-    <t>pou_d0d3523f0b1d8b31</t>
-  </si>
-  <si>
-    <t>pou_e3ebb476da27a1c4</t>
-  </si>
-  <si>
-    <t>pou_f2293bde249e218e</t>
-  </si>
-  <si>
-    <t>pou_a8e9986fc61e18e5;pou_202cb28ad0f19314</t>
-  </si>
-  <si>
-    <t>pou_7d67205bf9754906</t>
-  </si>
-  <si>
-    <t>pou_b5af3448018b66c0;pou_b71b3e5e2948b0e2;pou_04ef899fddd32a3f;pou_bf25e8a62d0dbd1a;pou_def8bb814ed8a13e;pou_5b78d9b0924f3c9a;pou_134f1368ddbe239c;pou_0730adf44c58834c;pou_83f54b99c768424b;pou_42246e96509b341a;pou_9479ca761fcbf247;pou_e43de8ae5c8284e0</t>
-  </si>
-  <si>
-    <t>pou_679fffd8a58db840</t>
-  </si>
-  <si>
-    <t>pou_dd717ea47e10579c</t>
-  </si>
-  <si>
-    <t>pou_22d67dfe243cf90a</t>
-  </si>
-  <si>
-    <t>pou_3504b17f0fef5ae0</t>
-  </si>
-  <si>
-    <t>pou_5ce4dcd76f5d896d</t>
-  </si>
-  <si>
-    <t>pou_9aa3e0186ddafc8a</t>
-  </si>
-  <si>
-    <t>pou_52c87abb4c49a3a0</t>
-  </si>
-  <si>
-    <t>pou_ec0375aef53b06b7</t>
-  </si>
-  <si>
-    <t>pou_3fd14922aca140e0</t>
-  </si>
-  <si>
-    <t>pou_aec341cdf9a42b3f</t>
-  </si>
-  <si>
-    <t>pou_f5b18ccd8081bcb3;pou_e16b9cce4a183e3b</t>
-  </si>
-  <si>
-    <t>pou_d5fac640a045f744</t>
-  </si>
-  <si>
-    <t>pou_0085219a91e3c95f</t>
-  </si>
-  <si>
-    <t>pou_dfb4650ad3def175</t>
-  </si>
-  <si>
-    <t>pou_be5e53f7d26c749f</t>
-  </si>
-  <si>
-    <t>pou_fbb89cf7a5063b0c</t>
-  </si>
-  <si>
-    <t>pou_82b65bbefd4ef257</t>
-  </si>
-  <si>
-    <t>pou_8bb581eab286b339</t>
-  </si>
-  <si>
-    <t>pou_5ca0ddcef18cff09</t>
-  </si>
-  <si>
-    <t>pou_f33115d53405a0cd</t>
-  </si>
-  <si>
-    <t>pou_82c3c0f5f36bf9e7;pou_adce4adf8789bc46;pou_5545eb9f8e780c13;pou_c06f5d442089c389;pou_abdd16b0633bf2e7;pou_3f32398718eafd01;pou_c7f84555331e5d13</t>
-  </si>
-  <si>
-    <t>pou_ed6e724c73c3a37d;pou_074ca0ee12f34606</t>
-  </si>
-  <si>
-    <t>pou_879143cea5792e77</t>
-  </si>
-  <si>
-    <t>pou_8b74b923ceaff47d</t>
-  </si>
-  <si>
-    <t>pou_cd143f2f92bf4bbf</t>
-  </si>
-  <si>
-    <t>pou_b9fd5d9bf10f9573</t>
-  </si>
-  <si>
-    <t>pou_b2c45f2c13911b19</t>
-  </si>
-  <si>
-    <t>pou_94fabfcf8bb3a96f</t>
-  </si>
-  <si>
-    <t>pou_6ec294707028468e</t>
-  </si>
-  <si>
-    <t>pou_3bcce3ad2efb9a22</t>
-  </si>
-  <si>
-    <t>pou_dd5cedab4497787b</t>
-  </si>
-  <si>
-    <t>pou_a89e46254a060a13</t>
-  </si>
-  <si>
-    <t>pou_8d9862972c32a15c</t>
-  </si>
-  <si>
-    <t>pou_6517a9d93b381466;pou_6318d9d291e76bf4;pou_b845eb94db94de70;pou_3e922ace65a33021;pou_550c377167769450;pou_29f3b21c655da696;pou_1dabd5ca0aef7c48;pou_133709820463bb68;pou_57df51620c220351</t>
-  </si>
-  <si>
-    <t>pou_4e52e4f0ae84ec16;pou_1c4e741daef8f29d;pou_a562fc0f1c7152e8;pou_05be32f1007b6c19;pou_c7c3f1e01688cfff;pou_24b4a2550553564f;pou_5386443f75a2f75f</t>
-  </si>
-  <si>
-    <t>pou_da062f7afb88fdfa</t>
-  </si>
-  <si>
-    <t>pou_739103e9029a456a;pou_3679a3ac1ba0e87f;pou_969e7a829233cc27;pou_a361025696b8534b</t>
-  </si>
-  <si>
-    <t>pou_3830170dadd76b2a;pou_a55e5ad3accc365f;pou_4ceb6c76d0c18532;pou_6fe5b9b8aaedde2d;pou_01a613cf763faedb;pou_84e4b1f5f7c91dad;pou_00b12a8d06464c02;pou_c62a5fd072e67b47;pou_949b0e53e1164df3;pou_70dce072928aa85e</t>
-  </si>
-  <si>
-    <t>pou_4e95623e8c5fe990</t>
-  </si>
-  <si>
-    <t>pou_9ff819029c43bccc;pou_9d7dc319dcd03cd0;pou_b2f33b3941530b7d;pou_f87e2a4640dbd38f;pou_81a3246aa09659ca;pou_cf450d008a3d2832;pou_ac1618b06b247191;pou_162b751398a1394f;pou_77af58bd6fc306af;pou_b8fdad2c0aaf8d92;pou_086608e6e619588c;pou_c87612bfa7fdbe77;pou_cd387c347ef7b5ac;pou_f40ff33c69611e1d;pou_c97bac5dd09f65bb;pou_d2e7114bb044e566;pou_ba91bca4c9833a9c;pou_c3f3f86bc0beb62a;pou_1d7c8313e23057b7;pou_0d6c7ab1ab6a8239;pou_d71e0f74d296e408;pou_3b51afc34b982b6f;pou_12e08721384170c1;pou_5be9f63031e62de6;pou_d1257de73f0d9c88;pou_63a37fb42625e491;pou_751b458fcbad0245;pou_39050b5c603bea0b;pou_04406ca0dccbce1f;pou_e604f5d654f26547;pou_7d407f8636b59c6a;pou_90a0b2928573cf25;pou_e81ad7c9994052e5;pou_ddb92736e7bcc60b;pou_dfddcc8ec181d550;pou_36b364617bcd1f9b;pou_b9417a7faa5611de;pou_66955f54fa197f1e;pou_14cb7829b6f0dbc4;pou_710249807e0b0e1d;pou_67bbe0db4c9add2c;pou_7c4c939dc996e020;pou_d297dba5535357c3;pou_db585db665896e71;pou_f9ad398d86cd4c79;pou_39e7574919c523ce;pou_2370a202222e9a19;pou_9fa4e003c3ef1fd3;pou_50ffb4f8be260fab;pou_d227ed6c7e71c86e;pou_f6955948ecf363b3;pou_9192f0d4d4660147;pou_e410f9c645e54900;pou_d852087255b8ba97;pou_7ffd5d12aee50ab9;pou_959a04b64200fa7f;pou_c0c7f4817869576d;pou_2bc123bc65bba091;pou_e7fec47be7eacd33;pou_3950742a38ef8430;pou_bb8921eda6ae1379;pou_ec47eb1061e3ea78;pou_827ff31f2082ffcc;pou_c48f9335e90e9030;pou_02eeaff75286215d;pou_db41f66ddf6dcdcd;pou_eb4136d3086c6f87;pou_c829bceb971a825d;pou_d957094d49f93b18;pou_480e5525a9485e3a;pou_03edf91472b9c636;pou_3be3b93761d61ae9;pou_4a3973019e84ba71;pou_34d83bc7b37bfc85;pou_64ae070dc2d1885d;pou_9092df28ef5d40a1;pou_67f01eb21a3c33a7;pou_e96da06bdc0317ea;pou_1532124fca09d6a1;pou_9519210c69bf526a;pou_bdd1515f6990d0ab;pou_4742d698a4ab1a81;pou_6d951d99dc8cf2c2;pou_f5ca8e0b039bf45b;pou_9a9d6c6013051e8d;pou_c9c7fd96b33f492e;pou_dc859009f6ab231c;pou_19c31d1f036c08e6;pou_0b0b6a8d7c2a7077;pou_cdbc01b6423c512c;pou_0e70659665fc240f;pou_a9756da83a5bb448;pou_306c9505257e17c8;pou_bd4e1a36429bcbfc;pou_a11edffdca78ba78;pou_3be75f60a79f2f30;pou_8b24d9f04b23c53b;pou_22ce20cbcf19f02d;pou_fcd73f3a5b0891c5;pou_4119866da3903c0d;pou_811799e653dadd46;pou_b871b0fdc5b8a5bc;pou_7c247db99d886e64;pou_4b1d4f290419059e;pou_aa7eed151b23f5f8;pou_bb24fe64ecc8f09c;pou_d5e9ea0f496dd820;pou_c9a957ae71b397c2;pou_533b25046747c207;pou_32a359229fd1c9c6;pou_d93ceb759d010067;pou_e79e542d512d7fb9;pou_215a02e92dc511db;pou_9b0e8bb620ad9e23;pou_37a5d3a9f3f70fc9;pou_7397f8cd3150fde1;pou_ba21165f5f1f2c82;pou_5685161ce49d79f2;pou_71a8412a52ccd7a6;pou_806b3dbeea19e643;pou_c3a4497a99e528ee;pou_f58f91bc3b1cfa70;pou_6d20abfe0f86fc67;pou_dc62cccd99d9ff12;pou_2880ddf71af75331;pou_7468daf73e0fb9f3;pou_4d6055c8b8537e7d;pou_5a0b4bada4053eac;pou_cf5bed5163941d71;pou_c2eaee31563bb4e0;pou_f41bb91c6abb7cbc;pou_41e8d1df414ff4c0;pou_86e9bc9609a97c9b;pou_8a792a129ead9dcf;pou_094c8a82831072f9;pou_1dd7ee14d4de5390;pou_c40d55ba2b351605;pou_06b27fbc6b0b7960;pou_f62e1c17d61813e6;pou_28ebdde88d345545;pou_c479dbe66afdc665;pou_61ef18704fe3662c;pou_bb2781e7825a0b3b</t>
-  </si>
-  <si>
-    <t>pou_3189b9a0da3d1df0;pou_1e1fabe913569a68;pou_6fe6ea2520aefb4b</t>
-  </si>
-  <si>
-    <t>pou_58f80b3b24681b3a</t>
-  </si>
-  <si>
-    <t>pou_0f1831727b410add</t>
-  </si>
-  <si>
-    <t>pou_3033e360e91830f1</t>
-  </si>
-  <si>
-    <t>pou_5868763483dbf056</t>
-  </si>
-  <si>
-    <t>pou_25c131b233f6f9a4</t>
-  </si>
-  <si>
-    <t>pou_9eafd45f76f2dd82;pou_7520fda55ae8dbcc;pou_0285f1d0d4748f81</t>
-  </si>
-  <si>
-    <t>pou_dfd88d8b73944ddc</t>
-  </si>
-  <si>
-    <t>pou_f0a081dcde5370db</t>
-  </si>
-  <si>
-    <t>pou_7a5eb0c75ee8204f</t>
-  </si>
-  <si>
-    <t>pou_d69c270d64b11deb</t>
-  </si>
-  <si>
-    <t>pou_262ec0687f62045e</t>
-  </si>
-  <si>
-    <t>pou_5ef6abe83e4ef1f7;pou_b69bbff9b270fa83;pou_b15cda00bb134de1;pou_854c402047e0bd32;pou_f0765b306f9a09a8;pou_b114b819646bafc7;pou_cc61da99f471583d</t>
-  </si>
-  <si>
-    <t>pou_9745cf77f6de3dd0</t>
-  </si>
-  <si>
-    <t>pou_559b7b78d292a5bc</t>
-  </si>
-  <si>
-    <t>pou_3dc5c370b70ff855;pou_c4679672f4748b45</t>
-  </si>
-  <si>
-    <t>pou_b6e1725488800f8e</t>
-  </si>
-  <si>
-    <t>pou_fba721267d202391</t>
-  </si>
-  <si>
-    <t>pou_3b8dd14734a0cebf</t>
-  </si>
-  <si>
-    <t>pou_543cc9ae080013b7</t>
-  </si>
-  <si>
-    <t>pou_2f94c2a0a92668a1</t>
-  </si>
-  <si>
-    <t>pou_a735f53f44c8de3d;pou_62442de976b3ef26</t>
-  </si>
-  <si>
-    <t>pou_4c951a9b5852371c;pou_f131571b81820d0d</t>
-  </si>
-  <si>
-    <t>pou_3107c553b6d3487a;pou_b013628752762592;pou_55b31216e3418de7;pou_aa4eb7e1c44b1bdd;pou_c532a2e4d2f1e9b1;pou_a9e9560d08b6026a;pou_2c4f14bd44c1c564;pou_3c13751dfb8a43cf;pou_ca3475932fbecb9e;pou_9802d834b282192b;pou_8b59912d1bbb69bb;pou_27b4d20e7c7ac7d5;pou_4133f187967f5838;pou_8bace32bc1f73b62;pou_62aea05f9524b075;pou_0963a07bb6a78007;pou_f0bb66b153086367;pou_58afd0edccf4c2da;pou_1ecf47bb3350dc70;pou_99b317a548021646;pou_551f3dc0a3c6efb8;pou_5d26374eb56f394f;pou_c9c82316f70402ca;pou_27986cbb4627f3a5;pou_95fd41a7d3234142;pou_be0532dad2510c8a;pou_6d12f2b037cdab39</t>
-  </si>
-  <si>
-    <t>pou_aa55405d559776ef</t>
-  </si>
-  <si>
-    <t>pou_5fc6007c0cec3b56</t>
-  </si>
-  <si>
-    <t>pou_9a838402b8f7bde5;pou_26385414a4af0c9e;pou_1650b719f5efb07b;pou_b56a67138fea4a43;pou_62749a3f3c671663</t>
-  </si>
-  <si>
-    <t>pou_ab11a32d29e6eaa3;pou_5fcee831d3bb0b2b;pou_f28738d643db8da6;pou_a6ec55437db66ee1;pou_b0cde5677a092256;pou_e06c963e14460977;pou_69fd451794f39fb6;pou_d8031e1c3dbeb046;pou_9bfb7a545354e028;pou_b62c2c66573e0eb1;pou_2c95a9e6cb43e61c;pou_b9fcdc7340156b6a;pou_68404dbccde2d23c;pou_926050efe189a38d;pou_5fc97e9763e5a110;pou_b772d999689aad8a;pou_3a7716c4671ca578;pou_0731c646cd18d49a;pou_82a4db8ed2826d3b;pou_beea13e7c0431210;pou_7535827663ff37a7;pou_f53687b351ed1de0;pou_ce716d89b7213256;pou_db33041c46d730dd;pou_5971bb1f23d24fd4;pou_867168c4466e833a;pou_0848932d5e083a97;pou_6f03d95c54ba56c8;pou_0e6a59adb0b8797e</t>
-  </si>
-  <si>
-    <t>pou_79f98f3de39f5fa8;pou_38751de1354842e3;pou_ae73be6642ece1ba;pou_d09ac70e8ec640de;pou_219edc6f942952ff;pou_ae0b1831e91a81a8;pou_5df1e160cff64711;pou_89dd04ebdf907815</t>
-  </si>
-  <si>
-    <t>pou_e96bba81906a11b8;pou_f322a7916558612b</t>
-  </si>
-  <si>
-    <t>pou_4f9f63382bf1d7ba</t>
-  </si>
-  <si>
-    <t>pou_41fd12077716ba45</t>
-  </si>
-  <si>
-    <t>pou_d2252c61b59981b4;pou_6937ec23f8cf92e8;pou_0e3424392894f755;pou_3901f1850d2315de;pou_9180b23b50a4714d;pou_9e8f2d6ea9aad579;pou_d3bb8966dbc7cc73;pou_18dbacbc34a8b276;pou_538ed9fae868cd25;pou_72dda3d45cf11530;pou_adc91dc46301e427;pou_ae247a48a241865a;pou_10246456b2396043;pou_e274aaab24710e5d;pou_5ae7e14d3c7f35a0</t>
-  </si>
-  <si>
-    <t>pou_d0c4c4ea87b7d7ac;pou_4505c46a063ef9ec;pou_fed3b333c54174cf;pou_8f8618f96a793584;pou_28452fcd317f8739;pou_326ec769728ed332;pou_8553662e8eb104d8</t>
-  </si>
-  <si>
-    <t>pou_ac4a3cf1c7468198</t>
-  </si>
-  <si>
-    <t>pou_b54a10ea684c581b</t>
-  </si>
-  <si>
-    <t>pou_21206953fb9fefa5</t>
-  </si>
-  <si>
-    <t>pou_72c1577b79376742</t>
-  </si>
-  <si>
-    <t>pou_831fd67d2da58b93</t>
-  </si>
-  <si>
-    <t>pou_93893c05fbb4cdfa</t>
-  </si>
-  <si>
-    <t>pou_499a89b33d7a4d51</t>
-  </si>
-  <si>
-    <t>pou_7236352f2a497386</t>
-  </si>
-  <si>
-    <t>pou_6186a0827a22e764</t>
-  </si>
-  <si>
-    <t>pou_ccdaaaf68e506d01;pou_6dcfa07b54828b82;pou_67bd227f6aa1bdb3;pou_10ed0e95200368e3;pou_1745389709e47d8c;pou_8fd8179ae524569f;pou_d41c03e3ea5bf83a;pou_865c42ca83ee9ee0;pou_7e3d07c6f906e3c5;pou_dfa8d5751ab96693;pou_e5ad233446a2302e;pou_f68a412eedb3f2b9</t>
-  </si>
-  <si>
-    <t>pou_8e330371a53bd796</t>
-  </si>
-  <si>
-    <t>pou_d93e0db0fbf6a93a;pou_4b64d6774fd16b4d</t>
-  </si>
-  <si>
-    <t>pou_18256706854ac884;pou_52149251f1dee744;pou_7e5c252cff234151;pou_93e2f694edd7fa41;pou_beab6d647269fd05;pou_dadb8dd7d974d84e</t>
-  </si>
-  <si>
-    <t>pou_05f3f107010000fa;pou_78399e921a303052;pou_d9a684f84a0b732f;pou_8f449ddf1fdc7f23;pou_74a09f05855d7067;pou_ce3dd7a22501892d;pou_4b6b5754a5c94fa2;pou_73c3bc11cc33578c;pou_ff8b17959437eec6;pou_af17cf752193a9d5;pou_36a7e1618b53f360;pou_b3b391b235b520c2;pou_dc1aaacdaeedf419;pou_f0a763a466fbffca</t>
-  </si>
-  <si>
-    <t>pou_eb5e6f58ca65ec13;pou_ab2d5652bebcde4c;pou_44d6dca8d236af7c;pou_e075a6456840856d;pou_1b207e0340dedfdd;pou_93fb9affa02ac651;pou_cab7da6b020ba689;pou_595d1b232359fa04;pou_f901a0ce400e0351;pou_5f5d7415f2d3bdba;pou_eca1a3bba16f6bfc</t>
-  </si>
-  <si>
-    <t>pou_60dff1466478f5ef</t>
-  </si>
-  <si>
-    <t>pou_f6590a8a83d34109</t>
-  </si>
-  <si>
-    <t>pou_028c944aa012093b;pou_17056e70b56750f4;pou_ddde0b64d5cebbc6;pou_fae522c0949b03c5;pou_1fb5b86e07a0eb38;pou_7e8eecc7de008eba;pou_77a6cca3ab9f650d</t>
-  </si>
-  <si>
-    <t>pou_a2a65e715ebd9963;pou_29f7ad6d333895fa;pou_45108c368e29cd95;pou_a4055e9d1f760b64;pou_491188961d448df8;pou_de495d6494687464;pou_f16058fa51eb6053;pou_a4452779b87ba987;pou_63afb9652f2132d0;pou_917facd75c96e1be;pou_aa4717ce4cbda09e;pou_594acfceec1bc143;pou_83890a3ab025c659;pou_e3928ce931dc793a;pou_1516be412cc8c47d;pou_094ae4a7a6ebb217;pou_fb3e7b7b9f5d4264;pou_c9b06c6908bd4fcb;pou_46ac0166317298a9</t>
-  </si>
-  <si>
-    <t>pou_b3a4664fb7254b70</t>
-  </si>
-  <si>
-    <t>pou_9f5603f6a0dfd589;pou_9fffaa522efefed0;pou_ca78e3ba95181096;pou_11cb77652ce5a39f;pou_afd7506f07f682fa;pou_fa38add8c6eefdd7</t>
-  </si>
-  <si>
-    <t>pou_0fa46620dff154eb</t>
-  </si>
-  <si>
-    <t>pou_a0e29302f30f5180;pou_095458d6125e44c0;pou_13313cb4ef06bc5b</t>
-  </si>
-  <si>
-    <t>pou_4addfc6d01779951</t>
-  </si>
-  <si>
-    <t>pou_37cdba0fcbd44c97;pou_23d9ed4c589a7ad2;pou_ce2ec1fb4264a2f5;pou_074c65a9ad935023;pou_81d965f76d41c98c;pou_4277cad7d26b544d</t>
-  </si>
-  <si>
-    <t>pou_800921757186ce51</t>
-  </si>
-  <si>
-    <t>pou_dafe7c69ed5a7665</t>
-  </si>
-  <si>
-    <t>pou_f9c9197f0a9a2c53</t>
-  </si>
-  <si>
-    <t>pou_be29fc0698c6fbda;pou_b72261651e6e814e;pou_224e7b3458ff42e4;pou_681f0c4870e0d214;pou_4ab704831174c869;pou_f29a0d46b6252555;pou_c7791c2c07c017b7;pou_c668219d39dd1882;pou_c12882ec705bb1b3;pou_4c6b218bfea5bbf7;pou_764a497c89e73df2;pou_aa7cc982d47b9960;pou_ad47cec01167c53d;pou_9e991c4ea5f20191;pou_f897dca395305b29;pou_6d8ce4a3ca025967;pou_cc24fe2e3252f3f5;pou_6209e3aa9414fb75;pou_9fbbdff39278d178;pou_b160e62009edf408;pou_4b2d898f47c64cea</t>
-  </si>
-  <si>
-    <t>pou_3017535a37009edd</t>
-  </si>
-  <si>
-    <t>pou_0095a15872fa9de3</t>
-  </si>
-  <si>
-    <t>pou_2225f2c63b8e9476</t>
-  </si>
-  <si>
-    <t>pou_d17c7e784f8c7b9b;pou_7e56f0ab3bfd0b21;pou_3d8ccc6fa7d628b4;pou_3fe08ca6acaae3d8;pou_6f9ad5d4a4244128;pou_e32869d45e46a3e0;pou_d09feff8671a055d;pou_afe99d986af2aaf0;pou_08cfa81dff575806;pou_568238b8197d2458;pou_99ce9b1b02451201;pou_f5dd79e814bbdc40;pou_c24af056ff503b52;pou_8cfaca752141b920;pou_0c95ef1db55a174e</t>
-  </si>
-  <si>
-    <t>pou_893e6967dfbb7c24</t>
-  </si>
-  <si>
-    <t>pou_78a67d0654370ec9</t>
-  </si>
-  <si>
-    <t>pou_e92d5dd8ac1dee0c</t>
-  </si>
-  <si>
-    <t>pou_b15bb719c022a88d</t>
-  </si>
-  <si>
-    <t>pou_d3ab831f718693d3</t>
-  </si>
-  <si>
-    <t>pou_47dcedf6d8dbd9e9</t>
-  </si>
-  <si>
-    <t>pou_10679746d8bfac99</t>
-  </si>
-  <si>
-    <t>pou_7d1bb4457c3c72f3</t>
-  </si>
-  <si>
-    <t>pou_e720c875db0fad8f</t>
-  </si>
-  <si>
-    <t>pou_23fab60103dc93e1</t>
-  </si>
-  <si>
-    <t>pou_ba6fe83c55c18d08</t>
-  </si>
-  <si>
-    <t>pou_078ece639cbcf9a1;pou_04780914073f982a</t>
-  </si>
-  <si>
-    <t>pou_6d438a02668dc906</t>
-  </si>
-  <si>
-    <t>pou_98f58b0f7cc5c38a</t>
-  </si>
-  <si>
-    <t>pou_670a1523140cce15</t>
-  </si>
-  <si>
-    <t>pou_73dc55934abe8579</t>
-  </si>
-  <si>
-    <t>pou_a3bfe3578778de55</t>
-  </si>
-  <si>
-    <t>pou_3bf4965df8b797dd</t>
-  </si>
-  <si>
-    <t>pou_dc1fc85c9bb08fc4</t>
-  </si>
-  <si>
-    <t>pou_df27db82cb9a336c</t>
-  </si>
-  <si>
-    <t>pou_b00aec1474cac6b6</t>
-  </si>
-  <si>
-    <t>pou_11437f5f149f5cb1</t>
-  </si>
-  <si>
-    <t>pou_bef628920d8099de</t>
-  </si>
-  <si>
-    <t>pou_538392e5fd6d4a04</t>
-  </si>
-  <si>
-    <t>pou_f9d956c55075175d</t>
-  </si>
-  <si>
-    <t>pou_e1becf9b7937a5f4</t>
-  </si>
-  <si>
-    <t>pou_dbd23ef6f0520f12</t>
-  </si>
-  <si>
-    <t>pou_ed71fb7c290f6461</t>
-  </si>
-  <si>
-    <t>pou_6faa9441bd344750</t>
-  </si>
-  <si>
-    <t>pou_41943f828a1b9d0b</t>
-  </si>
-  <si>
-    <t>pou_23b11181bb21034a</t>
-  </si>
-  <si>
-    <t>pou_739debb6c9e2a748</t>
-  </si>
-  <si>
-    <t>pou_1ae79634692c66db</t>
-  </si>
-  <si>
-    <t>pou_69dbd036e3687ad6</t>
-  </si>
-  <si>
-    <t>pou_193964122aa68294</t>
-  </si>
-  <si>
-    <t>pou_59f6e782c41cb94e</t>
-  </si>
-  <si>
-    <t>pou_8e48ca556c52c54f</t>
-  </si>
-  <si>
-    <t>pou_0410da2ed9cb4687</t>
-  </si>
-  <si>
-    <t>pou_28e2847c176a4b91</t>
-  </si>
-  <si>
-    <t>pou_a10959a3487fc4f2</t>
-  </si>
-  <si>
-    <t>pou_b71c81ed58ce332f</t>
-  </si>
-  <si>
-    <t>pou_50252f385c0f1647</t>
-  </si>
-  <si>
-    <t>pou_7ae61b994bed5062</t>
-  </si>
-  <si>
-    <t>pou_7ff38791429082ed</t>
-  </si>
-  <si>
-    <t>pou_d4f49cab55ae027b</t>
-  </si>
-  <si>
-    <t>pou_99be62a5b65bf64a</t>
-  </si>
-  <si>
-    <t>pou_ce07bd67f088c7a7</t>
-  </si>
-  <si>
-    <t>pou_79affb553c7fb6de</t>
-  </si>
-  <si>
-    <t>pou_bbb6ecb033326b8c</t>
-  </si>
-  <si>
-    <t>pou_08723caee6efe86b</t>
-  </si>
-  <si>
-    <t>pou_6ea4414173c62526</t>
-  </si>
-  <si>
-    <t>pou_6aab72087672e704</t>
-  </si>
-  <si>
-    <t>pou_ff37cc3d36f032f8</t>
-  </si>
-  <si>
-    <t>pou_2a5bd8e7fb46aeac</t>
-  </si>
-  <si>
-    <t>pou_1106c4cff33cc1eb</t>
-  </si>
-  <si>
-    <t>pou_908a456a878b5688</t>
-  </si>
-  <si>
-    <t>pou_7eb3fa73ed73617a</t>
-  </si>
-  <si>
-    <t>pou_92ccbe2a3682ec0e</t>
-  </si>
-  <si>
-    <t>pou_12b1d1bf88de56dc</t>
-  </si>
-  <si>
-    <t>pou_1d18c13a9bf8b069</t>
-  </si>
-  <si>
-    <t>pou_dce413f0b620ba00</t>
-  </si>
-  <si>
-    <t>pou_e405f5af9a1851d5</t>
-  </si>
-  <si>
-    <t>pou_f6e4e433a04e5014</t>
-  </si>
-  <si>
-    <t>pou_7fdd4a4e18c4ae5c</t>
-  </si>
-  <si>
-    <t>pou_487563b1177cf2c6</t>
-  </si>
-  <si>
-    <t>pou_970da51997b9c927</t>
-  </si>
-  <si>
-    <t>pou_f881164ffd2d0cf9</t>
-  </si>
-  <si>
-    <t>pou_47ffbea4d1b117cd</t>
-  </si>
-  <si>
-    <t>pou_714583128191c0b1</t>
-  </si>
-  <si>
-    <t>pou_869efee8e1f75570</t>
-  </si>
-  <si>
-    <t>pou_3439d2ef42cbf202</t>
-  </si>
-  <si>
-    <t>pou_46e3f1a1d47e557a</t>
-  </si>
-  <si>
-    <t>pou_665f322301454f61</t>
-  </si>
-  <si>
-    <t>pou_59fc5c16ce8c61d1</t>
-  </si>
-  <si>
-    <t>pou_9691f7fcea922c52</t>
-  </si>
-  <si>
-    <t>pou_61fdc811c75b2a7f</t>
-  </si>
-  <si>
-    <t>pou_b0b4f9e306ed6a32</t>
-  </si>
-  <si>
-    <t>pou_fb8311b1b70037c4</t>
-  </si>
-  <si>
-    <t>pou_587e7a87f200b86f</t>
-  </si>
-  <si>
-    <t>pou_1b7c616013342080</t>
-  </si>
-  <si>
-    <t>pou_4c57268506c65152</t>
-  </si>
-  <si>
-    <t>pou_dd909426041cc8e6</t>
-  </si>
-  <si>
-    <t>pou_606ad5f9b5b2ffbf</t>
-  </si>
-  <si>
-    <t>pou_effaa5d881a39c02</t>
-  </si>
-  <si>
-    <t>pou_b1d85f0595460585</t>
-  </si>
-  <si>
-    <t>pou_b3ba39a08f44c897</t>
-  </si>
-  <si>
-    <t>pou_1edac1cac816d682</t>
-  </si>
-  <si>
-    <t>pou_899557706b3d76ba</t>
-  </si>
-  <si>
-    <t>pou_91c4c543abb308ac</t>
-  </si>
-  <si>
-    <t>pou_fd0b054e20b957d9</t>
-  </si>
-  <si>
-    <t>pou_8d74ff17699cbf85</t>
-  </si>
-  <si>
-    <t>pou_990d006f1eb2e2df</t>
-  </si>
-  <si>
-    <t>pou_ba1a40fc266bd9b6</t>
-  </si>
-  <si>
-    <t>pou_6ac606b0193c08c8</t>
-  </si>
-  <si>
-    <t>pou_c962f566dac00edd</t>
-  </si>
-  <si>
-    <t>pou_1c0b44193fedaa4f</t>
-  </si>
-  <si>
-    <t>pou_341c8d0a36f7eb6c</t>
-  </si>
-  <si>
-    <t>pou_177b241f942e4d53</t>
-  </si>
-  <si>
-    <t>pou_9ed25de33910ef3c</t>
-  </si>
-  <si>
-    <t>pou_4d23bf077c07cd91</t>
-  </si>
-  <si>
-    <t>pou_13eaf8fa35087b42</t>
-  </si>
-  <si>
-    <t>pou_687217d72a602958</t>
-  </si>
-  <si>
-    <t>pou_cb11cc106500e6de</t>
-  </si>
-  <si>
-    <t>pou_09e6738b626df150</t>
-  </si>
-  <si>
-    <t>pou_30c0f35c7f387ee4</t>
-  </si>
-  <si>
-    <t>pou_418b31f41938df41</t>
-  </si>
-  <si>
-    <t>pou_d40468e7b9d9f17e</t>
-  </si>
-  <si>
-    <t>pou_073c8f0fb2c22cfe</t>
-  </si>
-  <si>
-    <t>pou_df5178c59f51aedf</t>
-  </si>
-  <si>
-    <t>pou_85fd3a99cc3cb87d</t>
-  </si>
-  <si>
-    <t>pou_03ad0da5b05246af</t>
-  </si>
-  <si>
-    <t>pou_214441a93b3957fc</t>
-  </si>
-  <si>
-    <t>pou_ec0d619c0a468afe</t>
-  </si>
-  <si>
-    <t>pou_a5750d7201bbcabd</t>
-  </si>
-  <si>
-    <t>pou_747c8a79ed21c00c</t>
-  </si>
-  <si>
-    <t>pou_8c1c1714e0f66b77</t>
-  </si>
-  <si>
-    <t>pou_fc9a38f45cbbfaf6</t>
-  </si>
-  <si>
-    <t>pou_411f1283373e1bab</t>
-  </si>
-  <si>
-    <t>pou_4554a07eee5e1435</t>
-  </si>
-  <si>
-    <t>pou_8822e09cd2ec39ec</t>
-  </si>
-  <si>
-    <t>pou_e892bed77e67aa01</t>
-  </si>
-  <si>
-    <t>pou_1fcccf0a896a6f68</t>
-  </si>
-  <si>
-    <t>pou_6869a16a3fcddefa</t>
-  </si>
-  <si>
-    <t>pou_bd0ed5dd0ffaed8d</t>
-  </si>
-  <si>
-    <t>pou_5341d34eea8b9c6f</t>
-  </si>
-  <si>
-    <t>pou_38809c7a10e214c6</t>
-  </si>
-  <si>
-    <t>pou_3b33f475edbb14af</t>
-  </si>
-  <si>
-    <t>pou_1650ca6e816d7a4c</t>
-  </si>
-  <si>
-    <t>pou_32836cba5f5ada1e</t>
-  </si>
-  <si>
-    <t>pou_ceddd40f8a215345</t>
-  </si>
-  <si>
-    <t>pou_0bacbb57862347c1</t>
-  </si>
-  <si>
-    <t>pou_ebf59644e3441235</t>
-  </si>
-  <si>
-    <t>pou_70d8fbe986b0386a</t>
-  </si>
-  <si>
-    <t>pou_13f44f318112fe34</t>
-  </si>
-  <si>
-    <t>pou_a20c85ae776ba32e</t>
-  </si>
-  <si>
-    <t>pou_760d997485f31ecd</t>
-  </si>
-  <si>
-    <t>pou_c6a38552004524d9</t>
-  </si>
-  <si>
-    <t>pou_43e15fb74be89e1c</t>
-  </si>
-  <si>
-    <t>pou_91c672bfc7781edb</t>
-  </si>
-  <si>
-    <t>pou_7572feb99811c363</t>
-  </si>
-  <si>
-    <t>pou_708b97fb847bac88</t>
-  </si>
-  <si>
-    <t>pou_e14f079bb284d443</t>
-  </si>
-  <si>
-    <t>pou_7a3b7713fb3a448d</t>
-  </si>
-  <si>
-    <t>pou_979a93ecc3e0d7d4</t>
-  </si>
-  <si>
-    <t>pou_a9d1632535c8ad87</t>
-  </si>
-  <si>
-    <t>pou_c954a2f172787b13</t>
-  </si>
-  <si>
-    <t>pou_3ad1b00cc6cf05f6</t>
-  </si>
-  <si>
-    <t>pou_918070c4fa402775</t>
-  </si>
-  <si>
-    <t>pou_7c12122f8fb09210</t>
-  </si>
-  <si>
-    <t>pou_f31c53956f2a0534</t>
-  </si>
-  <si>
-    <t>pou_8ffd9927fc45338d</t>
-  </si>
-  <si>
-    <t>pou_ed4c9a8c66ed1828</t>
-  </si>
-  <si>
-    <t>pou_4fb00ab0066e351b</t>
-  </si>
-  <si>
-    <t>pou_ecf987964af69281</t>
-  </si>
-  <si>
-    <t>pou_1157e7123dc2f8ae</t>
-  </si>
-  <si>
-    <t>pou_0b8ba6b0cd08ec70</t>
-  </si>
-  <si>
-    <t>pou_6a59653df839264a</t>
-  </si>
-  <si>
-    <t>pou_b6f41adf4ebfcfe6</t>
-  </si>
-  <si>
-    <t>pou_31bdde4d4a226088</t>
-  </si>
-  <si>
-    <t>pou_c5c3b6b511fe7923</t>
-  </si>
-  <si>
-    <t>pou_541726d87f2ac7c2</t>
-  </si>
-  <si>
-    <t>pou_fd04ed83936d04c5</t>
-  </si>
-  <si>
-    <t>pou_918149fa2f020c08</t>
-  </si>
-  <si>
-    <t>pou_f643f794bc5c8a7b</t>
-  </si>
-  <si>
-    <t>pou_e298cace5db6abbe</t>
-  </si>
-  <si>
-    <t>pou_43870d0d9b2a5f7c</t>
-  </si>
-  <si>
-    <t>pou_9a63dfaee626c036</t>
-  </si>
-  <si>
-    <t>pou_ef40d92548cb342c</t>
-  </si>
-  <si>
-    <t>pou_999490a237965f42</t>
-  </si>
-  <si>
-    <t>pou_b7583515dd45c105</t>
-  </si>
-  <si>
-    <t>pou_4501a21189a67296</t>
-  </si>
-  <si>
-    <t>pou_d8da82a0ccb57427</t>
-  </si>
-  <si>
-    <t>pou_ce5d78f4ec755e28</t>
-  </si>
-  <si>
-    <t>pou_f8a18707b453fd3b</t>
-  </si>
-  <si>
-    <t>pou_203ba004c923f949</t>
-  </si>
-  <si>
-    <t>pou_9aac9667cb88d0fd</t>
-  </si>
-  <si>
-    <t>pou_36e23ec156f693af</t>
-  </si>
-  <si>
-    <t>pou_8fd397cac86ec40f</t>
-  </si>
-  <si>
-    <t>pou_d8da7d86fd84fbf6</t>
-  </si>
-  <si>
-    <t>pou_1fbf4a72fc06be98</t>
-  </si>
-  <si>
-    <t>pou_4ba20e0eb1919156</t>
-  </si>
-  <si>
-    <t>pou_d50471a72744ecb6</t>
-  </si>
-  <si>
-    <t>pou_6b78162f58f0a554</t>
-  </si>
-  <si>
-    <t>pou_c249568cb5e73781</t>
-  </si>
-  <si>
-    <t>pou_cb29e7bfb1823af0</t>
-  </si>
-  <si>
-    <t>pou_ecc5eeaab7800425</t>
-  </si>
-  <si>
-    <t>pou_02990047044da357</t>
-  </si>
-  <si>
-    <t>pou_30a1b07f6a7055a7</t>
-  </si>
-  <si>
-    <t>pou_05b33c9f55317da4</t>
-  </si>
-  <si>
-    <t>pou_776aa11ad0901390</t>
-  </si>
-  <si>
-    <t>pou_8b103502d6d2c5b6</t>
-  </si>
-  <si>
-    <t>pou_9bb4639b457b77b5</t>
-  </si>
-  <si>
-    <t>pou_5ec525e17e96fff1</t>
-  </si>
-  <si>
-    <t>pou_0401728fd7c3751e</t>
-  </si>
-  <si>
-    <t>pou_4bbdbfce9cbfac9d</t>
-  </si>
-  <si>
-    <t>pou_c2d34cbf58ec427c</t>
-  </si>
-  <si>
-    <t>pou_a6ebf9b249207a25</t>
-  </si>
-  <si>
-    <t>pou_8bec9b2f4d59060c</t>
-  </si>
-  <si>
-    <t>pou_049dccbccf71bbb2</t>
-  </si>
-  <si>
-    <t>pou_ca5f2b490f9a4ecc</t>
-  </si>
-  <si>
-    <t>pou_6bd0f718fb769d0f</t>
-  </si>
-  <si>
-    <t>pou_87e666e9fd68904f</t>
-  </si>
-  <si>
-    <t>pou_be8e298ec5606daa</t>
-  </si>
-  <si>
-    <t>pou_fdbbb36c92825236</t>
-  </si>
-  <si>
-    <t>pou_e62e9b2d8ed69443</t>
-  </si>
-  <si>
-    <t>pou_7d357202fdb0c718</t>
-  </si>
-  <si>
-    <t>pou_16aab80c9768d499</t>
-  </si>
-  <si>
-    <t>pou_c26ca9fd2e18389b</t>
-  </si>
-  <si>
-    <t>pou_227119629a6287f7</t>
-  </si>
-  <si>
-    <t>pou_8fae9fd8f09b4bdd</t>
-  </si>
-  <si>
-    <t>pou_e13114292f993daf</t>
-  </si>
-  <si>
-    <t>pou_4c19ab33051280b8</t>
-  </si>
-  <si>
-    <t>pou_83a88cc6c22ddfdb</t>
-  </si>
-  <si>
-    <t>pou_55b918be47e0f518</t>
-  </si>
-  <si>
-    <t>pou_db50e3ef93586f11</t>
-  </si>
-  <si>
-    <t>pou_0fdf2b615f099f47</t>
-  </si>
-  <si>
-    <t>pou_f2fb291cc959f705</t>
-  </si>
-  <si>
-    <t>pou_7e35d2c863f4b70a</t>
-  </si>
-  <si>
-    <t>pou_1c15c137fcc519c5</t>
-  </si>
-  <si>
-    <t>pou_d552e7e1f43dc139</t>
-  </si>
-  <si>
-    <t>pou_0ca0b4673cfc115e</t>
-  </si>
-  <si>
-    <t>pou_a1241966cf72ecfa</t>
-  </si>
-  <si>
-    <t>pou_c8b63106e76835a1</t>
-  </si>
-  <si>
-    <t>pou_926ef1330b845517</t>
-  </si>
-  <si>
-    <t>pou_d70695451af625d4</t>
-  </si>
-  <si>
-    <t>pou_00f3f1f5871ceee7</t>
-  </si>
-  <si>
-    <t>pou_8bc860079f8f44d0;pou_4418fc569525b584</t>
-  </si>
-  <si>
-    <t>pou_0fe9e748d5503c72;pou_0286b56d29f4b8f8;pou_103f0bc9af1360a7;pou_4d91ef9e3915d8fc;pou_f5b7c43d8c8fc414;pou_ee586a24810fc466;pou_a7fd8659639dba85;pou_e56b2a2f544d16d3;pou_8d1e895099a6f9c9;pou_607a106aeb23da13;pou_b91032c204d90ba7;pou_cc7e69902f1f7a0f</t>
-  </si>
-  <si>
-    <t>pou_f2c82ed8ce770129</t>
-  </si>
-  <si>
-    <t>pou_d3326d7e110cb73c</t>
-  </si>
-  <si>
-    <t>pou_fd93e17a695e9f7c</t>
-  </si>
-  <si>
-    <t>pou_214781e4cbe7e473</t>
-  </si>
-  <si>
-    <t>pou_ed60111a48b1856f</t>
-  </si>
-  <si>
-    <t>pou_e4574329c278c836</t>
-  </si>
-  <si>
-    <t>pou_8dce89547aec4343</t>
-  </si>
-  <si>
-    <t>pou_52cd39ac797603da</t>
-  </si>
-  <si>
-    <t>pou_a8d47ac863e53e20</t>
-  </si>
-  <si>
-    <t>pou_9d4306fe5a9969ac</t>
-  </si>
-  <si>
-    <t>pou_5c8022a2817fc111</t>
-  </si>
-  <si>
-    <t>pou_c31a781906792ccf</t>
-  </si>
-  <si>
-    <t>pou_6969255589a0180f</t>
-  </si>
-  <si>
-    <t>pou_dcbc55e946d02507</t>
-  </si>
-  <si>
-    <t>pou_4c432a868379c35e</t>
-  </si>
-  <si>
-    <t>pou_a192a6952a93ff76</t>
-  </si>
-  <si>
-    <t>pou_2d8ff029dae08602</t>
-  </si>
-  <si>
-    <t>pou_9181f3c485f860f8</t>
-  </si>
-  <si>
-    <t>pou_4c86bf114dd9123c</t>
-  </si>
-  <si>
-    <t>pou_4814a5cba5e4ea7f</t>
-  </si>
-  <si>
-    <t>pou_ccb340a3dc422f47</t>
-  </si>
-  <si>
-    <t>pou_c1e7a13b0e9c3b01</t>
-  </si>
-  <si>
-    <t>pou_73cbcda58d69de89</t>
-  </si>
-  <si>
-    <t>pou_7476211cc1e933e2</t>
-  </si>
-  <si>
-    <t>pou_0e7f5937046d5235</t>
-  </si>
-  <si>
-    <t>pou_4860915301e2e0be</t>
-  </si>
-  <si>
-    <t>pou_4604ee7add548cec</t>
-  </si>
-  <si>
-    <t>pou_9c1cbcdd8357ec95</t>
-  </si>
-  <si>
-    <t>pou_ce82742912d76f55</t>
-  </si>
-  <si>
-    <t>pou_ee6f5fbb79c693d4</t>
-  </si>
-  <si>
-    <t>pou_af9c25c3e7a0d625</t>
-  </si>
-  <si>
-    <t>pou_3e0f6c3d4fdf607c</t>
-  </si>
-  <si>
-    <t>pou_534d0d93a4cbfe23</t>
-  </si>
-  <si>
-    <t>pou_6f2466a6f8e57743</t>
-  </si>
-  <si>
-    <t>pou_586c489edb3b5c80</t>
-  </si>
-  <si>
-    <t>pou_de301b4ecf862948</t>
-  </si>
-  <si>
-    <t>pou_f8d4ee3d75b0fd98</t>
-  </si>
-  <si>
-    <t>pou_84f2faf7e88b4b7c</t>
-  </si>
-  <si>
-    <t>pou_dbed1294a91a09e6</t>
-  </si>
-  <si>
-    <t>pou_001adb9ab341afe4</t>
-  </si>
-  <si>
-    <t>pou_536dc01df156efbc</t>
-  </si>
-  <si>
-    <t>pou_e8b2d87d9361eaf7</t>
+    <t>pou_27e54b3d27e557c7</t>
+  </si>
+  <si>
+    <t>pou_80b669f99b483fd4</t>
+  </si>
+  <si>
+    <t>pou_e879297c6b479255;pou_84c5cec8cd154ec4</t>
+  </si>
+  <si>
+    <t>pou_2e56f190f68b8364</t>
+  </si>
+  <si>
+    <t>pou_2df458adb54f9c23</t>
+  </si>
+  <si>
+    <t>pou_21dedd43d7ebc959</t>
+  </si>
+  <si>
+    <t>pou_4d5ee45c02635efb</t>
+  </si>
+  <si>
+    <t>pou_8da13b897917ba52</t>
+  </si>
+  <si>
+    <t>pou_765e700a7cb58c93</t>
+  </si>
+  <si>
+    <t>pou_7cf0dcc0dcff06b2</t>
+  </si>
+  <si>
+    <t>pou_c9e729f168bf06d0</t>
+  </si>
+  <si>
+    <t>pou_487e6cec70498df8</t>
+  </si>
+  <si>
+    <t>pou_cb504e04d146bb45</t>
+  </si>
+  <si>
+    <t>pou_72237b852a8344a7</t>
+  </si>
+  <si>
+    <t>pou_1b58b05130c7e38c;pou_0aedded10e7bb90c</t>
+  </si>
+  <si>
+    <t>pou_819e3e39071bae23</t>
+  </si>
+  <si>
+    <t>pou_de2a2b64fdc29df7</t>
+  </si>
+  <si>
+    <t>pou_e35051b773cbf291;pou_d3051ae1c25dde96</t>
+  </si>
+  <si>
+    <t>pou_50d11be223c93e5a</t>
+  </si>
+  <si>
+    <t>pou_4199f6a8b0ca1fba</t>
+  </si>
+  <si>
+    <t>pou_4a64bb57fdc6e34d</t>
+  </si>
+  <si>
+    <t>pou_f58895f5bb32e0d2</t>
+  </si>
+  <si>
+    <t>pou_20fedabb474897cd;pou_84a67c7931acb5cb</t>
+  </si>
+  <si>
+    <t>pou_82f450a0643ffd7d;pou_aa97bf28dc071c54</t>
+  </si>
+  <si>
+    <t>pou_b0278210a8bad108</t>
+  </si>
+  <si>
+    <t>pou_4a7a08a7775ba273</t>
+  </si>
+  <si>
+    <t>pou_785fef8738ea5368</t>
+  </si>
+  <si>
+    <t>pou_bad93249d1651cc8;pou_e6fd125b47ad8fbd;pou_176d6e0a77516b8d;pou_d1f2e77a01724b56;pou_0a853bcdfa1aa8e2;pou_1cb655f5bd8def87;pou_895748e63739cc70;pou_52d58d64891a5bc0;pou_2a998686ebc46991</t>
+  </si>
+  <si>
+    <t>pou_7dff4826c9e3a5c6</t>
+  </si>
+  <si>
+    <t>pou_80990ccb204c0b76</t>
+  </si>
+  <si>
+    <t>pou_7ddd015a8aaec4e6</t>
+  </si>
+  <si>
+    <t>pou_60f110d77494741f</t>
+  </si>
+  <si>
+    <t>pou_34986cff0026bd83</t>
+  </si>
+  <si>
+    <t>pou_3f650ed656efb01e</t>
+  </si>
+  <si>
+    <t>pou_b10fe7473d497cc0;pou_562ae979396b949a</t>
+  </si>
+  <si>
+    <t>pou_c204502031440747</t>
+  </si>
+  <si>
+    <t>pou_6af5d4a629997808</t>
+  </si>
+  <si>
+    <t>pou_1500be9ada15ee5c</t>
+  </si>
+  <si>
+    <t>pou_0dcf019e3ea0ca5f;pou_cf73a1a9ecdbbc2d</t>
+  </si>
+  <si>
+    <t>pou_862508291671cea4</t>
+  </si>
+  <si>
+    <t>pou_4f6c9f455d73352b</t>
+  </si>
+  <si>
+    <t>pou_a31a9ecea5a43464</t>
+  </si>
+  <si>
+    <t>pou_88fd224cf173a965</t>
+  </si>
+  <si>
+    <t>pou_16d8f93be1eff9cc</t>
+  </si>
+  <si>
+    <t>pou_d3f566b2dbe31844</t>
+  </si>
+  <si>
+    <t>pou_2b372ed515f1d773;pou_d369af8a57b40ef6</t>
+  </si>
+  <si>
+    <t>pou_8b0c30397f20cc69</t>
+  </si>
+  <si>
+    <t>pou_4c58f4184d367818</t>
+  </si>
+  <si>
+    <t>pou_efb51e5d7fe0e4c0</t>
+  </si>
+  <si>
+    <t>pou_9a1bac13ac15ea35</t>
+  </si>
+  <si>
+    <t>pou_e051501a0df5b114</t>
+  </si>
+  <si>
+    <t>pou_0cab916ab030c2ba</t>
+  </si>
+  <si>
+    <t>pou_265d490606850910</t>
+  </si>
+  <si>
+    <t>pou_d5fe2a3c99eed7b2</t>
+  </si>
+  <si>
+    <t>pou_31a6654672744768</t>
+  </si>
+  <si>
+    <t>pou_0f8177bba67704c1</t>
+  </si>
+  <si>
+    <t>pou_5f86856ec3b4a442</t>
+  </si>
+  <si>
+    <t>pou_21c94d19fbbde275</t>
+  </si>
+  <si>
+    <t>pou_19cf35344af9e1bd</t>
+  </si>
+  <si>
+    <t>pou_fbd745fe9a06a3a1</t>
+  </si>
+  <si>
+    <t>pou_0a194e34665f467c</t>
+  </si>
+  <si>
+    <t>pou_b822ccebc3a60fe2</t>
+  </si>
+  <si>
+    <t>pou_144408adc1908447</t>
+  </si>
+  <si>
+    <t>pou_3b69c12dfc871fc0</t>
+  </si>
+  <si>
+    <t>pou_f5035793cec413c6</t>
+  </si>
+  <si>
+    <t>pou_79f85b5096b8d1ce</t>
+  </si>
+  <si>
+    <t>pou_58a3c4e95da1fab9</t>
+  </si>
+  <si>
+    <t>pou_a0e305ad0c9bb7bc</t>
+  </si>
+  <si>
+    <t>pou_15f68679574eb452</t>
+  </si>
+  <si>
+    <t>pou_bc86ccfdb54a261f</t>
+  </si>
+  <si>
+    <t>pou_49a6343040f68517</t>
+  </si>
+  <si>
+    <t>pou_47a83a3f02791c12</t>
+  </si>
+  <si>
+    <t>pou_2c40af0741e7177f</t>
+  </si>
+  <si>
+    <t>pou_a6ebe6a6d36c7643</t>
+  </si>
+  <si>
+    <t>pou_abee8124cb8d05f9</t>
+  </si>
+  <si>
+    <t>pou_24e706d199c46d53</t>
+  </si>
+  <si>
+    <t>pou_dd1489858bf16518</t>
+  </si>
+  <si>
+    <t>pou_62a7b2be171f5bb7</t>
+  </si>
+  <si>
+    <t>pou_52780f0b4eac8a8c</t>
+  </si>
+  <si>
+    <t>pou_87d33827c4558b89</t>
+  </si>
+  <si>
+    <t>pou_f1f7e16a953ed9ad</t>
+  </si>
+  <si>
+    <t>pou_ffd78560ca3a67fd</t>
+  </si>
+  <si>
+    <t>pou_cc170eccee7db1e7</t>
+  </si>
+  <si>
+    <t>pou_655da86841ffdcec</t>
+  </si>
+  <si>
+    <t>pou_84a44aad4b8d36b1</t>
+  </si>
+  <si>
+    <t>pou_2818b8534ea734c2</t>
+  </si>
+  <si>
+    <t>pou_1d9b812b7b84b794</t>
+  </si>
+  <si>
+    <t>pou_f738f37d971168a5</t>
+  </si>
+  <si>
+    <t>pou_7f63b46e80273978</t>
+  </si>
+  <si>
+    <t>pou_74f0967db3dd7262</t>
+  </si>
+  <si>
+    <t>pou_51b6b1f049b19f59</t>
+  </si>
+  <si>
+    <t>pou_b5ac16ca44c39e97</t>
+  </si>
+  <si>
+    <t>pou_cf5e204fba8c7958</t>
+  </si>
+  <si>
+    <t>pou_4d04912b9059d8f3</t>
+  </si>
+  <si>
+    <t>pou_71e10fe2f843ffc8</t>
+  </si>
+  <si>
+    <t>pou_e4a4e4fdf391b3dc</t>
+  </si>
+  <si>
+    <t>pou_1fc1215c694a2f25</t>
+  </si>
+  <si>
+    <t>pou_ec5296f2d229539e</t>
+  </si>
+  <si>
+    <t>pou_91fc8869f78da456</t>
+  </si>
+  <si>
+    <t>pou_dff7d224c7e6185d</t>
+  </si>
+  <si>
+    <t>pou_0112314d382cc9ea</t>
+  </si>
+  <si>
+    <t>pou_e3acb526538a5d6b</t>
+  </si>
+  <si>
+    <t>pou_7c2454d0eb67670e</t>
+  </si>
+  <si>
+    <t>pou_6aba7b287e4b5c8e</t>
+  </si>
+  <si>
+    <t>pou_cbc32964f31ddea8</t>
+  </si>
+  <si>
+    <t>pou_fe85e7692e7e7473</t>
+  </si>
+  <si>
+    <t>pou_1a1fa54f97c88b2e</t>
+  </si>
+  <si>
+    <t>pou_9aefe71654e5f659</t>
+  </si>
+  <si>
+    <t>pou_bf8941da1aa7f051</t>
+  </si>
+  <si>
+    <t>pou_10b3294a24baeb83</t>
+  </si>
+  <si>
+    <t>pou_1b4af9ead74678d3</t>
+  </si>
+  <si>
+    <t>pou_cd87e789b0d58647</t>
+  </si>
+  <si>
+    <t>pou_92534e2f234f544f</t>
+  </si>
+  <si>
+    <t>pou_395d495b9985a891</t>
+  </si>
+  <si>
+    <t>pou_5a942921d4da49ff</t>
+  </si>
+  <si>
+    <t>pou_d2afb1cb32648a79</t>
+  </si>
+  <si>
+    <t>pou_2818576caf5a68d3</t>
+  </si>
+  <si>
+    <t>pou_14a52295dbba80a1</t>
+  </si>
+  <si>
+    <t>pou_6fea36a3935594c8</t>
+  </si>
+  <si>
+    <t>pou_4543dc007dbf1c7d</t>
+  </si>
+  <si>
+    <t>pou_f030a20a70d7a1e5</t>
+  </si>
+  <si>
+    <t>pou_bf8811c4909ead92</t>
+  </si>
+  <si>
+    <t>pou_6f2039ca4ef18916</t>
+  </si>
+  <si>
+    <t>pou_ecdc6c7950c443d2</t>
+  </si>
+  <si>
+    <t>pou_f70182bc312067bc</t>
+  </si>
+  <si>
+    <t>pou_c7707b8065af616d;pou_477af08c3a345325;pou_8392dc5bf58e485b</t>
+  </si>
+  <si>
+    <t>pou_779e5a06c1ac09d7</t>
+  </si>
+  <si>
+    <t>pou_5b0f9e4f5595d763</t>
+  </si>
+  <si>
+    <t>pou_ef9a0f76ce129ff0</t>
+  </si>
+  <si>
+    <t>pou_9690bb159d4b3fc3;pou_fbd24a8e918fc5cc</t>
+  </si>
+  <si>
+    <t>pou_de3b6ac2016cdf33</t>
+  </si>
+  <si>
+    <t>pou_c51a877ac53c0b1e</t>
+  </si>
+  <si>
+    <t>pou_0313c2f1796fa4b0</t>
+  </si>
+  <si>
+    <t>pou_eef34fee886143a8</t>
+  </si>
+  <si>
+    <t>pou_6722b845b053badd</t>
+  </si>
+  <si>
+    <t>pou_d77ca4792149812a</t>
+  </si>
+  <si>
+    <t>pou_405e4963431deaf8</t>
+  </si>
+  <si>
+    <t>pou_1920ae0fde51509d</t>
+  </si>
+  <si>
+    <t>pou_eeb20d0c969788cb</t>
+  </si>
+  <si>
+    <t>pou_92339186efe2a87b</t>
+  </si>
+  <si>
+    <t>pou_1f98c7e353c135ce</t>
+  </si>
+  <si>
+    <t>pou_5f955a33d4f6b3b3</t>
+  </si>
+  <si>
+    <t>pou_0f66a5fc4ed68705</t>
+  </si>
+  <si>
+    <t>pou_329dbb699e51ade9</t>
+  </si>
+  <si>
+    <t>pou_f821696a81dc0da1</t>
+  </si>
+  <si>
+    <t>pou_697ee6e64596197f</t>
+  </si>
+  <si>
+    <t>pou_8537faeb3d8731a1</t>
+  </si>
+  <si>
+    <t>pou_86a2f89f9b7ab52a</t>
+  </si>
+  <si>
+    <t>pou_6f65fcb984c97032</t>
+  </si>
+  <si>
+    <t>pou_e93d8218e2c5dd7f</t>
+  </si>
+  <si>
+    <t>pou_aa837141efef1334;pou_0a18cc7263027953;pou_ce67a4736bd07424;pou_9a63446c64a67d6d;pou_239dacd5c79c97a9;pou_a1abb21bb7e5d6a0;pou_0ddf0b45c32770ca;pou_2619cec6b20446b1;pou_8ba8c6733b91b195;pou_d7ca5d5c27f3f836;pou_b303040acda66160</t>
+  </si>
+  <si>
+    <t>pou_ed86c1bbf5f8fcec</t>
+  </si>
+  <si>
+    <t>pou_6a454fa9d8ff40cd</t>
+  </si>
+  <si>
+    <t>pou_f2957197c881648d;pou_f2aeb5ebf20bd889</t>
+  </si>
+  <si>
+    <t>pou_cb02f006d4dd724e</t>
+  </si>
+  <si>
+    <t>pou_6a5ea162fcc3bcc1</t>
+  </si>
+  <si>
+    <t>pou_cfa3ac2b6f372441</t>
+  </si>
+  <si>
+    <t>pou_8944181fac1f886c</t>
+  </si>
+  <si>
+    <t>pou_bb75faa5559c06f6</t>
+  </si>
+  <si>
+    <t>pou_73ff5caded2cb0b2</t>
+  </si>
+  <si>
+    <t>pou_4c9730a5a15cc48a</t>
+  </si>
+  <si>
+    <t>pou_bb9769e407d093e7</t>
+  </si>
+  <si>
+    <t>pou_70c6fd11914ab085</t>
+  </si>
+  <si>
+    <t>pou_e7b741975a7dc8b0</t>
+  </si>
+  <si>
+    <t>pou_d6d4d1178680014f</t>
+  </si>
+  <si>
+    <t>pou_f3fa02efdf049d96</t>
+  </si>
+  <si>
+    <t>pou_3b57200bc342b8a3</t>
+  </si>
+  <si>
+    <t>pou_3de74af0d2eb7e10</t>
+  </si>
+  <si>
+    <t>pou_87a9f14ab3fb9896</t>
+  </si>
+  <si>
+    <t>pou_05047aa6e52fa26e</t>
+  </si>
+  <si>
+    <t>pou_6b813b02239ab1ef</t>
+  </si>
+  <si>
+    <t>pou_74f1f22d1a36f0dc</t>
+  </si>
+  <si>
+    <t>pou_43ba067534f282b1</t>
+  </si>
+  <si>
+    <t>pou_25f85ce5ab44360a</t>
+  </si>
+  <si>
+    <t>pou_849e62f8c527e39c</t>
+  </si>
+  <si>
+    <t>pou_a5bf0a75115b47b9</t>
+  </si>
+  <si>
+    <t>pou_686de46225c4d38e</t>
+  </si>
+  <si>
+    <t>pou_1712377bcce166f8</t>
+  </si>
+  <si>
+    <t>pou_f32749723b48772f</t>
+  </si>
+  <si>
+    <t>pou_cc8b182fcace7f08</t>
+  </si>
+  <si>
+    <t>pou_7845d096786b2abd</t>
+  </si>
+  <si>
+    <t>pou_74a9f57e3bf96454</t>
+  </si>
+  <si>
+    <t>pou_16ca8bc99be16ed9</t>
+  </si>
+  <si>
+    <t>pou_3c3f07927609242b</t>
+  </si>
+  <si>
+    <t>pou_56e50ba94a1cfb73</t>
+  </si>
+  <si>
+    <t>pou_ac57a6a43b93f557</t>
+  </si>
+  <si>
+    <t>pou_971e0bb096cce679</t>
+  </si>
+  <si>
+    <t>pou_22b83090123edc29</t>
+  </si>
+  <si>
+    <t>pou_b1a6b33071e8fdb3</t>
+  </si>
+  <si>
+    <t>pou_52e0a6b9aa97b16d</t>
+  </si>
+  <si>
+    <t>pou_43da38ceab5166bc</t>
+  </si>
+  <si>
+    <t>pou_073a167ef8f747ad</t>
+  </si>
+  <si>
+    <t>pou_3d2ee8eb4d24b368</t>
+  </si>
+  <si>
+    <t>pou_561b71b5a981c519</t>
+  </si>
+  <si>
+    <t>pou_0150ce123cbe965a</t>
+  </si>
+  <si>
+    <t>pou_e58d280d038ec2df</t>
+  </si>
+  <si>
+    <t>pou_fe5ec05e1dea95d3</t>
+  </si>
+  <si>
+    <t>pou_d142fc3519460808</t>
+  </si>
+  <si>
+    <t>pou_fc49bbe730bd894f</t>
+  </si>
+  <si>
+    <t>pou_d5aa28578e393cdf</t>
+  </si>
+  <si>
+    <t>pou_59667ad7b59c4044</t>
+  </si>
+  <si>
+    <t>pou_cb3777a63a00bd60</t>
+  </si>
+  <si>
+    <t>pou_154a5bda25f4493a</t>
+  </si>
+  <si>
+    <t>pou_75a6d36343539ec3</t>
+  </si>
+  <si>
+    <t>pou_07e880330b7554f9</t>
+  </si>
+  <si>
+    <t>pou_66be6e5912d668b4</t>
+  </si>
+  <si>
+    <t>pou_53da077dd658bcfb</t>
+  </si>
+  <si>
+    <t>pou_2137447295a2be81</t>
+  </si>
+  <si>
+    <t>pou_b574d1a4ddda0533</t>
+  </si>
+  <si>
+    <t>pou_843b5df8e250d350</t>
+  </si>
+  <si>
+    <t>pou_dd14618d6c597a0f</t>
+  </si>
+  <si>
+    <t>pou_fdf361c793a4c3e4</t>
+  </si>
+  <si>
+    <t>pou_f4aba5de2a2fcd31</t>
+  </si>
+  <si>
+    <t>pou_c7aa44982ab40360</t>
+  </si>
+  <si>
+    <t>pou_9a1a3d4fe77b27fc</t>
+  </si>
+  <si>
+    <t>pou_f4179a221087f817</t>
+  </si>
+  <si>
+    <t>pou_5ccaf2debb7a94c5</t>
+  </si>
+  <si>
+    <t>pou_b88f81476c891fad</t>
+  </si>
+  <si>
+    <t>pou_ae52766bafe30a90</t>
+  </si>
+  <si>
+    <t>pou_114f8ede8c933f57</t>
+  </si>
+  <si>
+    <t>pou_00cba3342fe9e34f</t>
+  </si>
+  <si>
+    <t>pou_6eef08560de0e406</t>
+  </si>
+  <si>
+    <t>pou_b1042d7fb9d6f8e7</t>
+  </si>
+  <si>
+    <t>pou_c63873ed607c5d1c</t>
+  </si>
+  <si>
+    <t>pou_c83dca4eb69d8e91</t>
+  </si>
+  <si>
+    <t>pou_ebd028ea4d7ea811</t>
+  </si>
+  <si>
+    <t>pou_c4ec8c3b316c2072</t>
+  </si>
+  <si>
+    <t>pou_7fb570b94b365b5d</t>
+  </si>
+  <si>
+    <t>pou_a366366475bd2653</t>
+  </si>
+  <si>
+    <t>pou_3d955c44c6a915b8</t>
+  </si>
+  <si>
+    <t>pou_4a18c616183ad5d5</t>
+  </si>
+  <si>
+    <t>pou_38d5b35624aec902</t>
+  </si>
+  <si>
+    <t>pou_11a675385304ee25</t>
+  </si>
+  <si>
+    <t>pou_67b83488c022a76e</t>
+  </si>
+  <si>
+    <t>pou_455a79644689ad02</t>
+  </si>
+  <si>
+    <t>pou_046763d415a4a476</t>
+  </si>
+  <si>
+    <t>pou_cf5aace11b77022e</t>
+  </si>
+  <si>
+    <t>pou_6b200e88cf0211eb</t>
+  </si>
+  <si>
+    <t>pou_3f9b82148dd2103f</t>
+  </si>
+  <si>
+    <t>pou_a3e0378591030368</t>
+  </si>
+  <si>
+    <t>pou_cd7dd13b658ff4f4</t>
+  </si>
+  <si>
+    <t>pou_68935d2272d8f9be</t>
+  </si>
+  <si>
+    <t>pou_29196dbdbd085a35</t>
+  </si>
+  <si>
+    <t>pou_b051a3894949fc66</t>
+  </si>
+  <si>
+    <t>pou_7a679e99fc940330</t>
+  </si>
+  <si>
+    <t>pou_f650e32200784ff1</t>
+  </si>
+  <si>
+    <t>pou_36b31baf2cf628bb</t>
+  </si>
+  <si>
+    <t>pou_3df6ce1d91aa13aa</t>
+  </si>
+  <si>
+    <t>pou_8dd24f4945e243f6</t>
+  </si>
+  <si>
+    <t>pou_1ea99420b8bab706</t>
+  </si>
+  <si>
+    <t>pou_a4503d975de40443</t>
+  </si>
+  <si>
+    <t>pou_e74bb4e1d58764ac</t>
+  </si>
+  <si>
+    <t>pou_974241179758b74f</t>
+  </si>
+  <si>
+    <t>pou_aee391289aa7122c</t>
+  </si>
+  <si>
+    <t>pou_4a8c756c142845e0</t>
+  </si>
+  <si>
+    <t>pou_e1f2560173373d7d</t>
+  </si>
+  <si>
+    <t>pou_16daa4902a800a0b</t>
+  </si>
+  <si>
+    <t>pou_8e8363ba6eaf3d5a</t>
+  </si>
+  <si>
+    <t>pou_467f30cb803b5f58</t>
+  </si>
+  <si>
+    <t>pou_4c4649dc43f46991</t>
+  </si>
+  <si>
+    <t>pou_d98d9181b3a5b33e</t>
+  </si>
+  <si>
+    <t>pou_5dea5e10e22023fe</t>
+  </si>
+  <si>
+    <t>pou_04db12da544b6dc6;pou_7fd68457337fa2f6</t>
+  </si>
+  <si>
+    <t>pou_6d537d072e0efda5</t>
+  </si>
+  <si>
+    <t>pou_801cd562d0eabf0e;pou_3909cc494e43fe0d;pou_c2319102ae0ba209;pou_7fcec48644a170d5;pou_731f9e70b480a1be;pou_b192cc1fc5581e8a;pou_196fa71d85c92d5c;pou_48762fb5be00eb2d;pou_b05745f92e200ef5;pou_a2a1af8f570f21b2;pou_10c8149f86496df3;pou_562fdfec5af40066</t>
+  </si>
+  <si>
+    <t>pou_8588c1c2aad55819</t>
+  </si>
+  <si>
+    <t>pou_fb558bfa891cb6a5</t>
+  </si>
+  <si>
+    <t>pou_778e228b91fc4bfb</t>
+  </si>
+  <si>
+    <t>pou_5617401d943cb37b</t>
+  </si>
+  <si>
+    <t>pou_eb7b86fd5a1f43c0</t>
+  </si>
+  <si>
+    <t>pou_987887fed388c35a</t>
+  </si>
+  <si>
+    <t>pou_d927d9c338ebcd7a</t>
+  </si>
+  <si>
+    <t>pou_4d1ed61f6829a2de</t>
+  </si>
+  <si>
+    <t>pou_073eb6bb12d73f7a</t>
+  </si>
+  <si>
+    <t>pou_d47c5682fa765f33</t>
+  </si>
+  <si>
+    <t>pou_aa64d52e481239a1;pou_bf479fe8b63e8b5b</t>
+  </si>
+  <si>
+    <t>pou_8bd6aa82225006c8</t>
+  </si>
+  <si>
+    <t>pou_e2498f1d32428e61</t>
+  </si>
+  <si>
+    <t>pou_0dc4fc63416f2b89</t>
+  </si>
+  <si>
+    <t>pou_586413d8194a6a61</t>
+  </si>
+  <si>
+    <t>pou_4959eb65d7f94f50</t>
+  </si>
+  <si>
+    <t>pou_66b318796271d4c9</t>
+  </si>
+  <si>
+    <t>pou_908d7f1f4d6b066d</t>
+  </si>
+  <si>
+    <t>pou_bf347e0f391992cc</t>
+  </si>
+  <si>
+    <t>pou_23fdfc4061f0efc7</t>
+  </si>
+  <si>
+    <t>pou_39ec7630ade9b494;pou_9d3ed2d710954bb6;pou_a775990bd43dac66;pou_013c6d4f04cd7d9f;pou_df62c585110ed0e1;pou_5f8590665bec52a5;pou_e59332370f72fb50</t>
+  </si>
+  <si>
+    <t>pou_908cf3ab37a69920;pou_df232531b9f1bf8a</t>
+  </si>
+  <si>
+    <t>pou_9724501a98a3842d</t>
+  </si>
+  <si>
+    <t>pou_0038bd3adb32a68c</t>
+  </si>
+  <si>
+    <t>pou_138fd43684ef7492</t>
+  </si>
+  <si>
+    <t>pou_75e6d18db09beeb1</t>
+  </si>
+  <si>
+    <t>pou_61f289bf097a5c7d</t>
+  </si>
+  <si>
+    <t>pou_a4dc4f57eaa1777e</t>
+  </si>
+  <si>
+    <t>pou_b0d67b521e4f34ea</t>
+  </si>
+  <si>
+    <t>pou_172601cb9547af2e</t>
+  </si>
+  <si>
+    <t>pou_e8003dd4a4a96ded</t>
+  </si>
+  <si>
+    <t>pou_13d78b92ff9c0773</t>
+  </si>
+  <si>
+    <t>pou_8a4c41e0ec6fe020</t>
+  </si>
+  <si>
+    <t>pou_3cd8dbc2ab2680ba;pou_1bdd083947213d45;pou_f8eab749094cf604;pou_117763b7589d7e15;pou_40d5896bf462e98f;pou_a10ea5a67131907b;pou_8cf80b5737791fb2;pou_f7211257452b71e6;pou_b8c210072dd2b93a</t>
+  </si>
+  <si>
+    <t>pou_9d8d7db69ba19ffb;pou_76b858c851b47633;pou_bfe6c10e15fec09d;pou_37765f05b20ca95e;pou_5d36924e6989304f;pou_b82abb9c2590b05e;pou_3aca296a14711507</t>
+  </si>
+  <si>
+    <t>pou_6c1f6f02fd1b3a8c</t>
+  </si>
+  <si>
+    <t>pou_562e90f88ede464c;pou_db5329b0035c54be;pou_2359ac4ceb6c22b7;pou_9271ccf921f0c35a</t>
+  </si>
+  <si>
+    <t>pou_cb157a774ea5dfb8;pou_8c9623b714c7d1c1;pou_11c5c0307296dc84;pou_9cc58a5da407d76e;pou_03f24202ca48db06;pou_00d0ba6f125078cf;pou_0b1aab0c1500c180;pou_780402c4cf5199c4;pou_d012a859dbeb50a4;pou_4a6f71d3ab3e6346</t>
+  </si>
+  <si>
+    <t>pou_3f0824a2a9ed4306</t>
+  </si>
+  <si>
+    <t>pou_203ce97094530a84;pou_5c0cc6504629095b;pou_30e832f5ececdfd7;pou_18932a1efe8b69e6;pou_9fdcf5ad49262012;pou_128002d344739315;pou_9a5889b2d43f593d;pou_edccc0cfd18903ac;pou_98c63f7b4670a986;pou_f53ed94da606dce1;pou_002917a1d1d08084;pou_f3fc03c90f01a25e;pou_51efa72aed0a02c8;pou_48dd3ea9b530983a;pou_2d7773ba6051c53d;pou_72ca88ceebb3b354;pou_c27477be67521174;pou_9d09e3e6f7ea2aa5;pou_2d63f3baf64ab3e4;pou_f2ac51d0f7c2e755;pou_557a38c025d39ccf;pou_e7372217d819302d;pou_779f73ee5780bf4b;pou_118f661983ccca87;pou_0f12d0795c66f6e6;pou_1b44cf3d3d04889f;pou_d55bb7fae82b4f94;pou_82bf4dcabe2cd68f;pou_f7395fba53db7444;pou_997bd8d4b26642fc;pou_5f9ba7ccfc77f2dc;pou_41b95fdf44be5881;pou_0a0509255342947e;pou_89b26c33f2652739;pou_853ce4fccdcc9abe;pou_7b75fcbcb660a61e;pou_79411a128cffbcf7;pou_251b24c50695c469;pou_7d6d40d880790d84;pou_2dfec0797c7bf759;pou_96c9dcceeaec992a;pou_3d2ebcb5c4649499;pou_87c6ef52f176192c;pou_9fad0092ba9fbcdc;pou_59fb8823e9943e1a;pou_fccd43ebe981dfe5;pou_e9335366b2d98d3f;pou_18c61145ee05df15;pou_ee50c02a1776cb41;pou_2aa3cd4570c6cd85;pou_7097a41671c2ee6b;pou_653acb07ccb60f01;pou_771f060af560a3e3;pou_8bce3075ea547d6b;pou_6d2701e211624420;pou_58f28425751e3836;pou_6738adab46447edd;pou_b2c86787bbcba84d;pou_e674cdccac4914ca;pou_dddfb6b9c76751a9;pou_b23a38d0608474fb;pou_e3263ff6194b4b92;pou_2abbeab46edbf26f;pou_52a09d1bf3448e2b;pou_5a05bdd6af081695;pou_981ad4764e702e38;pou_c50720b29350fa8d;pou_7bf78f7f02cddbbd;pou_b6c67198323039fb;pou_bc06cb463b2c4eda;pou_1965c7dca07201d4;pou_d6366727d319c7aa;pou_547e17edf2fa72d5;pou_b34cf7262be1edb6;pou_ddd698a3fe3d8cd3;pou_ef020bda2f88c4d9;pou_2b603e002fffc8f8;pou_d8aa8c74ed49be66;pou_8b59b3e4f80a4971;pou_422eeeb4a7bca294;pou_2246a552d0633580;pou_8214893ab78ed76a;pou_fc17f9b0bc26d696;pou_6e6ec6176098731b;pou_4d63dca2ed9f43c0;pou_fb4d7131d342880d;pou_6b3431c298075427;pou_53d9b17842720fea;pou_d892141d1263f6e7;pou_092cdc62424f3db3;pou_4b0066ae42f9d9de;pou_484f6ffdfd644a65;pou_527252d91cbfe467;pou_e00f3d66aaf2f898;pou_e5350e54a159ff36;pou_7134fd1eb39eb39e;pou_23f3bfd1d4c831a0;pou_e48d417cb0c63e87;pou_8745fad5bdf3f009;pou_c6f6c78205f1e036;pou_c4c64a7f9cf34ff2;pou_f4d8d3b3a8c7fa2a;pou_1f5eb9fa3dadbc60;pou_83dc98b959a7bb4c;pou_0f20e1be57bda47a;pou_a1cb7941ff5d5318;pou_f272d802304e23a0;pou_e746f07faab140de;pou_4ce9dd66723ab0b3;pou_fd467a2dfef8370e;pou_1005dd4c7015c636;pou_8aeeaa21ccf98260;pou_67b35e3c1fc11d63;pou_25cf0359a56ec4e8;pou_b6f73e104f16f77b;pou_db077a5f890600d6;pou_4d8968ac60748af2;pou_aa288505b1ba7c63;pou_f124d88414fab81d;pou_fee9f1f1614b59e2;pou_913288831784a056;pou_6e4eacc5dbe4a433;pou_0f4609dffce63767;pou_e2be45d8ce207d4f;pou_c2869b2587a69bff;pou_0fd694a684cfe6e7;pou_12977a215cc066ff;pou_e152ddfafcabea1d;pou_4b49db0ec56afb15;pou_4d1a8488b80469ab;pou_71f99dbddfc11b7e;pou_8087217341198e92;pou_7a2d632f4f9df88d;pou_a448f84f201c436d;pou_059c60d37d2d68dd;pou_e5ecb29bf843d246;pou_c9cd3ecebaf5d6b6;pou_7476613d0c3eb3ef;pou_58029c319309e55a;pou_1d6d6d0ee5f31ea9;pou_e078932e206ec47f;pou_752b8ab5d0b0a752;pou_8fb68ed801107304</t>
+  </si>
+  <si>
+    <t>pou_aeb1c6eff074b7d0;pou_551fb67914a41b7a;pou_d5ff08debad6277b</t>
+  </si>
+  <si>
+    <t>pou_8881783ceff64f84</t>
+  </si>
+  <si>
+    <t>pou_a28667df33b83668</t>
+  </si>
+  <si>
+    <t>pou_6bdf6df67d81b837</t>
+  </si>
+  <si>
+    <t>pou_0b1f7cc89179154a</t>
+  </si>
+  <si>
+    <t>pou_cb6a453c71cdb858</t>
+  </si>
+  <si>
+    <t>pou_a218cc489c4e6126;pou_3448d1e179907adc;pou_6e53dfd31053b0cb</t>
+  </si>
+  <si>
+    <t>pou_5f59c2ae54bd04b5</t>
+  </si>
+  <si>
+    <t>pou_8e1e8c3605525e21</t>
+  </si>
+  <si>
+    <t>pou_7555c5f58deb2c75</t>
+  </si>
+  <si>
+    <t>pou_f2eeafb67d9569d7</t>
+  </si>
+  <si>
+    <t>pou_94fd3bbdacf72aa7</t>
+  </si>
+  <si>
+    <t>pou_2b16e15a71ef25d4;pou_b9b79b8e340edadb;pou_431cea328e63d8f0;pou_1f680f5eb1db889e;pou_9a5b5ee84c161ead;pou_558374b82593adf1;pou_9785e57b001dbe9f</t>
+  </si>
+  <si>
+    <t>pou_fbd025fb9bf06b1c</t>
+  </si>
+  <si>
+    <t>pou_f6d7234ccec48776</t>
+  </si>
+  <si>
+    <t>pou_fc246c2cf2150707;pou_79fdc720de0e08db</t>
+  </si>
+  <si>
+    <t>pou_5842c10b8f6379a6</t>
+  </si>
+  <si>
+    <t>pou_e77dcf71f3f3f049</t>
+  </si>
+  <si>
+    <t>pou_15d17c9d71cf45dc</t>
+  </si>
+  <si>
+    <t>pou_4b92ea24af733dcb</t>
+  </si>
+  <si>
+    <t>pou_31e61560b73ae2f4</t>
+  </si>
+  <si>
+    <t>pou_734ae2fd3c9433c1;pou_9f7e2e2fa98b42ee</t>
+  </si>
+  <si>
+    <t>pou_ccad5b2d906a9064;pou_6a9cdd134211e3de</t>
+  </si>
+  <si>
+    <t>pou_749cb14848753884;pou_ae04a26a3149a4fa;pou_0103ae86f43ba6e6;pou_f0b938b8b6e0df98;pou_2b4d52666a7b6a44;pou_f93d61ece0ee9948;pou_ff14bfbfd5eca9ed;pou_125456b330d4356e;pou_ed2dc52cae59f5e0;pou_044bab3fc80c4637;pou_3372abbbe1be8d93;pou_5b58d06dd5d3c983;pou_d85f4314cdb9d93f;pou_0dc3488928ed344f;pou_04d8abee47cb44b3;pou_c877384f9c69f463;pou_e1a8637aae761de9;pou_7fa536367cfba93d;pou_8bbb8cbfd36f2632;pou_d8fc1307dcc8f156;pou_256e45014c556ce0;pou_c27a1dcef952851b;pou_1d963320390dd824;pou_ff640adc0aed571f;pou_181fc3e477844019;pou_d126119f7996ae48;pou_c648b2516ecb55aa</t>
+  </si>
+  <si>
+    <t>pou_d7775bc2c9438153</t>
+  </si>
+  <si>
+    <t>pou_44346626f751308c</t>
+  </si>
+  <si>
+    <t>pou_0a64de45d0ce61f2;pou_54ae2ffd32322b6e;pou_a8989fbc50c3a5eb;pou_694ef8e27a7cfc1c;pou_a36619f2d96353e0</t>
+  </si>
+  <si>
+    <t>pou_cc283f4aefc8043a;pou_908d46a2aac8f00f;pou_4822e0fa97b7220d;pou_1b252939b21d5f8b;pou_72dc882a2b424e9a;pou_0222416077a863b9;pou_ed6d6fd48864df02;pou_00803fd7abb67c39;pou_33b838680eda9c0a;pou_1e6a0f6ad74fa11c;pou_2ea527af806e6796;pou_3f451231c038bab1;pou_2800c4e402da8db2;pou_a37cf0ba49ad86d3;pou_ed8debccbbd7499a;pou_57638688cd4313ed;pou_30b6a060349f5faa;pou_11ebcac331340053;pou_f6d9c6c8182b6d78;pou_21335eab4b53a891;pou_b6e9db055b9bfbdb;pou_38fcf3f4ec4035c8;pou_b4757c3806c87038;pou_5868e61c62622fb0;pou_813f838aada3c7f9;pou_7dd0a09c23c53e29;pou_66da02c5b19c14ae;pou_0499c31ba21d70c9;pou_65458ae5ac9134c3</t>
+  </si>
+  <si>
+    <t>pou_600fe708341a5fcc;pou_74d7f1395693e158;pou_165495ef7e261c8d;pou_58225ac4c6d5fedf;pou_8b3bde985db3df82;pou_6c493f06fa48301f;pou_ba45504604be47dd;pou_f362c5e585ea88ef</t>
+  </si>
+  <si>
+    <t>pou_d7b20257938c4a74;pou_ef79e99f35eff48b</t>
+  </si>
+  <si>
+    <t>pou_f5c5d5684e8a1049</t>
+  </si>
+  <si>
+    <t>pou_6b79cf55ad976ca4</t>
+  </si>
+  <si>
+    <t>pou_09ddf320d89bab08;pou_3ceee7d4af237058;pou_628054d93050bb18;pou_4e8ab60938d3a9c5;pou_e2957a69972a85af;pou_842da25000bc5b12;pou_5e55b0b43a644f0d;pou_7ad272778ccb21b3;pou_4c09cc6cc15dce6d;pou_a8501d779b6b1eac;pou_59bb585d2e177ae0;pou_06020b09d15de52b;pou_f7c5abe2d38a9c51;pou_480dc586fe6772e2;pou_680f47fe4023e542</t>
+  </si>
+  <si>
+    <t>pou_7673c52a16da50cc;pou_b77c5990fe502323;pou_b2e0e6be2d4bdf92;pou_ac30cac9a1cef783;pou_aac89e965fb32109;pou_a33809f858acd3a1;pou_695f3b9d0c04ecc1</t>
+  </si>
+  <si>
+    <t>pou_0810390d80aee091</t>
+  </si>
+  <si>
+    <t>pou_e8616dc87dc82260</t>
+  </si>
+  <si>
+    <t>pou_ebab02b8fce59010</t>
+  </si>
+  <si>
+    <t>pou_601062fede32256c</t>
+  </si>
+  <si>
+    <t>pou_f38e1a9c78c3a499</t>
+  </si>
+  <si>
+    <t>pou_84adf824466951ca</t>
+  </si>
+  <si>
+    <t>pou_d2aefeda3e5500b1</t>
+  </si>
+  <si>
+    <t>pou_38c81e1462d22bc4</t>
+  </si>
+  <si>
+    <t>pou_c82fba091921d30a</t>
+  </si>
+  <si>
+    <t>pou_d314943c4c339068;pou_10154012bd75b388;pou_506605150344b89a;pou_57547c11ce67ee69;pou_0219036040f3aba5;pou_fd6e7c2119fee665;pou_4d87f953178e2897;pou_7dd99c2bb5f5d2cd;pou_ada449ad3602b914;pou_c966e422f6b6416e;pou_7d068e2c75b7e842;pou_b339c80d353d7d91</t>
+  </si>
+  <si>
+    <t>pou_2ced702e179143b1</t>
+  </si>
+  <si>
+    <t>pou_35df497d79454890;pou_057677379ff72266</t>
+  </si>
+  <si>
+    <t>pou_14259b07ad5d4dc5;pou_bd5c9fb732af6ce4;pou_8ffaa959f3aa08fe;pou_be2b6bad72537c17;pou_d776fe1a1ff284a3;pou_a5d4481b5412ab66</t>
+  </si>
+  <si>
+    <t>pou_7487545c4ae59851;pou_649989a8181f3965;pou_63242545fcdd7897;pou_9729433f0078cd20;pou_cb32068eb9cdd749;pou_d5e462bf864f6287;pou_0d60263f63038401;pou_bfd280537ee858ca;pou_79f80f7afc0880c5;pou_6ccab4b9ce6f49bc;pou_831e9675308f3cb7;pou_2073e7305bb300dd;pou_c33710455307049e;pou_56a88e255bfd794a</t>
+  </si>
+  <si>
+    <t>pou_eacce84a36e430b6;pou_ee65ea7c737f65c0;pou_adf466ffa7e38fda;pou_595e92e8702321e7;pou_8dab83dc94f5b15f;pou_d3d02e809012ef2f;pou_6cc46cc593dfa2bf;pou_a2e140fc0261e71e;pou_8f98451da7e56290;pou_a2004fb944b943c5;pou_ed3d8e47baf5fd25</t>
+  </si>
+  <si>
+    <t>pou_4baa63e96288301d</t>
+  </si>
+  <si>
+    <t>pou_f6d7344d86714319</t>
+  </si>
+  <si>
+    <t>pou_8add2766b19ccf6f;pou_cee8de73753439fa;pou_16c55e7b8f9bb9ce;pou_d42e78edc3951184;pou_17b7e9d1897dd566;pou_26ff45ff9d0e4230;pou_c3ae4db3638af469</t>
+  </si>
+  <si>
+    <t>pou_6ae3cb9c2e201eb0;pou_bf0e08425544037a;pou_c1ef40ddf2daea5e;pou_864262fb260431ea;pou_979c17e6a6bd49cb;pou_603b00466d018f00;pou_342c85792a2979d6;pou_f6057685cfad979e;pou_f9d960ad78f5286b;pou_c57591eb5064222e;pou_d4433f80e27f8d62;pou_8b51f2ec6fbace2d;pou_70dcf124bb152b52;pou_b93587f8248df49f;pou_e84942edd5254708;pou_b82dc271428bee2a;pou_6552ec9def74f271;pou_d6b64d23ebc80aa4;pou_83274bd1dea2e75c</t>
+  </si>
+  <si>
+    <t>pou_97dec22f9f675823</t>
+  </si>
+  <si>
+    <t>pou_d60838f3bd158b59;pou_fcffffc76b769bfb;pou_4c71610676cac77e;pou_403402198d821a14;pou_5339f34ac2892d00;pou_edb7a20e01968056</t>
+  </si>
+  <si>
+    <t>pou_73e9fa3064427559</t>
+  </si>
+  <si>
+    <t>pou_7fa0db0e4d1cc310;pou_f772986c518f10c6;pou_65ecc94353c3811b</t>
+  </si>
+  <si>
+    <t>pou_67286d81fca90720</t>
+  </si>
+  <si>
+    <t>pou_d451aca89fce0e7f;pou_7c4555ebed1e1082;pou_5663573890f9a683;pou_476357fbdf56292d;pou_6a306488983acf4f;pou_9b82f40cc11a8d3d</t>
+  </si>
+  <si>
+    <t>pou_697006ecd0ba19c0</t>
+  </si>
+  <si>
+    <t>pou_2d1a7cbc48336455</t>
+  </si>
+  <si>
+    <t>pou_afc5a7bb41e42459</t>
+  </si>
+  <si>
+    <t>pou_6f594ba5fcc95783;pou_5c0306c1415ff1e6;pou_556c7e608d20f187;pou_20f2c1790f348e8b;pou_2e72ac942df676e5;pou_eeaaae9d390da4eb;pou_3e8a1b6cb378a374;pou_f08d2f60be939fc6;pou_21e5af715f8d6720;pou_eb79b13553cb5954;pou_eb0a994a47dd48f1;pou_a908e69052b46dcf;pou_02036320d4e44a9f;pou_ee5ab7526d24ebe0;pou_86c7856e1b1d21d3;pou_16556cf2493e0285;pou_064aa6151cc948ab;pou_dfb9d19ea77898f6;pou_c749815e9fff2b0f;pou_73e1094cdd818d94;pou_e3fae77eb0e2c562</t>
+  </si>
+  <si>
+    <t>pou_ee623079ace280fa</t>
+  </si>
+  <si>
+    <t>pou_081c0a0f01ac70c0</t>
+  </si>
+  <si>
+    <t>pou_8e017d81fd5e883d</t>
+  </si>
+  <si>
+    <t>pou_84ae02c8b6546f0d;pou_8c9fe83a892e8f8d;pou_472f1936c783f51e;pou_a359c278653f595e;pou_b0613ec50ef7d4be;pou_e3dcb16fbd288f99;pou_b7006bec7c5cd1f5;pou_03a0a918835743d8;pou_1067a99e18013f45;pou_7d2d5ef6e7222c7e;pou_25e3e5f430e18ed5;pou_95436972a3ca7e1a;pou_833d351c19387f17;pou_7c216cb350239d55;pou_79337ad18e9e03d3</t>
+  </si>
+  <si>
+    <t>pou_24e716efdfde9994</t>
+  </si>
+  <si>
+    <t>pou_064c8aa60128a441</t>
+  </si>
+  <si>
+    <t>pou_4fb3cb79eb6de751</t>
+  </si>
+  <si>
+    <t>pou_d4f314eb496f7dc1</t>
+  </si>
+  <si>
+    <t>pou_2235074ffc69238c</t>
+  </si>
+  <si>
+    <t>pou_40e585edd34c9a93</t>
+  </si>
+  <si>
+    <t>pou_a0a6af13de41309c</t>
+  </si>
+  <si>
+    <t>pou_ffd85f8c46993107</t>
+  </si>
+  <si>
+    <t>pou_54734434aa93d821</t>
+  </si>
+  <si>
+    <t>pou_73ea8374b1b10094</t>
+  </si>
+  <si>
+    <t>pou_b335b37aae1dd47c</t>
+  </si>
+  <si>
+    <t>pou_535ac26de24f6e10;pou_d5e5edbe05587534</t>
+  </si>
+  <si>
+    <t>pou_55535ab3bda8ea0b</t>
+  </si>
+  <si>
+    <t>pou_383bf688c726a783</t>
+  </si>
+  <si>
+    <t>pou_f19b176af82a5ec5</t>
+  </si>
+  <si>
+    <t>pou_a91ae63c6df89b5c</t>
+  </si>
+  <si>
+    <t>pou_cd3ca4926a73b4bb</t>
+  </si>
+  <si>
+    <t>pou_6b632048561444a2</t>
+  </si>
+  <si>
+    <t>pou_a0a4b062ab16ba62</t>
+  </si>
+  <si>
+    <t>pou_6ce350bedd6549af</t>
+  </si>
+  <si>
+    <t>pou_327fad70f4543816</t>
+  </si>
+  <si>
+    <t>pou_722dac701ddbf7fc</t>
+  </si>
+  <si>
+    <t>pou_9f8ab68c5f2a78a9</t>
+  </si>
+  <si>
+    <t>pou_16a5f24fd943b6f1</t>
+  </si>
+  <si>
+    <t>pou_c1b8ef291beb17e7</t>
+  </si>
+  <si>
+    <t>pou_a1a282f7969c6a3e</t>
+  </si>
+  <si>
+    <t>pou_2d11a2388d87f16c</t>
+  </si>
+  <si>
+    <t>pou_12acf62c49faaa16</t>
+  </si>
+  <si>
+    <t>pou_45247081d45286bc</t>
+  </si>
+  <si>
+    <t>pou_2003440b294873c7</t>
+  </si>
+  <si>
+    <t>pou_9aa613a8c07f0160</t>
+  </si>
+  <si>
+    <t>pou_5bba38835f92ecb9</t>
+  </si>
+  <si>
+    <t>pou_0e826f899116327e</t>
+  </si>
+  <si>
+    <t>pou_86f3fbe45aa82072</t>
+  </si>
+  <si>
+    <t>pou_61c307c1d057d216</t>
+  </si>
+  <si>
+    <t>pou_f4bbf77dac4cd932</t>
+  </si>
+  <si>
+    <t>pou_eeca78f8c76c86bf</t>
+  </si>
+  <si>
+    <t>pou_a026ab17fdc7d074</t>
+  </si>
+  <si>
+    <t>pou_c8089936d6c69e1f</t>
+  </si>
+  <si>
+    <t>pou_665dbd91965a48d5</t>
+  </si>
+  <si>
+    <t>pou_4e5b97d92c55c81a</t>
+  </si>
+  <si>
+    <t>pou_7b4913b8ae5ec5ae</t>
+  </si>
+  <si>
+    <t>pou_301540bf5cd7edd8</t>
+  </si>
+  <si>
+    <t>pou_38bcaa323ff92b76</t>
+  </si>
+  <si>
+    <t>pou_9cb9758f1d5b50ff</t>
+  </si>
+  <si>
+    <t>pou_d0e5630c473010f1</t>
+  </si>
+  <si>
+    <t>pou_89466f438c9920b5</t>
+  </si>
+  <si>
+    <t>pou_3d3a3a49d9128558</t>
+  </si>
+  <si>
+    <t>pou_823091a75fea49b7</t>
+  </si>
+  <si>
+    <t>pou_6bf5b435ed610152</t>
+  </si>
+  <si>
+    <t>pou_669075a818ec4676</t>
+  </si>
+  <si>
+    <t>pou_6c5be9b0682f55e1</t>
+  </si>
+  <si>
+    <t>pou_e2b57b4272aad742</t>
+  </si>
+  <si>
+    <t>pou_2c8769d2635ba93d</t>
+  </si>
+  <si>
+    <t>pou_0e30504003939297</t>
+  </si>
+  <si>
+    <t>pou_3143c0c3a397f191</t>
+  </si>
+  <si>
+    <t>pou_f3037f790c6c0d89</t>
+  </si>
+  <si>
+    <t>pou_ead37dc17bc5169b</t>
+  </si>
+  <si>
+    <t>pou_c96484dcea0e50b2</t>
+  </si>
+  <si>
+    <t>pou_970bda730a6c465a</t>
+  </si>
+  <si>
+    <t>pou_ce601b1c4eceacb3</t>
+  </si>
+  <si>
+    <t>pou_4adbc5f06bb33ba0</t>
+  </si>
+  <si>
+    <t>pou_bdd2a2a56a91030f</t>
+  </si>
+  <si>
+    <t>pou_74ada83b5d64eedb</t>
+  </si>
+  <si>
+    <t>pou_355846d03d7fbdee</t>
+  </si>
+  <si>
+    <t>pou_f3835ec5ae3d8b9e</t>
+  </si>
+  <si>
+    <t>pou_7adb807584214a84</t>
+  </si>
+  <si>
+    <t>pou_954d6787012e0c23</t>
+  </si>
+  <si>
+    <t>pou_06fdf17a1cc89209</t>
+  </si>
+  <si>
+    <t>pou_672fcac1488aaead</t>
+  </si>
+  <si>
+    <t>pou_da145d46687e83bb</t>
+  </si>
+  <si>
+    <t>pou_603ad67f5880c201</t>
+  </si>
+  <si>
+    <t>pou_cd21e97c0757dc2f</t>
+  </si>
+  <si>
+    <t>pou_989fb59ce73b7a74</t>
+  </si>
+  <si>
+    <t>pou_033803f795c8bc31</t>
+  </si>
+  <si>
+    <t>pou_1d123897a2c13fa9</t>
+  </si>
+  <si>
+    <t>pou_3c7e21fa6135e1dc</t>
+  </si>
+  <si>
+    <t>pou_4e6c5663164bd941</t>
+  </si>
+  <si>
+    <t>pou_efa012e0e9f82add</t>
+  </si>
+  <si>
+    <t>pou_5c12e8e3b1e83d86</t>
+  </si>
+  <si>
+    <t>pou_a90a9014fcab9e5c</t>
+  </si>
+  <si>
+    <t>pou_1637a15b3bc62b63</t>
+  </si>
+  <si>
+    <t>pou_ae88515d2b8e73ec</t>
+  </si>
+  <si>
+    <t>pou_81be645a70d9e29d</t>
+  </si>
+  <si>
+    <t>pou_9bc93f2efbcf61a5</t>
+  </si>
+  <si>
+    <t>pou_34539d1a17ec097c</t>
+  </si>
+  <si>
+    <t>pou_1dcbf12173c2b3ee</t>
+  </si>
+  <si>
+    <t>pou_e4e3384af0899295</t>
+  </si>
+  <si>
+    <t>pou_958a78544433f417</t>
+  </si>
+  <si>
+    <t>pou_09a16082f74ba230</t>
+  </si>
+  <si>
+    <t>pou_4dafd4188d0c1b88</t>
+  </si>
+  <si>
+    <t>pou_7a62a993414fd31f</t>
+  </si>
+  <si>
+    <t>pou_c73573fad0565018</t>
+  </si>
+  <si>
+    <t>pou_7e4107180f197925</t>
+  </si>
+  <si>
+    <t>pou_1d1be9a94d6909e0</t>
+  </si>
+  <si>
+    <t>pou_77754dd253625977</t>
+  </si>
+  <si>
+    <t>pou_3bf2dfd8022e448a</t>
+  </si>
+  <si>
+    <t>pou_0e562475ef6e1356</t>
+  </si>
+  <si>
+    <t>pou_2e6d5d66c6cf62bd</t>
+  </si>
+  <si>
+    <t>pou_e02213b84d66180f</t>
+  </si>
+  <si>
+    <t>pou_8cc376a4602713d8</t>
+  </si>
+  <si>
+    <t>pou_207c7df1f0aedb68</t>
+  </si>
+  <si>
+    <t>pou_cbc601fb70554844</t>
+  </si>
+  <si>
+    <t>pou_921ad6ce0dc50b2f</t>
+  </si>
+  <si>
+    <t>pou_ca1153f059ef3d71</t>
+  </si>
+  <si>
+    <t>pou_3197b85270b85912</t>
+  </si>
+  <si>
+    <t>pou_cbac6ce825a1bd1b</t>
+  </si>
+  <si>
+    <t>pou_c31cbdf9746eb358</t>
+  </si>
+  <si>
+    <t>pou_a2f24919928ee939</t>
+  </si>
+  <si>
+    <t>pou_03eb5012adcfd427</t>
+  </si>
+  <si>
+    <t>pou_b0f283cf287a1499</t>
+  </si>
+  <si>
+    <t>pou_8eec9d5050ced4d6</t>
+  </si>
+  <si>
+    <t>pou_536e08500bebadbb</t>
+  </si>
+  <si>
+    <t>pou_df177aa8b7b446f0</t>
+  </si>
+  <si>
+    <t>pou_25f167edac2145b3</t>
+  </si>
+  <si>
+    <t>pou_1d16dfd8744cd86c</t>
+  </si>
+  <si>
+    <t>pou_511220b52313d6a8</t>
+  </si>
+  <si>
+    <t>pou_35727d2c48a05c15</t>
+  </si>
+  <si>
+    <t>pou_d691a85a0999abcd</t>
+  </si>
+  <si>
+    <t>pou_946b97dc22f10f3f</t>
+  </si>
+  <si>
+    <t>pou_b8a28ebb1e8d21ec</t>
+  </si>
+  <si>
+    <t>pou_de88fcb296cce312</t>
+  </si>
+  <si>
+    <t>pou_a23bddcb220e1c33</t>
+  </si>
+  <si>
+    <t>pou_b7c6ac9a6c05ad3b</t>
+  </si>
+  <si>
+    <t>pou_9def49c8614ed8c5</t>
+  </si>
+  <si>
+    <t>pou_bbb990154c3761d1</t>
+  </si>
+  <si>
+    <t>pou_841d57cbcc37a5af</t>
+  </si>
+  <si>
+    <t>pou_8a0683511a03bbbf</t>
+  </si>
+  <si>
+    <t>pou_b4d9fae459c72a29</t>
+  </si>
+  <si>
+    <t>pou_f4b56fa089919ad4</t>
+  </si>
+  <si>
+    <t>pou_3532ad529cbdc673</t>
+  </si>
+  <si>
+    <t>pou_20c23c3a27326ee1</t>
+  </si>
+  <si>
+    <t>pou_8db590909f5796e9</t>
+  </si>
+  <si>
+    <t>pou_8224a4519db5e3cb</t>
+  </si>
+  <si>
+    <t>pou_635e19a73e0c12ec</t>
+  </si>
+  <si>
+    <t>pou_925e4f303b32684f</t>
+  </si>
+  <si>
+    <t>pou_6b722ba0075450d9</t>
+  </si>
+  <si>
+    <t>pou_7616fe7a85051c9b</t>
+  </si>
+  <si>
+    <t>pou_1b5953caa24c4807</t>
+  </si>
+  <si>
+    <t>pou_f1488ebf54ec3a2a</t>
+  </si>
+  <si>
+    <t>pou_57c6d031fecb03b0</t>
+  </si>
+  <si>
+    <t>pou_6d000fd9391f8973</t>
+  </si>
+  <si>
+    <t>pou_ed7ff7eebc64cdc2</t>
+  </si>
+  <si>
+    <t>pou_90f17567594eb5cc</t>
+  </si>
+  <si>
+    <t>pou_e6db2b464b8e8626</t>
+  </si>
+  <si>
+    <t>pou_68a57c5756da012a</t>
+  </si>
+  <si>
+    <t>pou_ebb689f4d26a6b93</t>
+  </si>
+  <si>
+    <t>pou_0f035799ee1d050f</t>
+  </si>
+  <si>
+    <t>pou_2509f4380491580b</t>
+  </si>
+  <si>
+    <t>pou_a2c2675e91146c11</t>
+  </si>
+  <si>
+    <t>pou_e49e56daa77c1ee5</t>
+  </si>
+  <si>
+    <t>pou_edc27185e6f665d2</t>
+  </si>
+  <si>
+    <t>pou_10beca5d5ebeaee1</t>
+  </si>
+  <si>
+    <t>pou_89fa0c45e3bea2e5</t>
+  </si>
+  <si>
+    <t>pou_90d4b167a2a7a4c0</t>
+  </si>
+  <si>
+    <t>pou_78fe266bc4eed8d0</t>
+  </si>
+  <si>
+    <t>pou_c9c14c39d95cfb54</t>
+  </si>
+  <si>
+    <t>pou_4ecbbfc7809091ea</t>
+  </si>
+  <si>
+    <t>pou_116e7ef824e1b6d6</t>
+  </si>
+  <si>
+    <t>pou_9a916f0874821c59</t>
+  </si>
+  <si>
+    <t>pou_4a2c4810798b7bf7</t>
+  </si>
+  <si>
+    <t>pou_c326b2543fed429d</t>
+  </si>
+  <si>
+    <t>pou_fd3a1a41a62858dc</t>
+  </si>
+  <si>
+    <t>pou_93071af4931f866e</t>
+  </si>
+  <si>
+    <t>pou_deb5bc884ebebf1b</t>
+  </si>
+  <si>
+    <t>pou_aac0519deecec394</t>
+  </si>
+  <si>
+    <t>pou_d2afa77c0634190c</t>
+  </si>
+  <si>
+    <t>pou_1dcff6d1ab7747df</t>
+  </si>
+  <si>
+    <t>pou_482610552a57c2ce</t>
+  </si>
+  <si>
+    <t>pou_4da66e4904439e36</t>
+  </si>
+  <si>
+    <t>pou_60a224dfb07a82cf</t>
+  </si>
+  <si>
+    <t>pou_da281bea2033ca0f</t>
+  </si>
+  <si>
+    <t>pou_8f1b02c6e6404056</t>
+  </si>
+  <si>
+    <t>pou_9f76321cf122271a</t>
+  </si>
+  <si>
+    <t>pou_d03462b41bffd4ee</t>
+  </si>
+  <si>
+    <t>pou_f5e9a8a1f57a82e7</t>
+  </si>
+  <si>
+    <t>pou_4b3ce89036f90bf2</t>
+  </si>
+  <si>
+    <t>pou_dee9b3a72d8e2967</t>
+  </si>
+  <si>
+    <t>pou_1e9c1e452600ceaf</t>
+  </si>
+  <si>
+    <t>pou_c2b1e9f6a4615920</t>
+  </si>
+  <si>
+    <t>pou_8d9d3cf789c4bb75</t>
+  </si>
+  <si>
+    <t>pou_5aaca2e45d350afc</t>
+  </si>
+  <si>
+    <t>pou_e962b638005fc026</t>
+  </si>
+  <si>
+    <t>pou_e3d262cc0b2da410</t>
+  </si>
+  <si>
+    <t>pou_7d7eae260f4cd53c</t>
+  </si>
+  <si>
+    <t>pou_fa05e08f584aa056</t>
+  </si>
+  <si>
+    <t>pou_da975bfc6544c069</t>
+  </si>
+  <si>
+    <t>pou_b800dd5e3295c360</t>
+  </si>
+  <si>
+    <t>pou_2088c76bd227048a</t>
+  </si>
+  <si>
+    <t>pou_e3b584cf6950d547</t>
+  </si>
+  <si>
+    <t>pou_a7fa90c21d4d495d</t>
+  </si>
+  <si>
+    <t>pou_2fbaeeeef9d1b6d6</t>
+  </si>
+  <si>
+    <t>pou_3a1d8bc453d810fd</t>
+  </si>
+  <si>
+    <t>pou_3c677c35cc3d350f</t>
+  </si>
+  <si>
+    <t>pou_44f109c880691314</t>
+  </si>
+  <si>
+    <t>pou_44ccf3851f8d8f20</t>
+  </si>
+  <si>
+    <t>pou_5aed74acb414ed59</t>
+  </si>
+  <si>
+    <t>pou_f7d11ba373410c5d</t>
+  </si>
+  <si>
+    <t>pou_56fd8b870de285f2</t>
+  </si>
+  <si>
+    <t>pou_0c7ee6ff30e4e17e</t>
+  </si>
+  <si>
+    <t>pou_4f4472ab2ec54b13</t>
+  </si>
+  <si>
+    <t>pou_b3833c8b41cdb165</t>
+  </si>
+  <si>
+    <t>pou_bb51f9167b0a79a4</t>
+  </si>
+  <si>
+    <t>pou_e18b612a1ce54bcf</t>
+  </si>
+  <si>
+    <t>pou_203a95b5714b6d19</t>
+  </si>
+  <si>
+    <t>pou_26745ec14296ca7c</t>
+  </si>
+  <si>
+    <t>pou_4419f93993ac8e63</t>
+  </si>
+  <si>
+    <t>pou_f6c6d77665c3e90d</t>
+  </si>
+  <si>
+    <t>pou_d27709a392a1682f</t>
+  </si>
+  <si>
+    <t>pou_4d02afe377b9d7d9</t>
+  </si>
+  <si>
+    <t>pou_1b0b496a8347f46b</t>
+  </si>
+  <si>
+    <t>pou_87756194a978d742</t>
+  </si>
+  <si>
+    <t>pou_921126e467310c45</t>
+  </si>
+  <si>
+    <t>pou_e0a9c4ca05821487</t>
+  </si>
+  <si>
+    <t>pou_4972291b1b3ffadd</t>
+  </si>
+  <si>
+    <t>pou_99fe1e02c07876e5</t>
+  </si>
+  <si>
+    <t>pou_2aba8cf212f4cf30</t>
+  </si>
+  <si>
+    <t>pou_5359a6498d6e68a4</t>
+  </si>
+  <si>
+    <t>pou_7feca395b48715fd</t>
+  </si>
+  <si>
+    <t>pou_c20af954e9ab057e</t>
+  </si>
+  <si>
+    <t>pou_1c7972359d17ffbb</t>
+  </si>
+  <si>
+    <t>pou_a559215e5c4db57c</t>
+  </si>
+  <si>
+    <t>pou_a1dc3543d82d1ac3</t>
+  </si>
+  <si>
+    <t>pou_5f06a8ee6dfbd3ac</t>
+  </si>
+  <si>
+    <t>pou_36280f78048876d2</t>
+  </si>
+  <si>
+    <t>pou_7db0940756364613</t>
+  </si>
+  <si>
+    <t>pou_76bce60a89b606e1;pou_9e56667c2dd70225</t>
+  </si>
+  <si>
+    <t>pou_0f4b286f48e94605;pou_5a166d2d679e85f4;pou_f6e57a31f008f45e;pou_527650f44165b220;pou_1ee10693b8234fd1;pou_d88b605613f42715;pou_d0e7eb3c7229d870;pou_4ae06fc22f47fafb;pou_80e7ff38b8ad87de;pou_7d5180881a80b632;pou_bb009c665833c67d;pou_9c533a799606c85a</t>
+  </si>
+  <si>
+    <t>pou_6a670a86879f9998</t>
+  </si>
+  <si>
+    <t>pou_39b6cd5fbca99f16</t>
+  </si>
+  <si>
+    <t>pou_051faa1508691457</t>
+  </si>
+  <si>
+    <t>pou_c4d221c52e5a3169</t>
+  </si>
+  <si>
+    <t>pou_2b907fe423e67e0b</t>
+  </si>
+  <si>
+    <t>pou_d277a76b2af02233</t>
+  </si>
+  <si>
+    <t>pou_23162226a76f89e1</t>
+  </si>
+  <si>
+    <t>pou_57c3f9386d8bc0dd</t>
+  </si>
+  <si>
+    <t>pou_4a488b17bdc210d9</t>
+  </si>
+  <si>
+    <t>pou_f020b553737adf5b</t>
+  </si>
+  <si>
+    <t>pou_a98644ea26bbd58b</t>
+  </si>
+  <si>
+    <t>pou_12ca0046211c76e4</t>
+  </si>
+  <si>
+    <t>pou_5755d4fbf10b9099</t>
+  </si>
+  <si>
+    <t>pou_6f04b2138f59653d</t>
+  </si>
+  <si>
+    <t>pou_f90b08ee86981c4b</t>
+  </si>
+  <si>
+    <t>pou_7f158c60e1c096e6</t>
+  </si>
+  <si>
+    <t>pou_6df8283f02bf246e</t>
+  </si>
+  <si>
+    <t>pou_28e7fcc27c9cf35c</t>
+  </si>
+  <si>
+    <t>pou_7731ffddf09c6ff4</t>
+  </si>
+  <si>
+    <t>pou_c7a07a159d77d870</t>
+  </si>
+  <si>
+    <t>pou_b0127bda6b9a3a3a</t>
+  </si>
+  <si>
+    <t>pou_713140b159d6bf6e</t>
+  </si>
+  <si>
+    <t>pou_28c0f39f0bf66866</t>
+  </si>
+  <si>
+    <t>pou_804bd085b58e74cf</t>
+  </si>
+  <si>
+    <t>pou_e80534a1ca5e3912</t>
+  </si>
+  <si>
+    <t>pou_c53ea85733478b5a</t>
+  </si>
+  <si>
+    <t>pou_cb8f805f7b8da014</t>
+  </si>
+  <si>
+    <t>pou_c3485316da2afde9</t>
+  </si>
+  <si>
+    <t>pou_fe3ec837a3ee8d79</t>
+  </si>
+  <si>
+    <t>pou_70de3cb22c6ff5c5</t>
+  </si>
+  <si>
+    <t>pou_9173e78443f16810</t>
+  </si>
+  <si>
+    <t>pou_853b92f7eee1c51f</t>
+  </si>
+  <si>
+    <t>pou_65c32830585c628c</t>
+  </si>
+  <si>
+    <t>pou_505523539c5ff99f</t>
+  </si>
+  <si>
+    <t>pou_daf17574cfbacc7c</t>
+  </si>
+  <si>
+    <t>pou_cf1b4dcbec4beed8</t>
+  </si>
+  <si>
+    <t>pou_6cc2b13680b34b5f</t>
+  </si>
+  <si>
+    <t>pou_f4549823ddb08c8b</t>
+  </si>
+  <si>
+    <t>pou_42625880cce40665</t>
+  </si>
+  <si>
+    <t>pou_927e5b4979e682cd</t>
+  </si>
+  <si>
+    <t>pou_46fd7585fa71aa0b</t>
+  </si>
+  <si>
+    <t>pou_f99b53fe6b79ed08</t>
   </si>
 </sst>
 </file>

</xml_diff>